<commit_message>
se ajustan titulos de columnas
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0514B129-9990-458A-8617-7D439C85BC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226864E2-1ABF-4DF2-A7C8-04AD2475A2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2655,7 +2655,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2675,12 +2675,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3140,7 +3134,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J2"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se agrega ID_Cron al Plan de Trabajo y se mantienen habilitadas solo las funcionalidades de Distribución dentro del módulo inicial del Spooler.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226864E2-1ABF-4DF2-A7C8-04AD2475A2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7F21DE-5107-4B71-94FC-398C24E32FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
     <sheet name="Detalle" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$J$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$K$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$2:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,6 +46,7 @@
     <author>tc={B99868DF-D5CB-4B4D-8832-5CAEA9E9189B}</author>
     <author>tc={BBAD5277-51BC-4EC1-B176-090510E4CD69}</author>
     <author>tc={1A01895E-B4CA-43D8-9D26-987A1667FAE7}</author>
+    <author>tc={38372124-5616-401A-B40A-476DE7B44D8B}</author>
     <author>tc={11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}</author>
     <author>tc={B56B010C-6EB7-4B4F-9D8B-5579B701198E}</author>
     <author>tc={7F63E4B1-80CD-4575-908F-B1DCA061309F}</author>
@@ -93,7 +94,15 @@
     Nombre de la persona que migró el módulo.</t>
       </text>
     </comment>
-    <comment ref="J1" authorId="5" shapeId="0" xr:uid="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
+    <comment ref="J1" authorId="5" shapeId="0" xr:uid="{38372124-5616-401A-B40A-476DE7B44D8B}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Nombre de la persona que migró el módulo.</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="6" shapeId="0" xr:uid="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -101,7 +110,7 @@
     Observaciones o comentarios que se consideren importantes al migrar un módulo.</t>
       </text>
     </comment>
-    <comment ref="E2" authorId="6" shapeId="0" xr:uid="{B56B010C-6EB7-4B4F-9D8B-5579B701198E}">
+    <comment ref="E2" authorId="7" shapeId="0" xr:uid="{B56B010C-6EB7-4B4F-9D8B-5579B701198E}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -109,7 +118,7 @@
     El proceso ya se terminó en código local y es funcional.</t>
       </text>
     </comment>
-    <comment ref="F2" authorId="7" shapeId="0" xr:uid="{7F63E4B1-80CD-4575-908F-B1DCA061309F}">
+    <comment ref="F2" authorId="8" shapeId="0" xr:uid="{7F63E4B1-80CD-4575-908F-B1DCA061309F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -117,7 +126,7 @@
     El proceso se publicó y se validó en el Srv. de Desarrollo de forma satisfactoria.</t>
       </text>
     </comment>
-    <comment ref="G2" authorId="8" shapeId="0" xr:uid="{A93D80C5-D95F-45C9-9060-63249C22896D}">
+    <comment ref="G2" authorId="9" shapeId="0" xr:uid="{A93D80C5-D95F-45C9-9060-63249C22896D}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -125,7 +134,7 @@
     El proceso se publicó y se validó en el Srv. de Q.A.  de forma satisfactoria.</t>
       </text>
     </comment>
-    <comment ref="H2" authorId="9" shapeId="0" xr:uid="{08706989-DEF6-4746-8EDE-FFB49503C0FE}">
+    <comment ref="H2" authorId="10" shapeId="0" xr:uid="{08706989-DEF6-4746-8EDE-FFB49503C0FE}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -138,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3974" uniqueCount="838">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2649,13 +2658,16 @@
   </si>
   <si>
     <t>Se desarrolló módulo con funciones que se estarán reutilizando a lo largo del aplicativo.</t>
+  </si>
+  <si>
+    <t>ID_CRON - EJEMPLO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2675,6 +2687,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2756,7 +2774,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2808,6 +2826,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3110,7 +3134,10 @@
   <threadedComment ref="I1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{1A01895E-B4CA-43D8-9D26-987A1667FAE7}">
     <text>Nombre de la persona que migró el módulo.</text>
   </threadedComment>
-  <threadedComment ref="J1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
+  <threadedComment ref="J1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{38372124-5616-401A-B40A-476DE7B44D8B}">
+    <text>Nombre de la persona que migró el módulo.</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
     <text>Observaciones o comentarios que se consideren importantes al migrar un módulo.</text>
   </threadedComment>
   <threadedComment ref="E2" dT="2025-04-23T23:33:08.08" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{B56B010C-6EB7-4B4F-9D8B-5579B701198E}">
@@ -3130,11 +3157,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:K157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,10 +3175,11 @@
     <col min="7" max="7" width="7.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="72.5703125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="72.5703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>814</v>
       </c>
@@ -3173,11 +3201,14 @@
       <c r="I1" s="12" t="s">
         <v>716</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="18" t="s">
+        <v>837</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
@@ -3195,9 +3226,10 @@
         <v>708</v>
       </c>
       <c r="I2" s="13"/>
-      <c r="J2" s="11"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="19"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -3221,11 +3253,12 @@
       <c r="I3" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="3" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -3249,9 +3282,12 @@
       <c r="I4" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="6">
+        <v>3723307</v>
+      </c>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -3275,9 +3311,12 @@
       <c r="I5" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="4">
+        <v>6651805</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -3301,9 +3340,12 @@
       <c r="I6" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="6">
+        <v>4220496</v>
+      </c>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -3327,9 +3369,12 @@
       <c r="I7" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="4">
+        <v>5566768</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -3353,9 +3398,12 @@
       <c r="I8" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="6">
+        <v>5545714</v>
+      </c>
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -3379,9 +3427,12 @@
       <c r="I9" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="J9" s="3"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="4">
+        <v>7774047</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -3405,9 +3456,12 @@
       <c r="I10" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="6">
+        <v>7864811</v>
+      </c>
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -3425,9 +3479,10 @@
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="4"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -3445,9 +3500,10 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="6"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -3465,9 +3521,10 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="4"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -3485,9 +3542,10 @@
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="6"/>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -3505,9 +3563,10 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="4"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -3525,9 +3584,10 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J16" s="6"/>
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -3545,9 +3605,10 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="4"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -3565,9 +3626,10 @@
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J18" s="6"/>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -3585,9 +3647,10 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="4"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -3605,9 +3668,10 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J20" s="6"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -3625,9 +3689,10 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J21" s="4"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>19</v>
       </c>
@@ -3645,9 +3710,10 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J22" s="6"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -3665,9 +3731,10 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="4"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>21</v>
       </c>
@@ -3685,9 +3752,10 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="6"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -3705,9 +3773,10 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="4"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>23</v>
       </c>
@@ -3725,9 +3794,10 @@
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="6"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -3745,9 +3815,10 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="4"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>25</v>
       </c>
@@ -3765,9 +3836,10 @@
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="6"/>
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -3785,9 +3857,10 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="4"/>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>27</v>
       </c>
@@ -3805,9 +3878,10 @@
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="6"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -3825,9 +3899,10 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="4"/>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>29</v>
       </c>
@@ -3845,9 +3920,10 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="6"/>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="6"/>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -3865,9 +3941,10 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="4"/>
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="4"/>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>31</v>
       </c>
@@ -3885,9 +3962,10 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J34" s="6"/>
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -3905,9 +3983,10 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J35" s="4"/>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>33</v>
       </c>
@@ -3925,9 +4004,10 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="6"/>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J36" s="6"/>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -3945,9 +4025,10 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="4"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J37" s="4"/>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>35</v>
       </c>
@@ -3965,9 +4046,10 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="6"/>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J38" s="6"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>36</v>
       </c>
@@ -3985,9 +4067,10 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="4"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="4"/>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>37</v>
       </c>
@@ -4005,9 +4088,10 @@
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="6"/>
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>38</v>
       </c>
@@ -4025,9 +4109,10 @@
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="4"/>
-      <c r="J41" s="3"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="4"/>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>39</v>
       </c>
@@ -4045,9 +4130,10 @@
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="6"/>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J42" s="6"/>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>40</v>
       </c>
@@ -4065,9 +4151,10 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="4"/>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J43" s="4"/>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>41</v>
       </c>
@@ -4085,9 +4172,10 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="6"/>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="6"/>
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>42</v>
       </c>
@@ -4105,9 +4193,10 @@
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="4"/>
-      <c r="J45" s="3"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="4"/>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>43</v>
       </c>
@@ -4125,9 +4214,10 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="6"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J46" s="6"/>
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>44</v>
       </c>
@@ -4145,9 +4235,10 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="4"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J47" s="4"/>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>45</v>
       </c>
@@ -4165,9 +4256,10 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="6"/>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J48" s="6"/>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>46</v>
       </c>
@@ -4185,9 +4277,10 @@
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J49" s="4"/>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>47</v>
       </c>
@@ -4205,9 +4298,10 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="6"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J50" s="6"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>48</v>
       </c>
@@ -4225,9 +4319,10 @@
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="4"/>
-      <c r="J51" s="3"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J51" s="4"/>
+      <c r="K51" s="3"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>49</v>
       </c>
@@ -4245,9 +4340,10 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
       <c r="I52" s="6"/>
-      <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J52" s="6"/>
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>50</v>
       </c>
@@ -4265,9 +4361,10 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="4"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J53" s="4"/>
+      <c r="K53" s="3"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>51</v>
       </c>
@@ -4285,9 +4382,10 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="6"/>
-      <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J54" s="6"/>
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>52</v>
       </c>
@@ -4305,9 +4403,10 @@
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
       <c r="I55" s="4"/>
-      <c r="J55" s="3"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J55" s="4"/>
+      <c r="K55" s="3"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>53</v>
       </c>
@@ -4325,9 +4424,10 @@
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
       <c r="I56" s="6"/>
-      <c r="J56" s="5"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J56" s="6"/>
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>54</v>
       </c>
@@ -4345,9 +4445,10 @@
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="4"/>
-      <c r="J57" s="3"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J57" s="4"/>
+      <c r="K57" s="3"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>55</v>
       </c>
@@ -4365,9 +4466,10 @@
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" s="6"/>
-      <c r="J58" s="5"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J58" s="6"/>
+      <c r="K58" s="5"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>56</v>
       </c>
@@ -4385,9 +4487,10 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="4"/>
-      <c r="J59" s="3"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J59" s="4"/>
+      <c r="K59" s="3"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>57</v>
       </c>
@@ -4405,9 +4508,10 @@
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
       <c r="I60" s="6"/>
-      <c r="J60" s="5"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J60" s="6"/>
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>58</v>
       </c>
@@ -4425,9 +4529,10 @@
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="4"/>
-      <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J61" s="4"/>
+      <c r="K61" s="3"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>59</v>
       </c>
@@ -4445,9 +4550,10 @@
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="6"/>
-      <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J62" s="6"/>
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>60</v>
       </c>
@@ -4465,9 +4571,10 @@
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
       <c r="I63" s="4"/>
-      <c r="J63" s="3"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J63" s="4"/>
+      <c r="K63" s="3"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>61</v>
       </c>
@@ -4485,9 +4592,10 @@
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="6"/>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J64" s="6"/>
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>62</v>
       </c>
@@ -4505,9 +4613,10 @@
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="3"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J65" s="4"/>
+      <c r="K65" s="3"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>63</v>
       </c>
@@ -4525,9 +4634,10 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
       <c r="I66" s="6"/>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J66" s="6"/>
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -4545,9 +4655,10 @@
       <c r="G67" s="7"/>
       <c r="H67" s="7"/>
       <c r="I67" s="4"/>
-      <c r="J67" s="3"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J67" s="4"/>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>65</v>
       </c>
@@ -4565,9 +4676,10 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="6"/>
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J68" s="6"/>
+      <c r="K68" s="5"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>66</v>
       </c>
@@ -4585,9 +4697,10 @@
       <c r="G69" s="7"/>
       <c r="H69" s="7"/>
       <c r="I69" s="4"/>
-      <c r="J69" s="3"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J69" s="4"/>
+      <c r="K69" s="3"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>67</v>
       </c>
@@ -4605,9 +4718,10 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
       <c r="I70" s="6"/>
-      <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J70" s="6"/>
+      <c r="K70" s="5"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>68</v>
       </c>
@@ -4625,9 +4739,10 @@
       <c r="G71" s="7"/>
       <c r="H71" s="7"/>
       <c r="I71" s="4"/>
-      <c r="J71" s="3"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J71" s="4"/>
+      <c r="K71" s="3"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>69</v>
       </c>
@@ -4645,9 +4760,10 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="6"/>
-      <c r="J72" s="5"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J72" s="6"/>
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>70</v>
       </c>
@@ -4665,9 +4781,10 @@
       <c r="G73" s="7"/>
       <c r="H73" s="7"/>
       <c r="I73" s="4"/>
-      <c r="J73" s="3"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J73" s="4"/>
+      <c r="K73" s="3"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>71</v>
       </c>
@@ -4685,9 +4802,10 @@
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="6"/>
-      <c r="J74" s="5"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J74" s="6"/>
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>72</v>
       </c>
@@ -4705,9 +4823,10 @@
       <c r="G75" s="7"/>
       <c r="H75" s="7"/>
       <c r="I75" s="4"/>
-      <c r="J75" s="3"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J75" s="4"/>
+      <c r="K75" s="3"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>73</v>
       </c>
@@ -4725,9 +4844,10 @@
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
       <c r="I76" s="6"/>
-      <c r="J76" s="5"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J76" s="6"/>
+      <c r="K76" s="5"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>74</v>
       </c>
@@ -4745,9 +4865,10 @@
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
       <c r="I77" s="4"/>
-      <c r="J77" s="3"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J77" s="4"/>
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -4765,9 +4886,10 @@
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
       <c r="I78" s="6"/>
-      <c r="J78" s="5"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J78" s="6"/>
+      <c r="K78" s="5"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>76</v>
       </c>
@@ -4785,9 +4907,10 @@
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
       <c r="I79" s="4"/>
-      <c r="J79" s="3"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J79" s="4"/>
+      <c r="K79" s="3"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -4805,9 +4928,10 @@
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
       <c r="I80" s="6"/>
-      <c r="J80" s="5"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J80" s="6"/>
+      <c r="K80" s="5"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>78</v>
       </c>
@@ -4825,9 +4949,10 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="I81" s="4"/>
-      <c r="J81" s="3"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J81" s="4"/>
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -4845,9 +4970,10 @@
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="6"/>
-      <c r="J82" s="5"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J82" s="6"/>
+      <c r="K82" s="5"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>80</v>
       </c>
@@ -4865,9 +4991,10 @@
       <c r="G83" s="7"/>
       <c r="H83" s="7"/>
       <c r="I83" s="4"/>
-      <c r="J83" s="3"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J83" s="4"/>
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -4885,9 +5012,10 @@
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="6"/>
-      <c r="J84" s="5"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J84" s="6"/>
+      <c r="K84" s="5"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>82</v>
       </c>
@@ -4905,9 +5033,10 @@
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
       <c r="I85" s="4"/>
-      <c r="J85" s="3"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J85" s="4"/>
+      <c r="K85" s="3"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -4925,9 +5054,10 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="6"/>
-      <c r="J86" s="5"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J86" s="6"/>
+      <c r="K86" s="5"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>84</v>
       </c>
@@ -4945,9 +5075,10 @@
       <c r="G87" s="7"/>
       <c r="H87" s="7"/>
       <c r="I87" s="4"/>
-      <c r="J87" s="3"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J87" s="4"/>
+      <c r="K87" s="3"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -4965,9 +5096,10 @@
       <c r="G88" s="8"/>
       <c r="H88" s="8"/>
       <c r="I88" s="6"/>
-      <c r="J88" s="5"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J88" s="6"/>
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>86</v>
       </c>
@@ -4985,9 +5117,10 @@
       <c r="G89" s="7"/>
       <c r="H89" s="7"/>
       <c r="I89" s="4"/>
-      <c r="J89" s="3"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J89" s="4"/>
+      <c r="K89" s="3"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -5005,9 +5138,10 @@
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
       <c r="I90" s="6"/>
-      <c r="J90" s="5"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J90" s="6"/>
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>88</v>
       </c>
@@ -5025,9 +5159,10 @@
       <c r="G91" s="7"/>
       <c r="H91" s="7"/>
       <c r="I91" s="4"/>
-      <c r="J91" s="3"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J91" s="4"/>
+      <c r="K91" s="3"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -5045,9 +5180,10 @@
       <c r="G92" s="8"/>
       <c r="H92" s="8"/>
       <c r="I92" s="6"/>
-      <c r="J92" s="5"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J92" s="6"/>
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>90</v>
       </c>
@@ -5065,9 +5201,10 @@
       <c r="G93" s="7"/>
       <c r="H93" s="7"/>
       <c r="I93" s="4"/>
-      <c r="J93" s="3"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J93" s="4"/>
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -5085,9 +5222,10 @@
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
       <c r="I94" s="6"/>
-      <c r="J94" s="5"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J94" s="6"/>
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>92</v>
       </c>
@@ -5105,9 +5243,10 @@
       <c r="G95" s="7"/>
       <c r="H95" s="7"/>
       <c r="I95" s="4"/>
-      <c r="J95" s="3"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J95" s="4"/>
+      <c r="K95" s="3"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -5125,9 +5264,10 @@
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
       <c r="I96" s="6"/>
-      <c r="J96" s="5"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J96" s="6"/>
+      <c r="K96" s="5"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>94</v>
       </c>
@@ -5145,9 +5285,10 @@
       <c r="G97" s="7"/>
       <c r="H97" s="7"/>
       <c r="I97" s="4"/>
-      <c r="J97" s="3"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J97" s="4"/>
+      <c r="K97" s="3"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -5165,9 +5306,10 @@
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="6"/>
-      <c r="J98" s="5"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J98" s="6"/>
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>96</v>
       </c>
@@ -5185,9 +5327,10 @@
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
       <c r="I99" s="4"/>
-      <c r="J99" s="3"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J99" s="4"/>
+      <c r="K99" s="3"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -5205,9 +5348,10 @@
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
       <c r="I100" s="6"/>
-      <c r="J100" s="5"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J100" s="6"/>
+      <c r="K100" s="5"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>98</v>
       </c>
@@ -5225,9 +5369,10 @@
       <c r="G101" s="7"/>
       <c r="H101" s="7"/>
       <c r="I101" s="4"/>
-      <c r="J101" s="3"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J101" s="4"/>
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -5245,9 +5390,10 @@
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
       <c r="I102" s="6"/>
-      <c r="J102" s="5"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J102" s="6"/>
+      <c r="K102" s="5"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>100</v>
       </c>
@@ -5265,9 +5411,10 @@
       <c r="G103" s="7"/>
       <c r="H103" s="7"/>
       <c r="I103" s="4"/>
-      <c r="J103" s="3"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J103" s="4"/>
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -5285,9 +5432,10 @@
       <c r="G104" s="8"/>
       <c r="H104" s="8"/>
       <c r="I104" s="6"/>
-      <c r="J104" s="5"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J104" s="6"/>
+      <c r="K104" s="5"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>102</v>
       </c>
@@ -5305,9 +5453,10 @@
       <c r="G105" s="7"/>
       <c r="H105" s="7"/>
       <c r="I105" s="4"/>
-      <c r="J105" s="3"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J105" s="4"/>
+      <c r="K105" s="3"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -5325,9 +5474,10 @@
       <c r="G106" s="8"/>
       <c r="H106" s="8"/>
       <c r="I106" s="6"/>
-      <c r="J106" s="5"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J106" s="6"/>
+      <c r="K106" s="5"/>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>104</v>
       </c>
@@ -5345,9 +5495,10 @@
       <c r="G107" s="7"/>
       <c r="H107" s="7"/>
       <c r="I107" s="4"/>
-      <c r="J107" s="3"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J107" s="4"/>
+      <c r="K107" s="3"/>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -5365,9 +5516,10 @@
       <c r="G108" s="8"/>
       <c r="H108" s="8"/>
       <c r="I108" s="6"/>
-      <c r="J108" s="5"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J108" s="6"/>
+      <c r="K108" s="5"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>106</v>
       </c>
@@ -5385,9 +5537,10 @@
       <c r="G109" s="7"/>
       <c r="H109" s="7"/>
       <c r="I109" s="4"/>
-      <c r="J109" s="3"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J109" s="4"/>
+      <c r="K109" s="3"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>107</v>
       </c>
@@ -5405,9 +5558,10 @@
       <c r="G110" s="8"/>
       <c r="H110" s="8"/>
       <c r="I110" s="6"/>
-      <c r="J110" s="5"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J110" s="6"/>
+      <c r="K110" s="5"/>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>108</v>
       </c>
@@ -5425,9 +5579,10 @@
       <c r="G111" s="7"/>
       <c r="H111" s="7"/>
       <c r="I111" s="4"/>
-      <c r="J111" s="3"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J111" s="4"/>
+      <c r="K111" s="3"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>109</v>
       </c>
@@ -5445,9 +5600,10 @@
       <c r="G112" s="8"/>
       <c r="H112" s="8"/>
       <c r="I112" s="6"/>
-      <c r="J112" s="5"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J112" s="6"/>
+      <c r="K112" s="5"/>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>110</v>
       </c>
@@ -5465,9 +5621,10 @@
       <c r="G113" s="7"/>
       <c r="H113" s="7"/>
       <c r="I113" s="4"/>
-      <c r="J113" s="3"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J113" s="4"/>
+      <c r="K113" s="3"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>111</v>
       </c>
@@ -5485,9 +5642,10 @@
       <c r="G114" s="8"/>
       <c r="H114" s="8"/>
       <c r="I114" s="6"/>
-      <c r="J114" s="5"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J114" s="6"/>
+      <c r="K114" s="5"/>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>112</v>
       </c>
@@ -5505,9 +5663,10 @@
       <c r="G115" s="7"/>
       <c r="H115" s="7"/>
       <c r="I115" s="4"/>
-      <c r="J115" s="3"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J115" s="4"/>
+      <c r="K115" s="3"/>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>113</v>
       </c>
@@ -5525,9 +5684,10 @@
       <c r="G116" s="8"/>
       <c r="H116" s="8"/>
       <c r="I116" s="6"/>
-      <c r="J116" s="5"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J116" s="6"/>
+      <c r="K116" s="5"/>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>114</v>
       </c>
@@ -5545,9 +5705,10 @@
       <c r="G117" s="7"/>
       <c r="H117" s="7"/>
       <c r="I117" s="4"/>
-      <c r="J117" s="3"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J117" s="4"/>
+      <c r="K117" s="3"/>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>115</v>
       </c>
@@ -5565,9 +5726,10 @@
       <c r="G118" s="8"/>
       <c r="H118" s="8"/>
       <c r="I118" s="6"/>
-      <c r="J118" s="5"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J118" s="6"/>
+      <c r="K118" s="5"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>116</v>
       </c>
@@ -5585,9 +5747,10 @@
       <c r="G119" s="7"/>
       <c r="H119" s="7"/>
       <c r="I119" s="4"/>
-      <c r="J119" s="3"/>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J119" s="4"/>
+      <c r="K119" s="3"/>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>117</v>
       </c>
@@ -5605,9 +5768,10 @@
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
       <c r="I120" s="6"/>
-      <c r="J120" s="5"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J120" s="6"/>
+      <c r="K120" s="5"/>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>118</v>
       </c>
@@ -5625,9 +5789,10 @@
       <c r="G121" s="7"/>
       <c r="H121" s="7"/>
       <c r="I121" s="4"/>
-      <c r="J121" s="3"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J121" s="4"/>
+      <c r="K121" s="3"/>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>119</v>
       </c>
@@ -5645,9 +5810,10 @@
       <c r="G122" s="8"/>
       <c r="H122" s="8"/>
       <c r="I122" s="6"/>
-      <c r="J122" s="5"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J122" s="6"/>
+      <c r="K122" s="5"/>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>120</v>
       </c>
@@ -5665,9 +5831,10 @@
       <c r="G123" s="7"/>
       <c r="H123" s="7"/>
       <c r="I123" s="4"/>
-      <c r="J123" s="3"/>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J123" s="4"/>
+      <c r="K123" s="3"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>121</v>
       </c>
@@ -5685,9 +5852,10 @@
       <c r="G124" s="8"/>
       <c r="H124" s="8"/>
       <c r="I124" s="6"/>
-      <c r="J124" s="5"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J124" s="6"/>
+      <c r="K124" s="5"/>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>122</v>
       </c>
@@ -5705,9 +5873,10 @@
       <c r="G125" s="7"/>
       <c r="H125" s="7"/>
       <c r="I125" s="4"/>
-      <c r="J125" s="3"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J125" s="4"/>
+      <c r="K125" s="3"/>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>123</v>
       </c>
@@ -5725,9 +5894,10 @@
       <c r="G126" s="8"/>
       <c r="H126" s="8"/>
       <c r="I126" s="6"/>
-      <c r="J126" s="5"/>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J126" s="6"/>
+      <c r="K126" s="5"/>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>124</v>
       </c>
@@ -5745,9 +5915,10 @@
       <c r="G127" s="7"/>
       <c r="H127" s="7"/>
       <c r="I127" s="4"/>
-      <c r="J127" s="3"/>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J127" s="4"/>
+      <c r="K127" s="3"/>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>125</v>
       </c>
@@ -5765,9 +5936,10 @@
       <c r="G128" s="8"/>
       <c r="H128" s="8"/>
       <c r="I128" s="6"/>
-      <c r="J128" s="5"/>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J128" s="6"/>
+      <c r="K128" s="5"/>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>126</v>
       </c>
@@ -5785,9 +5957,10 @@
       <c r="G129" s="7"/>
       <c r="H129" s="7"/>
       <c r="I129" s="4"/>
-      <c r="J129" s="3"/>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J129" s="4"/>
+      <c r="K129" s="3"/>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>127</v>
       </c>
@@ -5805,9 +5978,10 @@
       <c r="G130" s="8"/>
       <c r="H130" s="8"/>
       <c r="I130" s="6"/>
-      <c r="J130" s="5"/>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J130" s="6"/>
+      <c r="K130" s="5"/>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>128</v>
       </c>
@@ -5825,9 +5999,10 @@
       <c r="G131" s="7"/>
       <c r="H131" s="7"/>
       <c r="I131" s="4"/>
-      <c r="J131" s="3"/>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J131" s="4"/>
+      <c r="K131" s="3"/>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>129</v>
       </c>
@@ -5845,9 +6020,10 @@
       <c r="G132" s="8"/>
       <c r="H132" s="8"/>
       <c r="I132" s="6"/>
-      <c r="J132" s="5"/>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J132" s="6"/>
+      <c r="K132" s="5"/>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>130</v>
       </c>
@@ -5865,9 +6041,10 @@
       <c r="G133" s="7"/>
       <c r="H133" s="7"/>
       <c r="I133" s="4"/>
-      <c r="J133" s="3"/>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J133" s="4"/>
+      <c r="K133" s="3"/>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>131</v>
       </c>
@@ -5885,9 +6062,10 @@
       <c r="G134" s="8"/>
       <c r="H134" s="8"/>
       <c r="I134" s="6"/>
-      <c r="J134" s="5"/>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J134" s="6"/>
+      <c r="K134" s="5"/>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>132</v>
       </c>
@@ -5905,9 +6083,10 @@
       <c r="G135" s="7"/>
       <c r="H135" s="7"/>
       <c r="I135" s="4"/>
-      <c r="J135" s="3"/>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J135" s="4"/>
+      <c r="K135" s="3"/>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>133</v>
       </c>
@@ -5925,9 +6104,10 @@
       <c r="G136" s="8"/>
       <c r="H136" s="8"/>
       <c r="I136" s="6"/>
-      <c r="J136" s="5"/>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J136" s="6"/>
+      <c r="K136" s="5"/>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>134</v>
       </c>
@@ -5945,9 +6125,10 @@
       <c r="G137" s="7"/>
       <c r="H137" s="7"/>
       <c r="I137" s="4"/>
-      <c r="J137" s="3"/>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J137" s="4"/>
+      <c r="K137" s="3"/>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>135</v>
       </c>
@@ -5965,9 +6146,10 @@
       <c r="G138" s="8"/>
       <c r="H138" s="8"/>
       <c r="I138" s="6"/>
-      <c r="J138" s="5"/>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J138" s="6"/>
+      <c r="K138" s="5"/>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>136</v>
       </c>
@@ -5985,9 +6167,10 @@
       <c r="G139" s="7"/>
       <c r="H139" s="7"/>
       <c r="I139" s="4"/>
-      <c r="J139" s="3"/>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J139" s="4"/>
+      <c r="K139" s="3"/>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>137</v>
       </c>
@@ -6005,9 +6188,10 @@
       <c r="G140" s="8"/>
       <c r="H140" s="8"/>
       <c r="I140" s="6"/>
-      <c r="J140" s="5"/>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J140" s="6"/>
+      <c r="K140" s="5"/>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>138</v>
       </c>
@@ -6025,9 +6209,10 @@
       <c r="G141" s="7"/>
       <c r="H141" s="7"/>
       <c r="I141" s="4"/>
-      <c r="J141" s="3"/>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J141" s="4"/>
+      <c r="K141" s="3"/>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>139</v>
       </c>
@@ -6045,9 +6230,10 @@
       <c r="G142" s="8"/>
       <c r="H142" s="8"/>
       <c r="I142" s="6"/>
-      <c r="J142" s="5"/>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J142" s="6"/>
+      <c r="K142" s="5"/>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>140</v>
       </c>
@@ -6065,9 +6251,10 @@
       <c r="G143" s="7"/>
       <c r="H143" s="7"/>
       <c r="I143" s="4"/>
-      <c r="J143" s="3"/>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J143" s="4"/>
+      <c r="K143" s="3"/>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>141</v>
       </c>
@@ -6085,9 +6272,10 @@
       <c r="G144" s="8"/>
       <c r="H144" s="8"/>
       <c r="I144" s="6"/>
-      <c r="J144" s="5"/>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J144" s="6"/>
+      <c r="K144" s="5"/>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>142</v>
       </c>
@@ -6105,9 +6293,10 @@
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
       <c r="I145" s="4"/>
-      <c r="J145" s="3"/>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J145" s="4"/>
+      <c r="K145" s="3"/>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>143</v>
       </c>
@@ -6125,9 +6314,10 @@
       <c r="G146" s="8"/>
       <c r="H146" s="8"/>
       <c r="I146" s="6"/>
-      <c r="J146" s="5"/>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J146" s="6"/>
+      <c r="K146" s="5"/>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>144</v>
       </c>
@@ -6145,9 +6335,10 @@
       <c r="G147" s="7"/>
       <c r="H147" s="7"/>
       <c r="I147" s="4"/>
-      <c r="J147" s="3"/>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J147" s="4"/>
+      <c r="K147" s="3"/>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>145</v>
       </c>
@@ -6165,9 +6356,10 @@
       <c r="G148" s="8"/>
       <c r="H148" s="8"/>
       <c r="I148" s="6"/>
-      <c r="J148" s="5"/>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J148" s="6"/>
+      <c r="K148" s="5"/>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>146</v>
       </c>
@@ -6185,9 +6377,10 @@
       <c r="G149" s="7"/>
       <c r="H149" s="7"/>
       <c r="I149" s="4"/>
-      <c r="J149" s="3"/>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J149" s="4"/>
+      <c r="K149" s="3"/>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>147</v>
       </c>
@@ -6205,9 +6398,10 @@
       <c r="G150" s="8"/>
       <c r="H150" s="8"/>
       <c r="I150" s="6"/>
-      <c r="J150" s="5"/>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J150" s="6"/>
+      <c r="K150" s="5"/>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>148</v>
       </c>
@@ -6225,9 +6419,10 @@
       <c r="G151" s="7"/>
       <c r="H151" s="7"/>
       <c r="I151" s="4"/>
-      <c r="J151" s="3"/>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J151" s="4"/>
+      <c r="K151" s="3"/>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>149</v>
       </c>
@@ -6245,9 +6440,10 @@
       <c r="G152" s="8"/>
       <c r="H152" s="8"/>
       <c r="I152" s="6"/>
-      <c r="J152" s="5"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J152" s="6"/>
+      <c r="K152" s="5"/>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>150</v>
       </c>
@@ -6265,9 +6461,10 @@
       <c r="G153" s="7"/>
       <c r="H153" s="7"/>
       <c r="I153" s="4"/>
-      <c r="J153" s="3"/>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J153" s="4"/>
+      <c r="K153" s="3"/>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>151</v>
       </c>
@@ -6285,9 +6482,10 @@
       <c r="G154" s="8"/>
       <c r="H154" s="8"/>
       <c r="I154" s="6"/>
-      <c r="J154" s="5"/>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J154" s="6"/>
+      <c r="K154" s="5"/>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>152</v>
       </c>
@@ -6305,9 +6503,10 @@
       <c r="G155" s="7"/>
       <c r="H155" s="7"/>
       <c r="I155" s="4"/>
-      <c r="J155" s="3"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J155" s="4"/>
+      <c r="K155" s="3"/>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>153</v>
       </c>
@@ -6325,9 +6524,10 @@
       <c r="G156" s="8"/>
       <c r="H156" s="8"/>
       <c r="I156" s="6"/>
-      <c r="J156" s="5"/>
-    </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J156" s="6"/>
+      <c r="K156" s="5"/>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>154</v>
       </c>
@@ -6345,25 +6545,27 @@
       <c r="G157" s="7"/>
       <c r="H157" s="7"/>
       <c r="I157" s="4"/>
-      <c r="J157" s="3"/>
+      <c r="J157" s="4"/>
+      <c r="K157" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:J2" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J157">
+  <autoFilter ref="A2:K2" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K157">
     <sortCondition ref="F4:F157"/>
     <sortCondition ref="E4:E157"/>
     <sortCondition ref="A4:A157"/>
     <sortCondition ref="C4:C157"/>
     <sortCondition ref="B4:B157"/>
   </sortState>
-  <mergeCells count="7">
-    <mergeCell ref="J1:J2"/>
+  <mergeCells count="8">
+    <mergeCell ref="K1:K2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrega diagrama E-R de la funcionalidad basica del Spooler y se actualiza el listado de procesos a Migrar para Distribución
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\net\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F15D210-EB10-426A-BE6D-CA54C81BEA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C3D30D-A082-465D-A6AB-4182A624A270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3976" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3978" uniqueCount="840">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2661,6 +2661,12 @@
   </si>
   <si>
     <t>ID_CRON - EJEMPLO</t>
+  </si>
+  <si>
+    <t>Evidencias Clientes SFTP</t>
+  </si>
+  <si>
+    <t>evid_clientes_sftp</t>
   </si>
 </sst>
 </file>
@@ -2715,7 +2721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2764,11 +2770,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF68A042"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2827,12 +2848,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF68A042"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3151,11 +3195,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
-  <dimension ref="A1:K157"/>
+  <dimension ref="A1:K158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3523,13 +3567,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="5">
-        <v>102</v>
+        <v>351</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>742</v>
+        <v>838</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>119</v>
+        <v>839</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -3547,10 +3591,10 @@
         <v>102</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>817</v>
+        <v>742</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>818</v>
+        <v>119</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -3568,10 +3612,10 @@
         <v>102</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -3589,10 +3633,10 @@
         <v>102</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -3610,10 +3654,10 @@
         <v>102</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -3628,13 +3672,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="3">
-        <v>341</v>
+        <v>102</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>811</v>
+        <v>823</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>699</v>
+        <v>824</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -3649,13 +3693,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="5">
-        <v>282</v>
+        <v>341</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>800</v>
+        <v>811</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>651</v>
+        <v>699</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -3670,13 +3714,13 @@
         <v>18</v>
       </c>
       <c r="B21" s="3">
-        <v>348</v>
+        <v>282</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>703</v>
+        <v>651</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -3691,13 +3735,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="5">
-        <v>186</v>
+        <v>348</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>825</v>
+        <v>813</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>826</v>
+        <v>703</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
@@ -3712,13 +3756,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="3">
-        <v>347</v>
+        <v>186</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>812</v>
+        <v>825</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>701</v>
+        <v>826</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -3733,13 +3777,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="5">
-        <v>235</v>
+        <v>347</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>787</v>
+        <v>812</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>446</v>
+        <v>701</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
@@ -3754,13 +3798,13 @@
         <v>22</v>
       </c>
       <c r="B25" s="3">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -3775,13 +3819,13 @@
         <v>23</v>
       </c>
       <c r="B26" s="5">
-        <v>80</v>
+        <v>234</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>728</v>
+        <v>786</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>68</v>
+        <v>444</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -3796,13 +3840,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="3">
-        <v>226</v>
+        <v>80</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>784</v>
+        <v>728</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>439</v>
+        <v>68</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -3817,13 +3861,13 @@
         <v>25</v>
       </c>
       <c r="B28" s="5">
-        <v>89</v>
+        <v>226</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>732</v>
+        <v>784</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>94</v>
+        <v>439</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -3838,13 +3882,13 @@
         <v>26</v>
       </c>
       <c r="B29" s="3">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>758</v>
+        <v>732</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>214</v>
+        <v>94</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -3859,21 +3903,19 @@
         <v>27</v>
       </c>
       <c r="B30" s="5">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="6" t="s">
-        <v>833</v>
-      </c>
+      <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="5"/>
     </row>
@@ -3882,19 +3924,21 @@
         <v>28</v>
       </c>
       <c r="B31" s="3">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
-      <c r="I31" s="4"/>
+      <c r="I31" s="4" t="s">
+        <v>833</v>
+      </c>
       <c r="J31" s="4"/>
       <c r="K31" s="3"/>
     </row>
@@ -3903,13 +3947,13 @@
         <v>29</v>
       </c>
       <c r="B32" s="5">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>419</v>
+        <v>757</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>420</v>
+        <v>207</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -3924,21 +3968,19 @@
         <v>30</v>
       </c>
       <c r="B33" s="3">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>771</v>
+        <v>419</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>401</v>
+        <v>420</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
-      <c r="I33" s="4" t="s">
-        <v>833</v>
-      </c>
+      <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="3"/>
     </row>
@@ -3947,76 +3989,78 @@
         <v>31</v>
       </c>
       <c r="B34" s="5">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>717</v>
+        <v>771</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>13</v>
+        <v>401</v>
       </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="6"/>
+      <c r="I34" s="6" t="s">
+        <v>833</v>
+      </c>
       <c r="J34" s="6"/>
       <c r="K34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="23">
         <v>32</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="23">
+        <v>36</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>717</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="23"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="20">
+        <v>33</v>
+      </c>
+      <c r="B36" s="20">
         <v>37</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="20" t="s">
         <v>718</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="3"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>33</v>
-      </c>
-      <c r="B36" s="5">
-        <v>39</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="5"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="20"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>34</v>
       </c>
       <c r="B37" s="3">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>734</v>
+        <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -4031,13 +4075,13 @@
         <v>35</v>
       </c>
       <c r="B38" s="5">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>21</v>
+        <v>734</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -4052,13 +4096,13 @@
         <v>36</v>
       </c>
       <c r="B39" s="3">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>170</v>
+        <v>22</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -4073,13 +4117,13 @@
         <v>37</v>
       </c>
       <c r="B40" s="5">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>39</v>
+        <v>169</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
@@ -4094,10 +4138,10 @@
         <v>38</v>
       </c>
       <c r="B41" s="3">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>24</v>
@@ -4115,10 +4159,10 @@
         <v>39</v>
       </c>
       <c r="B42" s="5">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>24</v>
@@ -4136,10 +4180,10 @@
         <v>40</v>
       </c>
       <c r="B43" s="3">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>24</v>
@@ -4157,10 +4201,10 @@
         <v>41</v>
       </c>
       <c r="B44" s="5">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>721</v>
+        <v>41</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>24</v>
@@ -4178,10 +4222,10 @@
         <v>42</v>
       </c>
       <c r="B45" s="3">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>36</v>
+        <v>721</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>24</v>
@@ -4199,10 +4243,10 @@
         <v>43</v>
       </c>
       <c r="B46" s="5">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>24</v>
@@ -4220,10 +4264,10 @@
         <v>44</v>
       </c>
       <c r="B47" s="3">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>24</v>
@@ -4241,10 +4285,10 @@
         <v>45</v>
       </c>
       <c r="B48" s="5">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>24</v>
@@ -4262,10 +4306,10 @@
         <v>46</v>
       </c>
       <c r="B49" s="3">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>24</v>
@@ -4283,13 +4327,13 @@
         <v>47</v>
       </c>
       <c r="B50" s="5">
-        <v>165</v>
+        <v>57</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>765</v>
+        <v>38</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>231</v>
+        <v>24</v>
       </c>
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
@@ -4304,13 +4348,13 @@
         <v>48</v>
       </c>
       <c r="B51" s="3">
-        <v>250</v>
+        <v>165</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>792</v>
+        <v>765</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>634</v>
+        <v>231</v>
       </c>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -4325,13 +4369,13 @@
         <v>49</v>
       </c>
       <c r="B52" s="5">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
@@ -4346,13 +4390,13 @@
         <v>50</v>
       </c>
       <c r="B53" s="3">
-        <v>107</v>
+        <v>251</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>745</v>
+        <v>793</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>137</v>
+        <v>636</v>
       </c>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
@@ -4367,13 +4411,13 @@
         <v>51</v>
       </c>
       <c r="B54" s="5">
-        <v>288</v>
+        <v>107</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>802</v>
+        <v>745</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>657</v>
+        <v>137</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
@@ -4388,13 +4432,13 @@
         <v>52</v>
       </c>
       <c r="B55" s="3">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>678</v>
+        <v>802</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>679</v>
+        <v>657</v>
       </c>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
@@ -4409,13 +4453,13 @@
         <v>53</v>
       </c>
       <c r="B56" s="5">
-        <v>77</v>
+        <v>320</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>61</v>
+        <v>678</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>62</v>
+        <v>679</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
@@ -4430,13 +4474,13 @@
         <v>54</v>
       </c>
       <c r="B57" s="3">
-        <v>268</v>
+        <v>77</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>799</v>
+        <v>61</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>649</v>
+        <v>62</v>
       </c>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -4451,13 +4495,13 @@
         <v>55</v>
       </c>
       <c r="B58" s="5">
-        <v>132</v>
+        <v>268</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>189</v>
+        <v>799</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>190</v>
+        <v>649</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
@@ -4472,13 +4516,13 @@
         <v>56</v>
       </c>
       <c r="B59" s="3">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -4493,13 +4537,13 @@
         <v>57</v>
       </c>
       <c r="B60" s="5">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>754</v>
+        <v>193</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="8"/>
@@ -4514,13 +4558,13 @@
         <v>58</v>
       </c>
       <c r="B61" s="3">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -4535,13 +4579,13 @@
         <v>59</v>
       </c>
       <c r="B62" s="5">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>226</v>
+        <v>198</v>
       </c>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
@@ -4556,13 +4600,13 @@
         <v>60</v>
       </c>
       <c r="B63" s="3">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -4577,13 +4621,13 @@
         <v>61</v>
       </c>
       <c r="B64" s="5">
-        <v>244</v>
+        <v>174</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>790</v>
+        <v>770</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>462</v>
+        <v>244</v>
       </c>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
@@ -4598,13 +4642,13 @@
         <v>62</v>
       </c>
       <c r="B65" s="3">
-        <v>318</v>
+        <v>244</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>808</v>
+        <v>790</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>677</v>
+        <v>462</v>
       </c>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -4619,13 +4663,13 @@
         <v>63</v>
       </c>
       <c r="B66" s="5">
-        <v>263</v>
+        <v>318</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>644</v>
+        <v>808</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>645</v>
+        <v>677</v>
       </c>
       <c r="E66" s="8"/>
       <c r="F66" s="8"/>
@@ -4640,13 +4684,13 @@
         <v>64</v>
       </c>
       <c r="B67" s="3">
-        <v>54</v>
+        <v>263</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>720</v>
+        <v>644</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>24</v>
+        <v>645</v>
       </c>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -4661,10 +4705,10 @@
         <v>65</v>
       </c>
       <c r="B68" s="5">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>24</v>
@@ -4682,13 +4726,13 @@
         <v>66</v>
       </c>
       <c r="B69" s="3">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>29</v>
+        <v>719</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -4703,13 +4747,13 @@
         <v>67</v>
       </c>
       <c r="B70" s="5">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E70" s="8"/>
       <c r="F70" s="8"/>
@@ -4724,10 +4768,10 @@
         <v>68</v>
       </c>
       <c r="B71" s="3">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>24</v>
@@ -4745,13 +4789,13 @@
         <v>69</v>
       </c>
       <c r="B72" s="5">
-        <v>176</v>
+        <v>52</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>772</v>
+        <v>33</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>403</v>
+        <v>24</v>
       </c>
       <c r="E72" s="8"/>
       <c r="F72" s="8"/>
@@ -4766,13 +4810,13 @@
         <v>70</v>
       </c>
       <c r="B73" s="3">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>764</v>
+        <v>772</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>229</v>
+        <v>403</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
@@ -4787,13 +4831,13 @@
         <v>71</v>
       </c>
       <c r="B74" s="5">
-        <v>82</v>
+        <v>161</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>729</v>
+        <v>764</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>86</v>
+        <v>229</v>
       </c>
       <c r="E74" s="8"/>
       <c r="F74" s="8"/>
@@ -4808,13 +4852,13 @@
         <v>72</v>
       </c>
       <c r="B75" s="3">
-        <v>262</v>
+        <v>82</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>797</v>
+        <v>729</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>631</v>
+        <v>86</v>
       </c>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
@@ -4829,10 +4873,10 @@
         <v>73</v>
       </c>
       <c r="B76" s="5">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>631</v>
@@ -4850,13 +4894,13 @@
         <v>74</v>
       </c>
       <c r="B77" s="3">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>447</v>
+        <v>796</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>448</v>
+        <v>631</v>
       </c>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
@@ -4871,13 +4915,13 @@
         <v>75</v>
       </c>
       <c r="B78" s="5">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>794</v>
+        <v>447</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>631</v>
+        <v>448</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="8"/>
@@ -4892,10 +4936,10 @@
         <v>76</v>
       </c>
       <c r="B79" s="3">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>631</v>
@@ -4913,13 +4957,13 @@
         <v>77</v>
       </c>
       <c r="B80" s="5">
-        <v>100</v>
+        <v>249</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>741</v>
+        <v>791</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>117</v>
+        <v>631</v>
       </c>
       <c r="E80" s="8"/>
       <c r="F80" s="8"/>
@@ -4934,13 +4978,13 @@
         <v>78</v>
       </c>
       <c r="B81" s="3">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>177</v>
+        <v>117</v>
       </c>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
@@ -4955,13 +4999,13 @@
         <v>79</v>
       </c>
       <c r="B82" s="5">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>735</v>
+        <v>749</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>100</v>
+        <v>177</v>
       </c>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
@@ -4976,13 +5020,13 @@
         <v>80</v>
       </c>
       <c r="B83" s="3">
-        <v>315</v>
+        <v>94</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>674</v>
+        <v>735</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>675</v>
+        <v>100</v>
       </c>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
@@ -4997,13 +5041,13 @@
         <v>81</v>
       </c>
       <c r="B84" s="5">
-        <v>197</v>
+        <v>315</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>777</v>
+        <v>674</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>418</v>
+        <v>675</v>
       </c>
       <c r="E84" s="8"/>
       <c r="F84" s="8"/>
@@ -5018,13 +5062,13 @@
         <v>82</v>
       </c>
       <c r="B85" s="3">
-        <v>109</v>
+        <v>197</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>161</v>
+        <v>777</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>162</v>
+        <v>418</v>
       </c>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -5039,13 +5083,13 @@
         <v>83</v>
       </c>
       <c r="B86" s="5">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="E86" s="8"/>
       <c r="F86" s="8"/>
@@ -5060,13 +5104,13 @@
         <v>84</v>
       </c>
       <c r="B87" s="3">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>27</v>
+        <v>89</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -5081,13 +5125,13 @@
         <v>85</v>
       </c>
       <c r="B88" s="5">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="E88" s="8"/>
       <c r="F88" s="8"/>
@@ -5102,13 +5146,13 @@
         <v>86</v>
       </c>
       <c r="B89" s="3">
-        <v>221</v>
+        <v>78</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>782</v>
+        <v>63</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>433</v>
+        <v>64</v>
       </c>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -5123,13 +5167,13 @@
         <v>87</v>
       </c>
       <c r="B90" s="5">
-        <v>333</v>
+        <v>221</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>680</v>
+        <v>782</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>681</v>
+        <v>433</v>
       </c>
       <c r="E90" s="8"/>
       <c r="F90" s="8"/>
@@ -5144,13 +5188,13 @@
         <v>88</v>
       </c>
       <c r="B91" s="3">
-        <v>79</v>
+        <v>333</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>727</v>
+        <v>680</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>66</v>
+        <v>681</v>
       </c>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
@@ -5165,13 +5209,13 @@
         <v>89</v>
       </c>
       <c r="B92" s="5">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>737</v>
+        <v>727</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="E92" s="8"/>
       <c r="F92" s="8"/>
@@ -5186,13 +5230,13 @@
         <v>90</v>
       </c>
       <c r="B93" s="3">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -5207,13 +5251,13 @@
         <v>91</v>
       </c>
       <c r="B94" s="5">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>731</v>
+        <v>739</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="E94" s="8"/>
       <c r="F94" s="8"/>
@@ -5228,13 +5272,13 @@
         <v>92</v>
       </c>
       <c r="B95" s="3">
-        <v>237</v>
+        <v>88</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>450</v>
+        <v>731</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>451</v>
+        <v>92</v>
       </c>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
@@ -5249,13 +5293,13 @@
         <v>93</v>
       </c>
       <c r="B96" s="5">
-        <v>203</v>
+        <v>237</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>779</v>
+        <v>450</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>426</v>
+        <v>451</v>
       </c>
       <c r="E96" s="8"/>
       <c r="F96" s="8"/>
@@ -5270,13 +5314,13 @@
         <v>94</v>
       </c>
       <c r="B97" s="3">
-        <v>105</v>
+        <v>203</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>130</v>
+        <v>779</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>131</v>
+        <v>426</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
@@ -5291,13 +5335,13 @@
         <v>95</v>
       </c>
       <c r="B98" s="5">
-        <v>206</v>
+        <v>105</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>780</v>
+        <v>130</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>233</v>
+        <v>131</v>
       </c>
       <c r="E98" s="8"/>
       <c r="F98" s="8"/>
@@ -5312,10 +5356,10 @@
         <v>96</v>
       </c>
       <c r="B99" s="3">
-        <v>167</v>
+        <v>206</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>232</v>
+        <v>780</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>233</v>
@@ -5333,13 +5377,13 @@
         <v>97</v>
       </c>
       <c r="B100" s="5">
-        <v>290</v>
+        <v>167</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>803</v>
+        <v>232</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>660</v>
+        <v>233</v>
       </c>
       <c r="E100" s="8"/>
       <c r="F100" s="8"/>
@@ -5354,13 +5398,13 @@
         <v>98</v>
       </c>
       <c r="B101" s="3">
-        <v>228</v>
+        <v>290</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>785</v>
+        <v>803</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>441</v>
+        <v>660</v>
       </c>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -5375,13 +5419,13 @@
         <v>99</v>
       </c>
       <c r="B102" s="5">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>627</v>
+        <v>785</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>628</v>
+        <v>441</v>
       </c>
       <c r="E102" s="8"/>
       <c r="F102" s="8"/>
@@ -5396,13 +5440,13 @@
         <v>100</v>
       </c>
       <c r="B103" s="3">
-        <v>142</v>
+        <v>248</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>755</v>
+        <v>627</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>202</v>
+        <v>628</v>
       </c>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
@@ -5417,13 +5461,13 @@
         <v>101</v>
       </c>
       <c r="B104" s="5">
-        <v>95</v>
+        <v>142</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>736</v>
+        <v>755</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
       <c r="E104" s="8"/>
       <c r="F104" s="8"/>
@@ -5438,13 +5482,13 @@
         <v>102</v>
       </c>
       <c r="B105" s="3">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>750</v>
+        <v>736</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>179</v>
+        <v>102</v>
       </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
@@ -5459,13 +5503,13 @@
         <v>103</v>
       </c>
       <c r="B106" s="5">
-        <v>309</v>
+        <v>126</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>806</v>
+        <v>750</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>671</v>
+        <v>179</v>
       </c>
       <c r="E106" s="8"/>
       <c r="F106" s="8"/>
@@ -5480,13 +5524,13 @@
         <v>104</v>
       </c>
       <c r="B107" s="3">
-        <v>179</v>
+        <v>309</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>773</v>
+        <v>806</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>406</v>
+        <v>671</v>
       </c>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
@@ -5501,13 +5545,13 @@
         <v>105</v>
       </c>
       <c r="B108" s="5">
-        <v>66</v>
+        <v>179</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>723</v>
+        <v>773</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>24</v>
+        <v>406</v>
       </c>
       <c r="E108" s="8"/>
       <c r="F108" s="8"/>
@@ -5522,10 +5566,10 @@
         <v>106</v>
       </c>
       <c r="B109" s="3">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>31</v>
+        <v>723</v>
       </c>
       <c r="D109" s="3" t="s">
         <v>24</v>
@@ -5543,13 +5587,13 @@
         <v>107</v>
       </c>
       <c r="B110" s="5">
-        <v>169</v>
+        <v>50</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>766</v>
+        <v>31</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>235</v>
+        <v>24</v>
       </c>
       <c r="E110" s="8"/>
       <c r="F110" s="8"/>
@@ -5564,13 +5608,13 @@
         <v>108</v>
       </c>
       <c r="B111" s="3">
-        <v>65</v>
+        <v>169</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>722</v>
+        <v>766</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>46</v>
+        <v>235</v>
       </c>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -5585,13 +5629,13 @@
         <v>109</v>
       </c>
       <c r="B112" s="5">
-        <v>133</v>
+        <v>65</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>191</v>
+        <v>722</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>192</v>
+        <v>46</v>
       </c>
       <c r="E112" s="8"/>
       <c r="F112" s="8"/>
@@ -5606,13 +5650,13 @@
         <v>110</v>
       </c>
       <c r="B113" s="3">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>768</v>
+        <v>191</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
@@ -5627,13 +5671,13 @@
         <v>111</v>
       </c>
       <c r="B114" s="5">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>733</v>
+        <v>768</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>96</v>
+        <v>240</v>
       </c>
       <c r="E114" s="8"/>
       <c r="F114" s="8"/>
@@ -5648,13 +5692,13 @@
         <v>112</v>
       </c>
       <c r="B115" s="3">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>756</v>
+        <v>733</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>205</v>
+        <v>96</v>
       </c>
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
@@ -5669,13 +5713,13 @@
         <v>113</v>
       </c>
       <c r="B116" s="5">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>743</v>
+        <v>756</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>129</v>
+        <v>205</v>
       </c>
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
@@ -5690,13 +5734,13 @@
         <v>114</v>
       </c>
       <c r="B117" s="3">
-        <v>172</v>
+        <v>103</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>769</v>
+        <v>743</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>242</v>
+        <v>129</v>
       </c>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
@@ -5711,13 +5755,13 @@
         <v>115</v>
       </c>
       <c r="B118" s="5">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>748</v>
+        <v>769</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>175</v>
+        <v>242</v>
       </c>
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
@@ -5732,13 +5776,13 @@
         <v>116</v>
       </c>
       <c r="B119" s="3">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>738</v>
+        <v>748</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
@@ -5753,13 +5797,13 @@
         <v>117</v>
       </c>
       <c r="B120" s="5">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>25</v>
+        <v>738</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
@@ -5774,13 +5818,13 @@
         <v>118</v>
       </c>
       <c r="B121" s="3">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="E121" s="7"/>
       <c r="F121" s="7"/>
@@ -5795,13 +5839,13 @@
         <v>119</v>
       </c>
       <c r="B122" s="5">
-        <v>213</v>
+        <v>72</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>428</v>
+        <v>56</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>429</v>
+        <v>57</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
@@ -5816,13 +5860,13 @@
         <v>120</v>
       </c>
       <c r="B123" s="3">
-        <v>157</v>
+        <v>213</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>760</v>
+        <v>428</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>219</v>
+        <v>429</v>
       </c>
       <c r="E123" s="7"/>
       <c r="F123" s="7"/>
@@ -5837,13 +5881,13 @@
         <v>121</v>
       </c>
       <c r="B124" s="5">
-        <v>222</v>
+        <v>157</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>783</v>
+        <v>760</v>
       </c>
       <c r="D124" s="5" t="s">
-        <v>437</v>
+        <v>219</v>
       </c>
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
@@ -5858,13 +5902,13 @@
         <v>122</v>
       </c>
       <c r="B125" s="3">
-        <v>158</v>
+        <v>222</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>761</v>
+        <v>783</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>221</v>
+        <v>437</v>
       </c>
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
@@ -5879,13 +5923,13 @@
         <v>123</v>
       </c>
       <c r="B126" s="5">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
@@ -5900,13 +5944,13 @@
         <v>124</v>
       </c>
       <c r="B127" s="3">
-        <v>266</v>
+        <v>170</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>798</v>
+        <v>767</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>647</v>
+        <v>238</v>
       </c>
       <c r="E127" s="7"/>
       <c r="F127" s="7"/>
@@ -5921,13 +5965,13 @@
         <v>125</v>
       </c>
       <c r="B128" s="5">
-        <v>76</v>
+        <v>266</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>59</v>
+        <v>798</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>60</v>
+        <v>647</v>
       </c>
       <c r="E128" s="8"/>
       <c r="F128" s="8"/>
@@ -5942,13 +5986,13 @@
         <v>126</v>
       </c>
       <c r="B129" s="3">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>747</v>
+        <v>59</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>167</v>
+        <v>60</v>
       </c>
       <c r="E129" s="7"/>
       <c r="F129" s="7"/>
@@ -5963,13 +6007,13 @@
         <v>127</v>
       </c>
       <c r="B130" s="5">
-        <v>295</v>
+        <v>114</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>805</v>
+        <v>747</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>665</v>
+        <v>167</v>
       </c>
       <c r="E130" s="8"/>
       <c r="F130" s="8"/>
@@ -5984,13 +6028,13 @@
         <v>128</v>
       </c>
       <c r="B131" s="3">
-        <v>218</v>
+        <v>295</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>781</v>
+        <v>805</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>431</v>
+        <v>665</v>
       </c>
       <c r="E131" s="7"/>
       <c r="F131" s="7"/>
@@ -6005,13 +6049,13 @@
         <v>129</v>
       </c>
       <c r="B132" s="5">
-        <v>195</v>
+        <v>218</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>776</v>
+        <v>781</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="E132" s="8"/>
       <c r="F132" s="8"/>
@@ -6026,13 +6070,13 @@
         <v>130</v>
       </c>
       <c r="B133" s="3">
-        <v>287</v>
+        <v>195</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>801</v>
+        <v>776</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>653</v>
+        <v>414</v>
       </c>
       <c r="E133" s="7"/>
       <c r="F133" s="7"/>
@@ -6047,13 +6091,13 @@
         <v>131</v>
       </c>
       <c r="B134" s="5">
-        <v>242</v>
+        <v>287</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>789</v>
+        <v>801</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>456</v>
+        <v>653</v>
       </c>
       <c r="E134" s="8"/>
       <c r="F134" s="8"/>
@@ -6068,13 +6112,13 @@
         <v>132</v>
       </c>
       <c r="B135" s="3">
-        <v>99</v>
+        <v>242</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>740</v>
+        <v>789</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>115</v>
+        <v>456</v>
       </c>
       <c r="E135" s="7"/>
       <c r="F135" s="7"/>
@@ -6089,13 +6133,13 @@
         <v>133</v>
       </c>
       <c r="B136" s="5">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>752</v>
+        <v>740</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>196</v>
+        <v>115</v>
       </c>
       <c r="E136" s="8"/>
       <c r="F136" s="8"/>
@@ -6110,13 +6154,13 @@
         <v>134</v>
       </c>
       <c r="B137" s="3">
-        <v>191</v>
+        <v>137</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>775</v>
+        <v>752</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>412</v>
+        <v>196</v>
       </c>
       <c r="E137" s="7"/>
       <c r="F137" s="7"/>
@@ -6131,13 +6175,13 @@
         <v>135</v>
       </c>
       <c r="B138" s="5">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="E138" s="8"/>
       <c r="F138" s="8"/>
@@ -6152,13 +6196,13 @@
         <v>136</v>
       </c>
       <c r="B139" s="3">
-        <v>260</v>
+        <v>201</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>640</v>
+        <v>778</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>641</v>
+        <v>422</v>
       </c>
       <c r="E139" s="7"/>
       <c r="F139" s="7"/>
@@ -6173,13 +6217,13 @@
         <v>137</v>
       </c>
       <c r="B140" s="5">
-        <v>71</v>
+        <v>260</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>54</v>
+        <v>640</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>55</v>
+        <v>641</v>
       </c>
       <c r="E140" s="8"/>
       <c r="F140" s="8"/>
@@ -6194,13 +6238,13 @@
         <v>138</v>
       </c>
       <c r="B141" s="3">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>725</v>
+        <v>54</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E141" s="7"/>
       <c r="F141" s="7"/>
@@ -6215,13 +6259,13 @@
         <v>139</v>
       </c>
       <c r="B142" s="5">
-        <v>259</v>
+        <v>68</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>795</v>
+        <v>725</v>
       </c>
       <c r="D142" s="5" t="s">
-        <v>639</v>
+        <v>51</v>
       </c>
       <c r="E142" s="8"/>
       <c r="F142" s="8"/>
@@ -6236,13 +6280,13 @@
         <v>140</v>
       </c>
       <c r="B143" s="3">
-        <v>130</v>
+        <v>259</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>183</v>
+        <v>795</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>184</v>
+        <v>639</v>
       </c>
       <c r="E143" s="7"/>
       <c r="F143" s="7"/>
@@ -6257,13 +6301,13 @@
         <v>141</v>
       </c>
       <c r="B144" s="5">
-        <v>46</v>
+        <v>130</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>23</v>
+        <v>183</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>24</v>
+        <v>184</v>
       </c>
       <c r="E144" s="8"/>
       <c r="F144" s="8"/>
@@ -6278,13 +6322,13 @@
         <v>142</v>
       </c>
       <c r="B145" s="3">
-        <v>312</v>
+        <v>46</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>807</v>
+        <v>23</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>673</v>
+        <v>24</v>
       </c>
       <c r="E145" s="7"/>
       <c r="F145" s="7"/>
@@ -6299,13 +6343,13 @@
         <v>143</v>
       </c>
       <c r="B146" s="5">
-        <v>70</v>
+        <v>312</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>726</v>
+        <v>807</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>53</v>
+        <v>673</v>
       </c>
       <c r="E146" s="8"/>
       <c r="F146" s="8"/>
@@ -6320,13 +6364,13 @@
         <v>144</v>
       </c>
       <c r="B147" s="3">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>751</v>
+        <v>726</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>182</v>
+        <v>53</v>
       </c>
       <c r="E147" s="7"/>
       <c r="F147" s="7"/>
@@ -6341,13 +6385,13 @@
         <v>145</v>
       </c>
       <c r="B148" s="5">
-        <v>67</v>
+        <v>129</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>724</v>
+        <v>751</v>
       </c>
       <c r="D148" s="5" t="s">
-        <v>49</v>
+        <v>182</v>
       </c>
       <c r="E148" s="8"/>
       <c r="F148" s="8"/>
@@ -6362,13 +6406,13 @@
         <v>146</v>
       </c>
       <c r="B149" s="3">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>759</v>
+        <v>724</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>217</v>
+        <v>49</v>
       </c>
       <c r="E149" s="7"/>
       <c r="F149" s="7"/>
@@ -6383,13 +6427,13 @@
         <v>147</v>
       </c>
       <c r="B150" s="5">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>163</v>
+        <v>759</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="E150" s="8"/>
       <c r="F150" s="8"/>
@@ -6404,13 +6448,13 @@
         <v>148</v>
       </c>
       <c r="B151" s="3">
-        <v>338</v>
+        <v>110</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>696</v>
+        <v>163</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>697</v>
+        <v>164</v>
       </c>
       <c r="E151" s="7"/>
       <c r="F151" s="7"/>
@@ -6425,13 +6469,13 @@
         <v>149</v>
       </c>
       <c r="B152" s="5">
-        <v>118</v>
+        <v>338</v>
       </c>
       <c r="C152" s="5" t="s">
-        <v>171</v>
+        <v>696</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>172</v>
+        <v>697</v>
       </c>
       <c r="E152" s="8"/>
       <c r="F152" s="8"/>
@@ -6446,13 +6490,13 @@
         <v>150</v>
       </c>
       <c r="B153" s="3">
-        <v>294</v>
+        <v>118</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>804</v>
+        <v>171</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>663</v>
+        <v>172</v>
       </c>
       <c r="E153" s="7"/>
       <c r="F153" s="7"/>
@@ -6467,13 +6511,13 @@
         <v>151</v>
       </c>
       <c r="B154" s="5">
-        <v>240</v>
+        <v>294</v>
       </c>
       <c r="C154" s="5" t="s">
-        <v>788</v>
+        <v>804</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>453</v>
+        <v>663</v>
       </c>
       <c r="E154" s="8"/>
       <c r="F154" s="8"/>
@@ -6488,13 +6532,13 @@
         <v>152</v>
       </c>
       <c r="B155" s="3">
-        <v>84</v>
+        <v>240</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>730</v>
+        <v>788</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>88</v>
+        <v>453</v>
       </c>
       <c r="E155" s="7"/>
       <c r="F155" s="7"/>
@@ -6509,13 +6553,13 @@
         <v>153</v>
       </c>
       <c r="B156" s="5">
-        <v>303</v>
+        <v>84</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>666</v>
+        <v>730</v>
       </c>
       <c r="D156" s="5" t="s">
-        <v>667</v>
+        <v>88</v>
       </c>
       <c r="E156" s="8"/>
       <c r="F156" s="8"/>
@@ -6530,13 +6574,13 @@
         <v>154</v>
       </c>
       <c r="B157" s="3">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="E157" s="7"/>
       <c r="F157" s="7"/>
@@ -6546,14 +6590,35 @@
       <c r="J157" s="4"/>
       <c r="K157" s="3"/>
     </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A158" s="5">
+        <v>155</v>
+      </c>
+      <c r="B158" s="5">
+        <v>304</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>668</v>
+      </c>
+      <c r="D158" s="5" t="s">
+        <v>669</v>
+      </c>
+      <c r="E158" s="8"/>
+      <c r="F158" s="8"/>
+      <c r="G158" s="8"/>
+      <c r="H158" s="8"/>
+      <c r="I158" s="6"/>
+      <c r="J158" s="6"/>
+      <c r="K158" s="5"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:K2" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K157">
-    <sortCondition ref="F4:F157"/>
-    <sortCondition ref="E4:E157"/>
-    <sortCondition ref="A4:A157"/>
-    <sortCondition ref="C4:C157"/>
-    <sortCondition ref="B4:B157"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K158">
+    <sortCondition ref="F4:F158"/>
+    <sortCondition ref="E4:E158"/>
+    <sortCondition ref="A4:A158"/>
+    <sortCondition ref="C4:C158"/>
+    <sortCondition ref="B4:B158"/>
   </sortState>
   <mergeCells count="8">
     <mergeCell ref="K1:K2"/>
@@ -6566,7 +6631,8 @@
     <mergeCell ref="J1:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6575,8 +6641,8 @@
   <dimension ref="A1:O599"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A576" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8805,7 +8871,7 @@
       <c r="N69" s="7"/>
       <c r="O69" s="4"/>
     </row>
-    <row r="70" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>68</v>
       </c>
@@ -22684,7 +22750,7 @@
       <c r="N488" s="8"/>
       <c r="O488" s="6"/>
     </row>
-    <row r="489" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A489" s="3">
         <v>487</v>
       </c>
@@ -24885,7 +24951,7 @@
       <c r="N551" s="7"/>
       <c r="O551" s="4"/>
     </row>
-    <row r="552" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A552" s="5">
         <v>550</v>
       </c>
@@ -25754,7 +25820,7 @@
       <c r="N578" s="8"/>
       <c r="O578" s="6"/>
     </row>
-    <row r="579" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A579" s="3">
         <v>577</v>
       </c>

</xml_diff>

<commit_message>
Se inicia desarrollo del módulo 'conv_sin_exp'.
Se modifica plan de trabajo.
Se modifica el Main y se agregan los archivos correspondientes a la nueva funcionalidad.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C06351B-BD8B-45E1-B2FB-95EFE37CDA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59292F37-DC70-4286-B29A-FE581BA19F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4137" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4140" uniqueCount="849">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2685,6 +2685,15 @@
   </si>
   <si>
     <t>Ambos</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Enrique</t>
+  </si>
+  <si>
+    <t>08/05/2025: Se inicia desarrollo del módulo.</t>
   </si>
 </sst>
 </file>
@@ -2857,6 +2866,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2883,9 +2895,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3220,7 +3229,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:E14"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3240,47 +3249,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>814</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="25" t="s">
         <v>840</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="25" t="s">
         <v>841</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>704</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="18" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="19" t="s">
         <v>716</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="23" t="s">
         <v>837</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="18" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
       <c r="G2" s="9" t="s">
         <v>705</v>
       </c>
@@ -3293,9 +3302,9 @@
       <c r="J2" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="K2" s="19"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="17"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -3310,10 +3319,10 @@
       <c r="D3" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="17" t="s">
         <v>842</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="17" t="s">
         <v>842</v>
       </c>
       <c r="G3" s="7" t="s">
@@ -3659,7 +3668,9 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>846</v>
+      </c>
       <c r="L14" s="6"/>
       <c r="M14" s="5"/>
     </row>
@@ -3934,9 +3945,13 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="4"/>
+      <c r="K25" s="4" t="s">
+        <v>847</v>
+      </c>
       <c r="L25" s="4"/>
-      <c r="M25" s="3"/>
+      <c r="M25" s="3" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -7323,42 +7338,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>710</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -7386,7 +7401,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="21"/>
+      <c r="O2" s="22"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">

</xml_diff>

<commit_message>
Agrego columna al Plan de Trabajo para indicar la fecha de inicio del desarrollo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59292F37-DC70-4286-B29A-FE581BA19F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D867C0B9-F072-4C25-B325-92AC360A2991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Detalle" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$M$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$N$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$2:$O$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -86,7 +86,7 @@
     Nombre de la función principal a ejecutar en el código del Spooler.</t>
       </text>
     </comment>
-    <comment ref="K1" authorId="4" shapeId="0" xr:uid="{1A01895E-B4CA-43D8-9D26-987A1667FAE7}">
+    <comment ref="L1" authorId="4" shapeId="0" xr:uid="{1A01895E-B4CA-43D8-9D26-987A1667FAE7}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -94,7 +94,7 @@
     Nombre de la persona que migró el módulo.</t>
       </text>
     </comment>
-    <comment ref="L1" authorId="5" shapeId="0" xr:uid="{38372124-5616-401A-B40A-476DE7B44D8B}">
+    <comment ref="M1" authorId="5" shapeId="0" xr:uid="{38372124-5616-401A-B40A-476DE7B44D8B}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -102,7 +102,7 @@
     Nombre de la persona que migró el módulo.</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="6" shapeId="0" xr:uid="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
+    <comment ref="N1" authorId="6" shapeId="0" xr:uid="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -110,7 +110,7 @@
     Observaciones o comentarios que se consideren importantes al migrar un módulo.</t>
       </text>
     </comment>
-    <comment ref="G2" authorId="7" shapeId="0" xr:uid="{B56B010C-6EB7-4B4F-9D8B-5579B701198E}">
+    <comment ref="H2" authorId="7" shapeId="0" xr:uid="{B56B010C-6EB7-4B4F-9D8B-5579B701198E}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -118,7 +118,7 @@
     El proceso ya se terminó en código local y es funcional.</t>
       </text>
     </comment>
-    <comment ref="H2" authorId="8" shapeId="0" xr:uid="{7F63E4B1-80CD-4575-908F-B1DCA061309F}">
+    <comment ref="I2" authorId="8" shapeId="0" xr:uid="{7F63E4B1-80CD-4575-908F-B1DCA061309F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -126,7 +126,7 @@
     El proceso se publicó y se validó en el Srv. de Desarrollo de forma satisfactoria.</t>
       </text>
     </comment>
-    <comment ref="I2" authorId="9" shapeId="0" xr:uid="{A93D80C5-D95F-45C9-9060-63249C22896D}">
+    <comment ref="J2" authorId="9" shapeId="0" xr:uid="{A93D80C5-D95F-45C9-9060-63249C22896D}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -134,7 +134,7 @@
     El proceso se publicó y se validó en el Srv. de Q.A.  de forma satisfactoria.</t>
       </text>
     </comment>
-    <comment ref="J2" authorId="10" shapeId="0" xr:uid="{08706989-DEF6-4746-8EDE-FFB49503C0FE}">
+    <comment ref="K2" authorId="10" shapeId="0" xr:uid="{08706989-DEF6-4746-8EDE-FFB49503C0FE}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4140" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="850">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2694,6 +2694,9 @@
   </si>
   <si>
     <t>08/05/2025: Se inicia desarrollo del módulo.</t>
+  </si>
+  <si>
+    <t>Fecha de inicio</t>
   </si>
 </sst>
 </file>
@@ -2816,7 +2819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2895,6 +2898,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3199,25 +3223,25 @@
   <threadedComment ref="D1" dT="2025-04-23T23:38:16.12" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{BBAD5277-51BC-4EC1-B176-090510E4CD69}">
     <text>Nombre de la función principal a ejecutar en el código del Spooler.</text>
   </threadedComment>
-  <threadedComment ref="K1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{1A01895E-B4CA-43D8-9D26-987A1667FAE7}">
+  <threadedComment ref="L1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{1A01895E-B4CA-43D8-9D26-987A1667FAE7}">
     <text>Nombre de la persona que migró el módulo.</text>
   </threadedComment>
-  <threadedComment ref="L1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{38372124-5616-401A-B40A-476DE7B44D8B}">
+  <threadedComment ref="M1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{38372124-5616-401A-B40A-476DE7B44D8B}">
     <text>Nombre de la persona que migró el módulo.</text>
   </threadedComment>
-  <threadedComment ref="M1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
+  <threadedComment ref="N1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
     <text>Observaciones o comentarios que se consideren importantes al migrar un módulo.</text>
   </threadedComment>
-  <threadedComment ref="G2" dT="2025-04-23T23:33:08.08" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{B56B010C-6EB7-4B4F-9D8B-5579B701198E}">
+  <threadedComment ref="H2" dT="2025-04-23T23:33:08.08" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{B56B010C-6EB7-4B4F-9D8B-5579B701198E}">
     <text>El proceso ya se terminó en código local y es funcional.</text>
   </threadedComment>
-  <threadedComment ref="H2" dT="2025-04-23T23:33:37.68" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{7F63E4B1-80CD-4575-908F-B1DCA061309F}">
+  <threadedComment ref="I2" dT="2025-04-23T23:33:37.68" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{7F63E4B1-80CD-4575-908F-B1DCA061309F}">
     <text>El proceso se publicó y se validó en el Srv. de Desarrollo de forma satisfactoria.</text>
   </threadedComment>
-  <threadedComment ref="I2" dT="2025-04-23T23:33:56.94" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{A93D80C5-D95F-45C9-9060-63249C22896D}">
+  <threadedComment ref="J2" dT="2025-04-23T23:33:56.94" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{A93D80C5-D95F-45C9-9060-63249C22896D}">
     <text>El proceso se publicó y se validó en el Srv. de Q.A.  de forma satisfactoria.</text>
   </threadedComment>
-  <threadedComment ref="J2" dT="2025-04-23T23:34:10.38" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{08706989-DEF6-4746-8EDE-FFB49503C0FE}">
+  <threadedComment ref="K2" dT="2025-04-23T23:34:10.38" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{08706989-DEF6-4746-8EDE-FFB49503C0FE}">
     <text>El proceso se publicó y se validó en el Srv. Productivo de forma satisfactoria.</text>
   </threadedComment>
 </ThreadedComments>
@@ -3225,7 +3249,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
-  <dimension ref="A1:M158"/>
+  <dimension ref="A1:N158"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -3239,16 +3263,17 @@
     <col min="3" max="3" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="13" width="72.5703125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="15" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="72.5703125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>814</v>
       </c>
@@ -3267,46 +3292,50 @@
       <c r="F1" s="25" t="s">
         <v>841</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="28" t="s">
+        <v>849</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>704</v>
       </c>
-      <c r="H1" s="21"/>
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="19" t="s">
         <v>716</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="M1" s="23" t="s">
         <v>837</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="29"/>
+      <c r="H2" s="9" t="s">
         <v>705</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>706</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>707</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="K2" s="20"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="18"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L2" s="20"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="18"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -3325,23 +3354,24 @@
       <c r="F3" s="17" t="s">
         <v>842</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>711</v>
-      </c>
+      <c r="G3" s="27"/>
       <c r="H3" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7" t="s">
+        <v>711</v>
+      </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="7"/>
+      <c r="L3" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4"/>
+      <c r="N3" s="3" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -3358,23 +3388,24 @@
         <v>843</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="8" t="s">
-        <v>711</v>
-      </c>
+      <c r="G4" s="30"/>
       <c r="H4" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>711</v>
+      </c>
       <c r="J4" s="8"/>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="8"/>
+      <c r="L4" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="L4" s="6">
+      <c r="M4" s="6">
         <v>3723307</v>
       </c>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -3391,23 +3422,24 @@
         <v>843</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="7" t="s">
-        <v>711</v>
-      </c>
+      <c r="G5" s="27"/>
       <c r="H5" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>711</v>
+      </c>
       <c r="J5" s="7"/>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="7"/>
+      <c r="L5" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="L5" s="4">
+      <c r="M5" s="4">
         <v>6651805</v>
       </c>
-      <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -3424,23 +3456,24 @@
         <v>843</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="8" t="s">
-        <v>711</v>
-      </c>
+      <c r="G6" s="30"/>
       <c r="H6" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="8" t="s">
+        <v>711</v>
+      </c>
       <c r="J6" s="8"/>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="8"/>
+      <c r="L6" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="L6" s="6">
+      <c r="M6" s="6">
         <v>4220496</v>
       </c>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -3457,23 +3490,24 @@
         <v>843</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="7" t="s">
-        <v>711</v>
-      </c>
+      <c r="G7" s="27"/>
       <c r="H7" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="I7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>711</v>
+      </c>
       <c r="J7" s="7"/>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="7"/>
+      <c r="L7" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="L7" s="4">
+      <c r="M7" s="4">
         <v>5566768</v>
       </c>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -3490,23 +3524,24 @@
         <v>844</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="8" t="s">
-        <v>711</v>
-      </c>
+      <c r="G8" s="30"/>
       <c r="H8" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8" t="s">
+        <v>711</v>
+      </c>
       <c r="J8" s="8"/>
-      <c r="K8" s="6" t="s">
+      <c r="K8" s="8"/>
+      <c r="L8" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <v>5545714</v>
       </c>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -3523,23 +3558,24 @@
         <v>844</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="7" t="s">
-        <v>711</v>
-      </c>
+      <c r="G9" s="27"/>
       <c r="H9" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="I9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>711</v>
+      </c>
       <c r="J9" s="7"/>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="7"/>
+      <c r="L9" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="L9" s="4">
+      <c r="M9" s="4">
         <v>7774047</v>
       </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -3556,23 +3592,24 @@
         <v>844</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="8" t="s">
-        <v>711</v>
-      </c>
+      <c r="G10" s="30"/>
       <c r="H10" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="8" t="s">
+        <v>711</v>
+      </c>
       <c r="J10" s="8"/>
-      <c r="K10" s="6" t="s">
+      <c r="K10" s="8"/>
+      <c r="L10" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="6">
         <v>7864811</v>
       </c>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="5"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -3589,15 +3626,16 @@
         <v>843</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="4"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="4"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -3614,15 +3652,16 @@
         <v>843</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="8"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
-      <c r="K12" s="6"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="5"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="6"/>
+      <c r="N12" s="5"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -3639,15 +3678,16 @@
         <v>843</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="7"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="4"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="3"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="4"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -3664,17 +3704,18 @@
         <v>843</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="8"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
-      <c r="K14" s="6" t="s">
+      <c r="K14" s="8"/>
+      <c r="L14" s="6" t="s">
         <v>846</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="5"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="6"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -3691,15 +3732,16 @@
         <v>844</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-      <c r="K15" s="4"/>
+      <c r="K15" s="7"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="3"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="4"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -3716,15 +3758,16 @@
         <v>844</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="8"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
-      <c r="K16" s="6"/>
+      <c r="K16" s="8"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="5"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="6"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -3741,15 +3784,16 @@
         <v>844</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="4"/>
+      <c r="K17" s="7"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="4"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -3766,15 +3810,16 @@
         <v>844</v>
       </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="8"/>
+      <c r="G18" s="30"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
-      <c r="K18" s="6"/>
+      <c r="K18" s="8"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="6"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -3791,15 +3836,16 @@
         <v>844</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="7"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-      <c r="K19" s="4"/>
+      <c r="K19" s="7"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="3"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="4"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -3816,15 +3862,16 @@
         <v>844</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" s="8"/>
+      <c r="G20" s="30"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
-      <c r="K20" s="6"/>
+      <c r="K20" s="8"/>
       <c r="L20" s="6"/>
-      <c r="M20" s="5"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="6"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -3841,15 +3888,16 @@
         <v>843</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="7"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="4"/>
+      <c r="K21" s="7"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="3"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="4"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>19</v>
       </c>
@@ -3866,15 +3914,16 @@
         <v>843</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="8"/>
+      <c r="G22" s="30"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
-      <c r="K22" s="6"/>
+      <c r="K22" s="8"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="6"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -3891,15 +3940,16 @@
         <v>843</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="7"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="4"/>
+      <c r="K23" s="7"/>
       <c r="L23" s="4"/>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="4"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>21</v>
       </c>
@@ -3916,15 +3966,16 @@
         <v>843</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="8"/>
+      <c r="G24" s="30"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
-      <c r="K24" s="6"/>
+      <c r="K24" s="8"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="5"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="6"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -3941,19 +3992,22 @@
         <v>844</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="7"/>
+      <c r="G25" s="27">
+        <v>45785</v>
+      </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="4" t="s">
+      <c r="K25" s="7"/>
+      <c r="L25" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="L25" s="4"/>
-      <c r="M25" s="3" t="s">
+      <c r="M25" s="4"/>
+      <c r="N25" s="3" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>23</v>
       </c>
@@ -3970,15 +4024,16 @@
         <v>845</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="8"/>
+      <c r="G26" s="30"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="6"/>
+      <c r="K26" s="8"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="5"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="6"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -3995,15 +4050,16 @@
         <v>845</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="7"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
-      <c r="K27" s="4"/>
+      <c r="K27" s="7"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="3"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="4"/>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>25</v>
       </c>
@@ -4020,15 +4076,16 @@
         <v>844</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="8"/>
+      <c r="G28" s="30"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
-      <c r="K28" s="6"/>
+      <c r="K28" s="8"/>
       <c r="L28" s="6"/>
-      <c r="M28" s="5"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M28" s="6"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -4045,15 +4102,16 @@
         <v>843</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="7"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="7"/>
       <c r="L29" s="4"/>
-      <c r="M29" s="3"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="4"/>
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>27</v>
       </c>
@@ -4070,15 +4128,16 @@
         <v>843</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" s="8"/>
+      <c r="G30" s="30"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
-      <c r="K30" s="6"/>
+      <c r="K30" s="8"/>
       <c r="L30" s="6"/>
-      <c r="M30" s="5"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M30" s="6"/>
+      <c r="N30" s="5"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -4095,17 +4154,18 @@
         <v>845</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="7"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="7"/>
+      <c r="L31" s="4" t="s">
         <v>833</v>
       </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="3"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M31" s="4"/>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>29</v>
       </c>
@@ -4122,15 +4182,16 @@
         <v>845</v>
       </c>
       <c r="F32" s="5"/>
-      <c r="G32" s="8"/>
+      <c r="G32" s="30"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
-      <c r="K32" s="6"/>
+      <c r="K32" s="8"/>
       <c r="L32" s="6"/>
-      <c r="M32" s="5"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M32" s="6"/>
+      <c r="N32" s="5"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -4147,15 +4208,16 @@
         <v>844</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="7"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
-      <c r="K33" s="4"/>
+      <c r="K33" s="7"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="3"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="4"/>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>31</v>
       </c>
@@ -4172,17 +4234,18 @@
         <v>845</v>
       </c>
       <c r="F34" s="5"/>
-      <c r="G34" s="8"/>
+      <c r="G34" s="30"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
-      <c r="K34" s="6" t="s">
+      <c r="K34" s="8"/>
+      <c r="L34" s="6" t="s">
         <v>833</v>
       </c>
-      <c r="L34" s="6"/>
-      <c r="M34" s="5"/>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M34" s="6"/>
+      <c r="N34" s="5"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
         <v>32</v>
       </c>
@@ -4199,15 +4262,16 @@
         <v>843</v>
       </c>
       <c r="F35" s="14"/>
-      <c r="G35" s="15"/>
+      <c r="G35" s="31"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
-      <c r="K35" s="16"/>
+      <c r="K35" s="15"/>
       <c r="L35" s="16"/>
-      <c r="M35" s="14"/>
-    </row>
-    <row r="36" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="M35" s="16"/>
+      <c r="N35" s="14"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>33</v>
       </c>
@@ -4224,15 +4288,16 @@
         <v>843</v>
       </c>
       <c r="F36" s="11"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="32"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
-      <c r="K36" s="13"/>
+      <c r="K36" s="12"/>
       <c r="L36" s="13"/>
-      <c r="M36" s="11"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M36" s="13"/>
+      <c r="N36" s="11"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -4249,15 +4314,16 @@
         <v>843</v>
       </c>
       <c r="F37" s="3"/>
-      <c r="G37" s="7"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
-      <c r="K37" s="4"/>
+      <c r="K37" s="7"/>
       <c r="L37" s="4"/>
-      <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M37" s="4"/>
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>35</v>
       </c>
@@ -4274,15 +4340,16 @@
         <v>843</v>
       </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="8"/>
+      <c r="G38" s="30"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="6"/>
+      <c r="K38" s="8"/>
       <c r="L38" s="6"/>
-      <c r="M38" s="5"/>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M38" s="6"/>
+      <c r="N38" s="5"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>36</v>
       </c>
@@ -4299,15 +4366,16 @@
         <v>844</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="7"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
-      <c r="K39" s="4"/>
+      <c r="K39" s="7"/>
       <c r="L39" s="4"/>
-      <c r="M39" s="3"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M39" s="4"/>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>37</v>
       </c>
@@ -4324,15 +4392,16 @@
         <v>844</v>
       </c>
       <c r="F40" s="5"/>
-      <c r="G40" s="8"/>
+      <c r="G40" s="30"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
-      <c r="K40" s="6"/>
+      <c r="K40" s="8"/>
       <c r="L40" s="6"/>
-      <c r="M40" s="5"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M40" s="6"/>
+      <c r="N40" s="5"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>38</v>
       </c>
@@ -4349,15 +4418,16 @@
         <v>844</v>
       </c>
       <c r="F41" s="3"/>
-      <c r="G41" s="7"/>
+      <c r="G41" s="27"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
-      <c r="K41" s="4"/>
+      <c r="K41" s="7"/>
       <c r="L41" s="4"/>
-      <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M41" s="4"/>
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>39</v>
       </c>
@@ -4374,15 +4444,16 @@
         <v>844</v>
       </c>
       <c r="F42" s="5"/>
-      <c r="G42" s="8"/>
+      <c r="G42" s="30"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
-      <c r="K42" s="6"/>
+      <c r="K42" s="8"/>
       <c r="L42" s="6"/>
-      <c r="M42" s="5"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M42" s="6"/>
+      <c r="N42" s="5"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>40</v>
       </c>
@@ -4399,15 +4470,16 @@
         <v>844</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="7"/>
+      <c r="G43" s="27"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
-      <c r="K43" s="4"/>
+      <c r="K43" s="7"/>
       <c r="L43" s="4"/>
-      <c r="M43" s="3"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M43" s="4"/>
+      <c r="N43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>41</v>
       </c>
@@ -4424,15 +4496,16 @@
         <v>844</v>
       </c>
       <c r="F44" s="5"/>
-      <c r="G44" s="8"/>
+      <c r="G44" s="30"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
-      <c r="K44" s="6"/>
+      <c r="K44" s="8"/>
       <c r="L44" s="6"/>
-      <c r="M44" s="5"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M44" s="6"/>
+      <c r="N44" s="5"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>42</v>
       </c>
@@ -4449,15 +4522,16 @@
         <v>844</v>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="7"/>
+      <c r="G45" s="27"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
-      <c r="K45" s="4"/>
+      <c r="K45" s="7"/>
       <c r="L45" s="4"/>
-      <c r="M45" s="3"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M45" s="4"/>
+      <c r="N45" s="3"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>43</v>
       </c>
@@ -4474,15 +4548,16 @@
         <v>844</v>
       </c>
       <c r="F46" s="5"/>
-      <c r="G46" s="8"/>
+      <c r="G46" s="30"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="6"/>
+      <c r="K46" s="8"/>
       <c r="L46" s="6"/>
-      <c r="M46" s="5"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M46" s="6"/>
+      <c r="N46" s="5"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>44</v>
       </c>
@@ -4499,15 +4574,16 @@
         <v>844</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="7"/>
+      <c r="G47" s="27"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
-      <c r="K47" s="4"/>
+      <c r="K47" s="7"/>
       <c r="L47" s="4"/>
-      <c r="M47" s="3"/>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M47" s="4"/>
+      <c r="N47" s="3"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>45</v>
       </c>
@@ -4524,15 +4600,16 @@
         <v>844</v>
       </c>
       <c r="F48" s="5"/>
-      <c r="G48" s="8"/>
+      <c r="G48" s="30"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="6"/>
+      <c r="K48" s="8"/>
       <c r="L48" s="6"/>
-      <c r="M48" s="5"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M48" s="6"/>
+      <c r="N48" s="5"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>46</v>
       </c>
@@ -4549,15 +4626,16 @@
         <v>844</v>
       </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="7"/>
+      <c r="G49" s="27"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
-      <c r="K49" s="4"/>
+      <c r="K49" s="7"/>
       <c r="L49" s="4"/>
-      <c r="M49" s="3"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M49" s="4"/>
+      <c r="N49" s="3"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>47</v>
       </c>
@@ -4574,15 +4652,16 @@
         <v>844</v>
       </c>
       <c r="F50" s="5"/>
-      <c r="G50" s="8"/>
+      <c r="G50" s="30"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
-      <c r="K50" s="6"/>
+      <c r="K50" s="8"/>
       <c r="L50" s="6"/>
-      <c r="M50" s="5"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M50" s="6"/>
+      <c r="N50" s="5"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>48</v>
       </c>
@@ -4599,15 +4678,16 @@
         <v>843</v>
       </c>
       <c r="F51" s="3"/>
-      <c r="G51" s="7"/>
+      <c r="G51" s="27"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
-      <c r="K51" s="4"/>
+      <c r="K51" s="7"/>
       <c r="L51" s="4"/>
-      <c r="M51" s="3"/>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M51" s="4"/>
+      <c r="N51" s="3"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>49</v>
       </c>
@@ -4624,15 +4704,16 @@
         <v>844</v>
       </c>
       <c r="F52" s="5"/>
-      <c r="G52" s="8"/>
+      <c r="G52" s="30"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
-      <c r="K52" s="6"/>
+      <c r="K52" s="8"/>
       <c r="L52" s="6"/>
-      <c r="M52" s="5"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M52" s="6"/>
+      <c r="N52" s="5"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>50</v>
       </c>
@@ -4649,15 +4730,16 @@
         <v>844</v>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="7"/>
+      <c r="G53" s="27"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
-      <c r="K53" s="4"/>
+      <c r="K53" s="7"/>
       <c r="L53" s="4"/>
-      <c r="M53" s="3"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M53" s="4"/>
+      <c r="N53" s="3"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>51</v>
       </c>
@@ -4674,15 +4756,16 @@
         <v>843</v>
       </c>
       <c r="F54" s="5"/>
-      <c r="G54" s="8"/>
+      <c r="G54" s="30"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
-      <c r="K54" s="6"/>
+      <c r="K54" s="8"/>
       <c r="L54" s="6"/>
-      <c r="M54" s="5"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M54" s="6"/>
+      <c r="N54" s="5"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>52</v>
       </c>
@@ -4699,15 +4782,16 @@
         <v>845</v>
       </c>
       <c r="F55" s="3"/>
-      <c r="G55" s="7"/>
+      <c r="G55" s="27"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
-      <c r="K55" s="4"/>
+      <c r="K55" s="7"/>
       <c r="L55" s="4"/>
-      <c r="M55" s="3"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M55" s="4"/>
+      <c r="N55" s="3"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>53</v>
       </c>
@@ -4724,15 +4808,16 @@
         <v>844</v>
       </c>
       <c r="F56" s="5"/>
-      <c r="G56" s="8"/>
+      <c r="G56" s="30"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
-      <c r="K56" s="6"/>
+      <c r="K56" s="8"/>
       <c r="L56" s="6"/>
-      <c r="M56" s="5"/>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M56" s="6"/>
+      <c r="N56" s="5"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>54</v>
       </c>
@@ -4749,15 +4834,16 @@
         <v>844</v>
       </c>
       <c r="F57" s="3"/>
-      <c r="G57" s="7"/>
+      <c r="G57" s="27"/>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
-      <c r="K57" s="4"/>
+      <c r="K57" s="7"/>
       <c r="L57" s="4"/>
-      <c r="M57" s="3"/>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M57" s="4"/>
+      <c r="N57" s="3"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>55</v>
       </c>
@@ -4774,15 +4860,16 @@
         <v>843</v>
       </c>
       <c r="F58" s="5"/>
-      <c r="G58" s="8"/>
+      <c r="G58" s="30"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
-      <c r="K58" s="6"/>
+      <c r="K58" s="8"/>
       <c r="L58" s="6"/>
-      <c r="M58" s="5"/>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M58" s="6"/>
+      <c r="N58" s="5"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>56</v>
       </c>
@@ -4799,15 +4886,16 @@
         <v>844</v>
       </c>
       <c r="F59" s="3"/>
-      <c r="G59" s="7"/>
+      <c r="G59" s="27"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
-      <c r="K59" s="4"/>
+      <c r="K59" s="7"/>
       <c r="L59" s="4"/>
-      <c r="M59" s="3"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M59" s="4"/>
+      <c r="N59" s="3"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>57</v>
       </c>
@@ -4824,15 +4912,16 @@
         <v>844</v>
       </c>
       <c r="F60" s="5"/>
-      <c r="G60" s="8"/>
+      <c r="G60" s="30"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
-      <c r="K60" s="6"/>
+      <c r="K60" s="8"/>
       <c r="L60" s="6"/>
-      <c r="M60" s="5"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M60" s="6"/>
+      <c r="N60" s="5"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>58</v>
       </c>
@@ -4849,15 +4938,16 @@
         <v>843</v>
       </c>
       <c r="F61" s="3"/>
-      <c r="G61" s="7"/>
+      <c r="G61" s="27"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
-      <c r="K61" s="4"/>
+      <c r="K61" s="7"/>
       <c r="L61" s="4"/>
-      <c r="M61" s="3"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M61" s="4"/>
+      <c r="N61" s="3"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>59</v>
       </c>
@@ -4874,15 +4964,16 @@
         <v>844</v>
       </c>
       <c r="F62" s="5"/>
-      <c r="G62" s="8"/>
+      <c r="G62" s="30"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
-      <c r="K62" s="6"/>
+      <c r="K62" s="8"/>
       <c r="L62" s="6"/>
-      <c r="M62" s="5"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M62" s="6"/>
+      <c r="N62" s="5"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>60</v>
       </c>
@@ -4899,15 +4990,16 @@
         <v>845</v>
       </c>
       <c r="F63" s="3"/>
-      <c r="G63" s="7"/>
+      <c r="G63" s="27"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
-      <c r="K63" s="4"/>
+      <c r="K63" s="7"/>
       <c r="L63" s="4"/>
-      <c r="M63" s="3"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M63" s="4"/>
+      <c r="N63" s="3"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>61</v>
       </c>
@@ -4924,15 +5016,16 @@
         <v>845</v>
       </c>
       <c r="F64" s="5"/>
-      <c r="G64" s="8"/>
+      <c r="G64" s="30"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
-      <c r="K64" s="6"/>
+      <c r="K64" s="8"/>
       <c r="L64" s="6"/>
-      <c r="M64" s="5"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M64" s="6"/>
+      <c r="N64" s="5"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>62</v>
       </c>
@@ -4949,15 +5042,16 @@
         <v>843</v>
       </c>
       <c r="F65" s="3"/>
-      <c r="G65" s="7"/>
+      <c r="G65" s="27"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
-      <c r="K65" s="4"/>
+      <c r="K65" s="7"/>
       <c r="L65" s="4"/>
-      <c r="M65" s="3"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M65" s="4"/>
+      <c r="N65" s="3"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>63</v>
       </c>
@@ -4974,15 +5068,16 @@
         <v>844</v>
       </c>
       <c r="F66" s="5"/>
-      <c r="G66" s="8"/>
+      <c r="G66" s="30"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
-      <c r="K66" s="6"/>
+      <c r="K66" s="8"/>
       <c r="L66" s="6"/>
-      <c r="M66" s="5"/>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M66" s="6"/>
+      <c r="N66" s="5"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -4999,15 +5094,16 @@
         <v>844</v>
       </c>
       <c r="F67" s="3"/>
-      <c r="G67" s="7"/>
+      <c r="G67" s="27"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
-      <c r="K67" s="4"/>
+      <c r="K67" s="7"/>
       <c r="L67" s="4"/>
-      <c r="M67" s="3"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M67" s="4"/>
+      <c r="N67" s="3"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>65</v>
       </c>
@@ -5024,15 +5120,16 @@
         <v>844</v>
       </c>
       <c r="F68" s="5"/>
-      <c r="G68" s="8"/>
+      <c r="G68" s="30"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
-      <c r="K68" s="6"/>
+      <c r="K68" s="8"/>
       <c r="L68" s="6"/>
-      <c r="M68" s="5"/>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M68" s="6"/>
+      <c r="N68" s="5"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>66</v>
       </c>
@@ -5049,15 +5146,16 @@
         <v>844</v>
       </c>
       <c r="F69" s="3"/>
-      <c r="G69" s="7"/>
+      <c r="G69" s="27"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
-      <c r="K69" s="4"/>
+      <c r="K69" s="7"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="3"/>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M69" s="4"/>
+      <c r="N69" s="3"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>67</v>
       </c>
@@ -5074,15 +5172,16 @@
         <v>844</v>
       </c>
       <c r="F70" s="5"/>
-      <c r="G70" s="8"/>
+      <c r="G70" s="30"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8"/>
-      <c r="K70" s="6"/>
+      <c r="K70" s="8"/>
       <c r="L70" s="6"/>
-      <c r="M70" s="5"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M70" s="6"/>
+      <c r="N70" s="5"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>68</v>
       </c>
@@ -5099,15 +5198,16 @@
         <v>844</v>
       </c>
       <c r="F71" s="3"/>
-      <c r="G71" s="7"/>
+      <c r="G71" s="27"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
-      <c r="K71" s="4"/>
+      <c r="K71" s="7"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="3"/>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M71" s="4"/>
+      <c r="N71" s="3"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>69</v>
       </c>
@@ -5124,15 +5224,16 @@
         <v>844</v>
       </c>
       <c r="F72" s="5"/>
-      <c r="G72" s="8"/>
+      <c r="G72" s="30"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
-      <c r="K72" s="6"/>
+      <c r="K72" s="8"/>
       <c r="L72" s="6"/>
-      <c r="M72" s="5"/>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M72" s="6"/>
+      <c r="N72" s="5"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>70</v>
       </c>
@@ -5149,15 +5250,16 @@
         <v>845</v>
       </c>
       <c r="F73" s="3"/>
-      <c r="G73" s="7"/>
+      <c r="G73" s="27"/>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
-      <c r="K73" s="4"/>
+      <c r="K73" s="7"/>
       <c r="L73" s="4"/>
-      <c r="M73" s="3"/>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M73" s="4"/>
+      <c r="N73" s="3"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>71</v>
       </c>
@@ -5174,15 +5276,16 @@
         <v>843</v>
       </c>
       <c r="F74" s="5"/>
-      <c r="G74" s="8"/>
+      <c r="G74" s="30"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
-      <c r="K74" s="6"/>
+      <c r="K74" s="8"/>
       <c r="L74" s="6"/>
-      <c r="M74" s="5"/>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M74" s="6"/>
+      <c r="N74" s="5"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>72</v>
       </c>
@@ -5199,15 +5302,16 @@
         <v>844</v>
       </c>
       <c r="F75" s="3"/>
-      <c r="G75" s="7"/>
+      <c r="G75" s="27"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
-      <c r="K75" s="4"/>
+      <c r="K75" s="7"/>
       <c r="L75" s="4"/>
-      <c r="M75" s="3"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M75" s="4"/>
+      <c r="N75" s="3"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>73</v>
       </c>
@@ -5224,15 +5328,16 @@
         <v>845</v>
       </c>
       <c r="F76" s="5"/>
-      <c r="G76" s="8"/>
+      <c r="G76" s="30"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
-      <c r="K76" s="6"/>
+      <c r="K76" s="8"/>
       <c r="L76" s="6"/>
-      <c r="M76" s="5"/>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M76" s="6"/>
+      <c r="N76" s="5"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>74</v>
       </c>
@@ -5249,15 +5354,16 @@
         <v>845</v>
       </c>
       <c r="F77" s="3"/>
-      <c r="G77" s="7"/>
+      <c r="G77" s="27"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
-      <c r="K77" s="4"/>
+      <c r="K77" s="7"/>
       <c r="L77" s="4"/>
-      <c r="M77" s="3"/>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M77" s="4"/>
+      <c r="N77" s="3"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>75</v>
       </c>
@@ -5274,15 +5380,16 @@
         <v>843</v>
       </c>
       <c r="F78" s="5"/>
-      <c r="G78" s="8"/>
+      <c r="G78" s="30"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
-      <c r="K78" s="6"/>
+      <c r="K78" s="8"/>
       <c r="L78" s="6"/>
-      <c r="M78" s="5"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M78" s="6"/>
+      <c r="N78" s="5"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>76</v>
       </c>
@@ -5299,15 +5406,16 @@
         <v>845</v>
       </c>
       <c r="F79" s="3"/>
-      <c r="G79" s="7"/>
+      <c r="G79" s="27"/>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
-      <c r="K79" s="4"/>
+      <c r="K79" s="7"/>
       <c r="L79" s="4"/>
-      <c r="M79" s="3"/>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M79" s="4"/>
+      <c r="N79" s="3"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>77</v>
       </c>
@@ -5324,15 +5432,16 @@
         <v>845</v>
       </c>
       <c r="F80" s="5"/>
-      <c r="G80" s="8"/>
+      <c r="G80" s="30"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
       <c r="J80" s="8"/>
-      <c r="K80" s="6"/>
+      <c r="K80" s="8"/>
       <c r="L80" s="6"/>
-      <c r="M80" s="5"/>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M80" s="6"/>
+      <c r="N80" s="5"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>78</v>
       </c>
@@ -5349,15 +5458,16 @@
         <v>844</v>
       </c>
       <c r="F81" s="3"/>
-      <c r="G81" s="7"/>
+      <c r="G81" s="27"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
-      <c r="K81" s="4"/>
+      <c r="K81" s="7"/>
       <c r="L81" s="4"/>
-      <c r="M81" s="3"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M81" s="4"/>
+      <c r="N81" s="3"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>79</v>
       </c>
@@ -5374,15 +5484,16 @@
         <v>844</v>
       </c>
       <c r="F82" s="5"/>
-      <c r="G82" s="8"/>
+      <c r="G82" s="30"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
-      <c r="K82" s="6"/>
+      <c r="K82" s="8"/>
       <c r="L82" s="6"/>
-      <c r="M82" s="5"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M82" s="6"/>
+      <c r="N82" s="5"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>80</v>
       </c>
@@ -5399,15 +5510,16 @@
         <v>843</v>
       </c>
       <c r="F83" s="3"/>
-      <c r="G83" s="7"/>
+      <c r="G83" s="27"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
-      <c r="K83" s="4"/>
+      <c r="K83" s="7"/>
       <c r="L83" s="4"/>
-      <c r="M83" s="3"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M83" s="4"/>
+      <c r="N83" s="3"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>81</v>
       </c>
@@ -5424,15 +5536,16 @@
         <v>844</v>
       </c>
       <c r="F84" s="5"/>
-      <c r="G84" s="8"/>
+      <c r="G84" s="30"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
-      <c r="K84" s="6"/>
+      <c r="K84" s="8"/>
       <c r="L84" s="6"/>
-      <c r="M84" s="5"/>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M84" s="6"/>
+      <c r="N84" s="5"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>82</v>
       </c>
@@ -5449,15 +5562,16 @@
         <v>843</v>
       </c>
       <c r="F85" s="3"/>
-      <c r="G85" s="7"/>
+      <c r="G85" s="27"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
-      <c r="K85" s="4"/>
+      <c r="K85" s="7"/>
       <c r="L85" s="4"/>
-      <c r="M85" s="3"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M85" s="4"/>
+      <c r="N85" s="3"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>83</v>
       </c>
@@ -5474,15 +5588,16 @@
         <v>843</v>
       </c>
       <c r="F86" s="5"/>
-      <c r="G86" s="8"/>
+      <c r="G86" s="30"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
-      <c r="K86" s="6"/>
+      <c r="K86" s="8"/>
       <c r="L86" s="6"/>
-      <c r="M86" s="5"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M86" s="6"/>
+      <c r="N86" s="5"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>84</v>
       </c>
@@ -5499,15 +5614,16 @@
         <v>843</v>
       </c>
       <c r="F87" s="3"/>
-      <c r="G87" s="7"/>
+      <c r="G87" s="27"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
-      <c r="K87" s="4"/>
+      <c r="K87" s="7"/>
       <c r="L87" s="4"/>
-      <c r="M87" s="3"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M87" s="4"/>
+      <c r="N87" s="3"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>85</v>
       </c>
@@ -5524,15 +5640,16 @@
         <v>844</v>
       </c>
       <c r="F88" s="5"/>
-      <c r="G88" s="8"/>
+      <c r="G88" s="30"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
-      <c r="K88" s="6"/>
+      <c r="K88" s="8"/>
       <c r="L88" s="6"/>
-      <c r="M88" s="5"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M88" s="6"/>
+      <c r="N88" s="5"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>86</v>
       </c>
@@ -5549,15 +5666,16 @@
         <v>844</v>
       </c>
       <c r="F89" s="3"/>
-      <c r="G89" s="7"/>
+      <c r="G89" s="27"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
-      <c r="K89" s="4"/>
+      <c r="K89" s="7"/>
       <c r="L89" s="4"/>
-      <c r="M89" s="3"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M89" s="4"/>
+      <c r="N89" s="3"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>87</v>
       </c>
@@ -5574,15 +5692,16 @@
         <v>845</v>
       </c>
       <c r="F90" s="5"/>
-      <c r="G90" s="8"/>
+      <c r="G90" s="30"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
-      <c r="K90" s="6"/>
+      <c r="K90" s="8"/>
       <c r="L90" s="6"/>
-      <c r="M90" s="5"/>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M90" s="6"/>
+      <c r="N90" s="5"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>88</v>
       </c>
@@ -5599,15 +5718,16 @@
         <v>844</v>
       </c>
       <c r="F91" s="3"/>
-      <c r="G91" s="7"/>
+      <c r="G91" s="27"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
-      <c r="K91" s="4"/>
+      <c r="K91" s="7"/>
       <c r="L91" s="4"/>
-      <c r="M91" s="3"/>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M91" s="4"/>
+      <c r="N91" s="3"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>89</v>
       </c>
@@ -5624,15 +5744,16 @@
         <v>844</v>
       </c>
       <c r="F92" s="5"/>
-      <c r="G92" s="8"/>
+      <c r="G92" s="30"/>
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
       <c r="J92" s="8"/>
-      <c r="K92" s="6"/>
+      <c r="K92" s="8"/>
       <c r="L92" s="6"/>
-      <c r="M92" s="5"/>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M92" s="6"/>
+      <c r="N92" s="5"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>90</v>
       </c>
@@ -5649,15 +5770,16 @@
         <v>844</v>
       </c>
       <c r="F93" s="3"/>
-      <c r="G93" s="7"/>
+      <c r="G93" s="27"/>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
-      <c r="K93" s="4"/>
+      <c r="K93" s="7"/>
       <c r="L93" s="4"/>
-      <c r="M93" s="3"/>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M93" s="4"/>
+      <c r="N93" s="3"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>91</v>
       </c>
@@ -5674,15 +5796,16 @@
         <v>845</v>
       </c>
       <c r="F94" s="5"/>
-      <c r="G94" s="8"/>
+      <c r="G94" s="30"/>
       <c r="H94" s="8"/>
       <c r="I94" s="8"/>
       <c r="J94" s="8"/>
-      <c r="K94" s="6"/>
+      <c r="K94" s="8"/>
       <c r="L94" s="6"/>
-      <c r="M94" s="5"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M94" s="6"/>
+      <c r="N94" s="5"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>92</v>
       </c>
@@ -5699,15 +5822,16 @@
         <v>844</v>
       </c>
       <c r="F95" s="3"/>
-      <c r="G95" s="7"/>
+      <c r="G95" s="27"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
-      <c r="K95" s="4"/>
+      <c r="K95" s="7"/>
       <c r="L95" s="4"/>
-      <c r="M95" s="3"/>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M95" s="4"/>
+      <c r="N95" s="3"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>93</v>
       </c>
@@ -5724,15 +5848,16 @@
         <v>844</v>
       </c>
       <c r="F96" s="5"/>
-      <c r="G96" s="8"/>
+      <c r="G96" s="30"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
       <c r="J96" s="8"/>
-      <c r="K96" s="6"/>
+      <c r="K96" s="8"/>
       <c r="L96" s="6"/>
-      <c r="M96" s="5"/>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M96" s="6"/>
+      <c r="N96" s="5"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>94</v>
       </c>
@@ -5749,15 +5874,16 @@
         <v>843</v>
       </c>
       <c r="F97" s="3"/>
-      <c r="G97" s="7"/>
+      <c r="G97" s="27"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
-      <c r="K97" s="4"/>
+      <c r="K97" s="7"/>
       <c r="L97" s="4"/>
-      <c r="M97" s="3"/>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M97" s="4"/>
+      <c r="N97" s="3"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>95</v>
       </c>
@@ -5774,15 +5900,16 @@
         <v>844</v>
       </c>
       <c r="F98" s="5"/>
-      <c r="G98" s="8"/>
+      <c r="G98" s="30"/>
       <c r="H98" s="8"/>
       <c r="I98" s="8"/>
       <c r="J98" s="8"/>
-      <c r="K98" s="6"/>
+      <c r="K98" s="8"/>
       <c r="L98" s="6"/>
-      <c r="M98" s="5"/>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M98" s="6"/>
+      <c r="N98" s="5"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>96</v>
       </c>
@@ -5799,15 +5926,16 @@
         <v>844</v>
       </c>
       <c r="F99" s="3"/>
-      <c r="G99" s="7"/>
+      <c r="G99" s="27"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
-      <c r="K99" s="4"/>
+      <c r="K99" s="7"/>
       <c r="L99" s="4"/>
-      <c r="M99" s="3"/>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M99" s="4"/>
+      <c r="N99" s="3"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>97</v>
       </c>
@@ -5824,15 +5952,16 @@
         <v>844</v>
       </c>
       <c r="F100" s="5"/>
-      <c r="G100" s="8"/>
+      <c r="G100" s="30"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8"/>
       <c r="J100" s="8"/>
-      <c r="K100" s="6"/>
+      <c r="K100" s="8"/>
       <c r="L100" s="6"/>
-      <c r="M100" s="5"/>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M100" s="6"/>
+      <c r="N100" s="5"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>98</v>
       </c>
@@ -5849,15 +5978,16 @@
         <v>843</v>
       </c>
       <c r="F101" s="3"/>
-      <c r="G101" s="7"/>
+      <c r="G101" s="27"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
-      <c r="K101" s="4"/>
+      <c r="K101" s="7"/>
       <c r="L101" s="4"/>
-      <c r="M101" s="3"/>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M101" s="4"/>
+      <c r="N101" s="3"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>99</v>
       </c>
@@ -5874,15 +6004,16 @@
         <v>843</v>
       </c>
       <c r="F102" s="5"/>
-      <c r="G102" s="8"/>
+      <c r="G102" s="30"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
       <c r="J102" s="8"/>
-      <c r="K102" s="6"/>
+      <c r="K102" s="8"/>
       <c r="L102" s="6"/>
-      <c r="M102" s="5"/>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M102" s="6"/>
+      <c r="N102" s="5"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>100</v>
       </c>
@@ -5899,15 +6030,16 @@
         <v>843</v>
       </c>
       <c r="F103" s="3"/>
-      <c r="G103" s="7"/>
+      <c r="G103" s="27"/>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
-      <c r="K103" s="4"/>
+      <c r="K103" s="7"/>
       <c r="L103" s="4"/>
-      <c r="M103" s="3"/>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M103" s="4"/>
+      <c r="N103" s="3"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>101</v>
       </c>
@@ -5924,15 +6056,16 @@
         <v>843</v>
       </c>
       <c r="F104" s="5"/>
-      <c r="G104" s="8"/>
+      <c r="G104" s="30"/>
       <c r="H104" s="8"/>
       <c r="I104" s="8"/>
       <c r="J104" s="8"/>
-      <c r="K104" s="6"/>
+      <c r="K104" s="8"/>
       <c r="L104" s="6"/>
-      <c r="M104" s="5"/>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M104" s="6"/>
+      <c r="N104" s="5"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>102</v>
       </c>
@@ -5949,15 +6082,16 @@
         <v>845</v>
       </c>
       <c r="F105" s="3"/>
-      <c r="G105" s="7"/>
+      <c r="G105" s="27"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
-      <c r="K105" s="4"/>
+      <c r="K105" s="7"/>
       <c r="L105" s="4"/>
-      <c r="M105" s="3"/>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M105" s="4"/>
+      <c r="N105" s="3"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>103</v>
       </c>
@@ -5974,15 +6108,16 @@
         <v>843</v>
       </c>
       <c r="F106" s="5"/>
-      <c r="G106" s="8"/>
+      <c r="G106" s="30"/>
       <c r="H106" s="8"/>
       <c r="I106" s="8"/>
       <c r="J106" s="8"/>
-      <c r="K106" s="6"/>
+      <c r="K106" s="8"/>
       <c r="L106" s="6"/>
-      <c r="M106" s="5"/>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M106" s="6"/>
+      <c r="N106" s="5"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>104</v>
       </c>
@@ -5999,15 +6134,16 @@
         <v>844</v>
       </c>
       <c r="F107" s="3"/>
-      <c r="G107" s="7"/>
+      <c r="G107" s="27"/>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
-      <c r="K107" s="4"/>
+      <c r="K107" s="7"/>
       <c r="L107" s="4"/>
-      <c r="M107" s="3"/>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M107" s="4"/>
+      <c r="N107" s="3"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>105</v>
       </c>
@@ -6024,15 +6160,16 @@
         <v>843</v>
       </c>
       <c r="F108" s="5"/>
-      <c r="G108" s="8"/>
+      <c r="G108" s="30"/>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
       <c r="J108" s="8"/>
-      <c r="K108" s="6"/>
+      <c r="K108" s="8"/>
       <c r="L108" s="6"/>
-      <c r="M108" s="5"/>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M108" s="6"/>
+      <c r="N108" s="5"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>106</v>
       </c>
@@ -6049,15 +6186,16 @@
         <v>844</v>
       </c>
       <c r="F109" s="3"/>
-      <c r="G109" s="7"/>
+      <c r="G109" s="27"/>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
-      <c r="K109" s="4"/>
+      <c r="K109" s="7"/>
       <c r="L109" s="4"/>
-      <c r="M109" s="3"/>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M109" s="4"/>
+      <c r="N109" s="3"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>107</v>
       </c>
@@ -6074,15 +6212,16 @@
         <v>844</v>
       </c>
       <c r="F110" s="5"/>
-      <c r="G110" s="8"/>
+      <c r="G110" s="30"/>
       <c r="H110" s="8"/>
       <c r="I110" s="8"/>
       <c r="J110" s="8"/>
-      <c r="K110" s="6"/>
+      <c r="K110" s="8"/>
       <c r="L110" s="6"/>
-      <c r="M110" s="5"/>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M110" s="6"/>
+      <c r="N110" s="5"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>108</v>
       </c>
@@ -6099,15 +6238,16 @@
         <v>844</v>
       </c>
       <c r="F111" s="3"/>
-      <c r="G111" s="7"/>
+      <c r="G111" s="27"/>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
-      <c r="K111" s="4"/>
+      <c r="K111" s="7"/>
       <c r="L111" s="4"/>
-      <c r="M111" s="3"/>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M111" s="4"/>
+      <c r="N111" s="3"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>109</v>
       </c>
@@ -6124,15 +6264,16 @@
         <v>844</v>
       </c>
       <c r="F112" s="5"/>
-      <c r="G112" s="8"/>
+      <c r="G112" s="30"/>
       <c r="H112" s="8"/>
       <c r="I112" s="8"/>
       <c r="J112" s="8"/>
-      <c r="K112" s="6"/>
+      <c r="K112" s="8"/>
       <c r="L112" s="6"/>
-      <c r="M112" s="5"/>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M112" s="6"/>
+      <c r="N112" s="5"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>110</v>
       </c>
@@ -6149,15 +6290,16 @@
         <v>844</v>
       </c>
       <c r="F113" s="3"/>
-      <c r="G113" s="7"/>
+      <c r="G113" s="27"/>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
-      <c r="K113" s="4"/>
+      <c r="K113" s="7"/>
       <c r="L113" s="4"/>
-      <c r="M113" s="3"/>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M113" s="4"/>
+      <c r="N113" s="3"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>111</v>
       </c>
@@ -6174,15 +6316,16 @@
         <v>844</v>
       </c>
       <c r="F114" s="5"/>
-      <c r="G114" s="8"/>
+      <c r="G114" s="30"/>
       <c r="H114" s="8"/>
       <c r="I114" s="8"/>
       <c r="J114" s="8"/>
-      <c r="K114" s="6"/>
+      <c r="K114" s="8"/>
       <c r="L114" s="6"/>
-      <c r="M114" s="5"/>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M114" s="6"/>
+      <c r="N114" s="5"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>112</v>
       </c>
@@ -6199,15 +6342,16 @@
         <v>844</v>
       </c>
       <c r="F115" s="3"/>
-      <c r="G115" s="7"/>
+      <c r="G115" s="27"/>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
-      <c r="K115" s="4"/>
+      <c r="K115" s="7"/>
       <c r="L115" s="4"/>
-      <c r="M115" s="3"/>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M115" s="4"/>
+      <c r="N115" s="3"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>113</v>
       </c>
@@ -6224,15 +6368,16 @@
         <v>844</v>
       </c>
       <c r="F116" s="5"/>
-      <c r="G116" s="8"/>
+      <c r="G116" s="30"/>
       <c r="H116" s="8"/>
       <c r="I116" s="8"/>
       <c r="J116" s="8"/>
-      <c r="K116" s="6"/>
+      <c r="K116" s="8"/>
       <c r="L116" s="6"/>
-      <c r="M116" s="5"/>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M116" s="6"/>
+      <c r="N116" s="5"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>114</v>
       </c>
@@ -6249,15 +6394,16 @@
         <v>844</v>
       </c>
       <c r="F117" s="3"/>
-      <c r="G117" s="7"/>
+      <c r="G117" s="27"/>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
-      <c r="K117" s="4"/>
+      <c r="K117" s="7"/>
       <c r="L117" s="4"/>
-      <c r="M117" s="3"/>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M117" s="4"/>
+      <c r="N117" s="3"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="5">
         <v>115</v>
       </c>
@@ -6274,15 +6420,16 @@
         <v>844</v>
       </c>
       <c r="F118" s="5"/>
-      <c r="G118" s="8"/>
+      <c r="G118" s="30"/>
       <c r="H118" s="8"/>
       <c r="I118" s="8"/>
       <c r="J118" s="8"/>
-      <c r="K118" s="6"/>
+      <c r="K118" s="8"/>
       <c r="L118" s="6"/>
-      <c r="M118" s="5"/>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M118" s="6"/>
+      <c r="N118" s="5"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>116</v>
       </c>
@@ -6299,15 +6446,16 @@
         <v>844</v>
       </c>
       <c r="F119" s="3"/>
-      <c r="G119" s="7"/>
+      <c r="G119" s="27"/>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
-      <c r="K119" s="4"/>
+      <c r="K119" s="7"/>
       <c r="L119" s="4"/>
-      <c r="M119" s="3"/>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M119" s="4"/>
+      <c r="N119" s="3"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="5">
         <v>117</v>
       </c>
@@ -6324,15 +6472,16 @@
         <v>844</v>
       </c>
       <c r="F120" s="5"/>
-      <c r="G120" s="8"/>
+      <c r="G120" s="30"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
-      <c r="K120" s="6"/>
+      <c r="K120" s="8"/>
       <c r="L120" s="6"/>
-      <c r="M120" s="5"/>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M120" s="6"/>
+      <c r="N120" s="5"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>118</v>
       </c>
@@ -6349,15 +6498,16 @@
         <v>844</v>
       </c>
       <c r="F121" s="3"/>
-      <c r="G121" s="7"/>
+      <c r="G121" s="27"/>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
-      <c r="K121" s="4"/>
+      <c r="K121" s="7"/>
       <c r="L121" s="4"/>
-      <c r="M121" s="3"/>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M121" s="4"/>
+      <c r="N121" s="3"/>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>119</v>
       </c>
@@ -6374,15 +6524,16 @@
         <v>844</v>
       </c>
       <c r="F122" s="5"/>
-      <c r="G122" s="8"/>
+      <c r="G122" s="30"/>
       <c r="H122" s="8"/>
       <c r="I122" s="8"/>
       <c r="J122" s="8"/>
-      <c r="K122" s="6"/>
+      <c r="K122" s="8"/>
       <c r="L122" s="6"/>
-      <c r="M122" s="5"/>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M122" s="6"/>
+      <c r="N122" s="5"/>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>120</v>
       </c>
@@ -6399,15 +6550,16 @@
         <v>844</v>
       </c>
       <c r="F123" s="3"/>
-      <c r="G123" s="7"/>
+      <c r="G123" s="27"/>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
-      <c r="K123" s="4"/>
+      <c r="K123" s="7"/>
       <c r="L123" s="4"/>
-      <c r="M123" s="3"/>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M123" s="4"/>
+      <c r="N123" s="3"/>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>121</v>
       </c>
@@ -6424,15 +6576,16 @@
         <v>844</v>
       </c>
       <c r="F124" s="5"/>
-      <c r="G124" s="8"/>
+      <c r="G124" s="30"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
-      <c r="K124" s="6"/>
+      <c r="K124" s="8"/>
       <c r="L124" s="6"/>
-      <c r="M124" s="5"/>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M124" s="6"/>
+      <c r="N124" s="5"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>122</v>
       </c>
@@ -6449,15 +6602,16 @@
         <v>844</v>
       </c>
       <c r="F125" s="3"/>
-      <c r="G125" s="7"/>
+      <c r="G125" s="27"/>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
-      <c r="K125" s="4"/>
+      <c r="K125" s="7"/>
       <c r="L125" s="4"/>
-      <c r="M125" s="3"/>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M125" s="4"/>
+      <c r="N125" s="3"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>123</v>
       </c>
@@ -6474,15 +6628,16 @@
         <v>844</v>
       </c>
       <c r="F126" s="5"/>
-      <c r="G126" s="8"/>
+      <c r="G126" s="30"/>
       <c r="H126" s="8"/>
       <c r="I126" s="8"/>
       <c r="J126" s="8"/>
-      <c r="K126" s="6"/>
+      <c r="K126" s="8"/>
       <c r="L126" s="6"/>
-      <c r="M126" s="5"/>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M126" s="6"/>
+      <c r="N126" s="5"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>124</v>
       </c>
@@ -6499,15 +6654,16 @@
         <v>844</v>
       </c>
       <c r="F127" s="3"/>
-      <c r="G127" s="7"/>
+      <c r="G127" s="27"/>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
-      <c r="K127" s="4"/>
+      <c r="K127" s="7"/>
       <c r="L127" s="4"/>
-      <c r="M127" s="3"/>
-    </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M127" s="4"/>
+      <c r="N127" s="3"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="5">
         <v>125</v>
       </c>
@@ -6524,15 +6680,16 @@
         <v>844</v>
       </c>
       <c r="F128" s="5"/>
-      <c r="G128" s="8"/>
+      <c r="G128" s="30"/>
       <c r="H128" s="8"/>
       <c r="I128" s="8"/>
       <c r="J128" s="8"/>
-      <c r="K128" s="6"/>
+      <c r="K128" s="8"/>
       <c r="L128" s="6"/>
-      <c r="M128" s="5"/>
-    </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M128" s="6"/>
+      <c r="N128" s="5"/>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>126</v>
       </c>
@@ -6549,15 +6706,16 @@
         <v>844</v>
       </c>
       <c r="F129" s="3"/>
-      <c r="G129" s="7"/>
+      <c r="G129" s="27"/>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
-      <c r="K129" s="4"/>
+      <c r="K129" s="7"/>
       <c r="L129" s="4"/>
-      <c r="M129" s="3"/>
-    </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M129" s="4"/>
+      <c r="N129" s="3"/>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="5">
         <v>127</v>
       </c>
@@ -6574,15 +6732,16 @@
         <v>843</v>
       </c>
       <c r="F130" s="5"/>
-      <c r="G130" s="8"/>
+      <c r="G130" s="30"/>
       <c r="H130" s="8"/>
       <c r="I130" s="8"/>
       <c r="J130" s="8"/>
-      <c r="K130" s="6"/>
+      <c r="K130" s="8"/>
       <c r="L130" s="6"/>
-      <c r="M130" s="5"/>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M130" s="6"/>
+      <c r="N130" s="5"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>128</v>
       </c>
@@ -6599,15 +6758,16 @@
         <v>844</v>
       </c>
       <c r="F131" s="3"/>
-      <c r="G131" s="7"/>
+      <c r="G131" s="27"/>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
-      <c r="K131" s="4"/>
+      <c r="K131" s="7"/>
       <c r="L131" s="4"/>
-      <c r="M131" s="3"/>
-    </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M131" s="4"/>
+      <c r="N131" s="3"/>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>129</v>
       </c>
@@ -6624,15 +6784,16 @@
         <v>844</v>
       </c>
       <c r="F132" s="5"/>
-      <c r="G132" s="8"/>
+      <c r="G132" s="30"/>
       <c r="H132" s="8"/>
       <c r="I132" s="8"/>
       <c r="J132" s="8"/>
-      <c r="K132" s="6"/>
+      <c r="K132" s="8"/>
       <c r="L132" s="6"/>
-      <c r="M132" s="5"/>
-    </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M132" s="6"/>
+      <c r="N132" s="5"/>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>130</v>
       </c>
@@ -6649,15 +6810,16 @@
         <v>844</v>
       </c>
       <c r="F133" s="3"/>
-      <c r="G133" s="7"/>
+      <c r="G133" s="27"/>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
-      <c r="K133" s="4"/>
+      <c r="K133" s="7"/>
       <c r="L133" s="4"/>
-      <c r="M133" s="3"/>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M133" s="4"/>
+      <c r="N133" s="3"/>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="5">
         <v>131</v>
       </c>
@@ -6674,15 +6836,16 @@
         <v>843</v>
       </c>
       <c r="F134" s="5"/>
-      <c r="G134" s="8"/>
+      <c r="G134" s="30"/>
       <c r="H134" s="8"/>
       <c r="I134" s="8"/>
       <c r="J134" s="8"/>
-      <c r="K134" s="6"/>
+      <c r="K134" s="8"/>
       <c r="L134" s="6"/>
-      <c r="M134" s="5"/>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M134" s="6"/>
+      <c r="N134" s="5"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>132</v>
       </c>
@@ -6699,15 +6862,16 @@
         <v>843</v>
       </c>
       <c r="F135" s="3"/>
-      <c r="G135" s="7"/>
+      <c r="G135" s="27"/>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
-      <c r="K135" s="4"/>
+      <c r="K135" s="7"/>
       <c r="L135" s="4"/>
-      <c r="M135" s="3"/>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M135" s="4"/>
+      <c r="N135" s="3"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="5">
         <v>133</v>
       </c>
@@ -6724,15 +6888,16 @@
         <v>844</v>
       </c>
       <c r="F136" s="5"/>
-      <c r="G136" s="8"/>
+      <c r="G136" s="30"/>
       <c r="H136" s="8"/>
       <c r="I136" s="8"/>
       <c r="J136" s="8"/>
-      <c r="K136" s="6"/>
+      <c r="K136" s="8"/>
       <c r="L136" s="6"/>
-      <c r="M136" s="5"/>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M136" s="6"/>
+      <c r="N136" s="5"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>134</v>
       </c>
@@ -6749,15 +6914,16 @@
         <v>844</v>
       </c>
       <c r="F137" s="3"/>
-      <c r="G137" s="7"/>
+      <c r="G137" s="27"/>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
-      <c r="K137" s="4"/>
+      <c r="K137" s="7"/>
       <c r="L137" s="4"/>
-      <c r="M137" s="3"/>
-    </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M137" s="4"/>
+      <c r="N137" s="3"/>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="5">
         <v>135</v>
       </c>
@@ -6774,15 +6940,16 @@
         <v>844</v>
       </c>
       <c r="F138" s="5"/>
-      <c r="G138" s="8"/>
+      <c r="G138" s="30"/>
       <c r="H138" s="8"/>
       <c r="I138" s="8"/>
       <c r="J138" s="8"/>
-      <c r="K138" s="6"/>
+      <c r="K138" s="8"/>
       <c r="L138" s="6"/>
-      <c r="M138" s="5"/>
-    </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M138" s="6"/>
+      <c r="N138" s="5"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>136</v>
       </c>
@@ -6799,15 +6966,16 @@
         <v>845</v>
       </c>
       <c r="F139" s="3"/>
-      <c r="G139" s="7"/>
+      <c r="G139" s="27"/>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
-      <c r="K139" s="4"/>
+      <c r="K139" s="7"/>
       <c r="L139" s="4"/>
-      <c r="M139" s="3"/>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M139" s="4"/>
+      <c r="N139" s="3"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="5">
         <v>137</v>
       </c>
@@ -6824,15 +6992,16 @@
         <v>844</v>
       </c>
       <c r="F140" s="5"/>
-      <c r="G140" s="8"/>
+      <c r="G140" s="30"/>
       <c r="H140" s="8"/>
       <c r="I140" s="8"/>
       <c r="J140" s="8"/>
-      <c r="K140" s="6"/>
+      <c r="K140" s="8"/>
       <c r="L140" s="6"/>
-      <c r="M140" s="5"/>
-    </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M140" s="6"/>
+      <c r="N140" s="5"/>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>138</v>
       </c>
@@ -6849,15 +7018,16 @@
         <v>844</v>
       </c>
       <c r="F141" s="3"/>
-      <c r="G141" s="7"/>
+      <c r="G141" s="27"/>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
-      <c r="K141" s="4"/>
+      <c r="K141" s="7"/>
       <c r="L141" s="4"/>
-      <c r="M141" s="3"/>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M141" s="4"/>
+      <c r="N141" s="3"/>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="5">
         <v>139</v>
       </c>
@@ -6874,15 +7044,16 @@
         <v>844</v>
       </c>
       <c r="F142" s="5"/>
-      <c r="G142" s="8"/>
+      <c r="G142" s="30"/>
       <c r="H142" s="8"/>
       <c r="I142" s="8"/>
       <c r="J142" s="8"/>
-      <c r="K142" s="6"/>
+      <c r="K142" s="8"/>
       <c r="L142" s="6"/>
-      <c r="M142" s="5"/>
-    </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M142" s="6"/>
+      <c r="N142" s="5"/>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>140</v>
       </c>
@@ -6899,15 +7070,16 @@
         <v>844</v>
       </c>
       <c r="F143" s="3"/>
-      <c r="G143" s="7"/>
+      <c r="G143" s="27"/>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
-      <c r="K143" s="4"/>
+      <c r="K143" s="7"/>
       <c r="L143" s="4"/>
-      <c r="M143" s="3"/>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M143" s="4"/>
+      <c r="N143" s="3"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>141</v>
       </c>
@@ -6924,15 +7096,16 @@
         <v>845</v>
       </c>
       <c r="F144" s="5"/>
-      <c r="G144" s="8"/>
+      <c r="G144" s="30"/>
       <c r="H144" s="8"/>
       <c r="I144" s="8"/>
       <c r="J144" s="8"/>
-      <c r="K144" s="6"/>
+      <c r="K144" s="8"/>
       <c r="L144" s="6"/>
-      <c r="M144" s="5"/>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M144" s="6"/>
+      <c r="N144" s="5"/>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>142</v>
       </c>
@@ -6949,15 +7122,16 @@
         <v>844</v>
       </c>
       <c r="F145" s="3"/>
-      <c r="G145" s="7"/>
+      <c r="G145" s="27"/>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
-      <c r="K145" s="4"/>
+      <c r="K145" s="7"/>
       <c r="L145" s="4"/>
-      <c r="M145" s="3"/>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M145" s="4"/>
+      <c r="N145" s="3"/>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>143</v>
       </c>
@@ -6974,15 +7148,16 @@
         <v>844</v>
       </c>
       <c r="F146" s="5"/>
-      <c r="G146" s="8"/>
+      <c r="G146" s="30"/>
       <c r="H146" s="8"/>
       <c r="I146" s="8"/>
       <c r="J146" s="8"/>
-      <c r="K146" s="6"/>
+      <c r="K146" s="8"/>
       <c r="L146" s="6"/>
-      <c r="M146" s="5"/>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M146" s="6"/>
+      <c r="N146" s="5"/>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>144</v>
       </c>
@@ -6999,15 +7174,16 @@
         <v>844</v>
       </c>
       <c r="F147" s="3"/>
-      <c r="G147" s="7"/>
+      <c r="G147" s="27"/>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
-      <c r="K147" s="4"/>
+      <c r="K147" s="7"/>
       <c r="L147" s="4"/>
-      <c r="M147" s="3"/>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M147" s="4"/>
+      <c r="N147" s="3"/>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="5">
         <v>145</v>
       </c>
@@ -7024,15 +7200,16 @@
         <v>843</v>
       </c>
       <c r="F148" s="5"/>
-      <c r="G148" s="8"/>
+      <c r="G148" s="30"/>
       <c r="H148" s="8"/>
       <c r="I148" s="8"/>
       <c r="J148" s="8"/>
-      <c r="K148" s="6"/>
+      <c r="K148" s="8"/>
       <c r="L148" s="6"/>
-      <c r="M148" s="5"/>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M148" s="6"/>
+      <c r="N148" s="5"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>146</v>
       </c>
@@ -7049,15 +7226,16 @@
         <v>844</v>
       </c>
       <c r="F149" s="3"/>
-      <c r="G149" s="7"/>
+      <c r="G149" s="27"/>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
-      <c r="K149" s="4"/>
+      <c r="K149" s="7"/>
       <c r="L149" s="4"/>
-      <c r="M149" s="3"/>
-    </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M149" s="4"/>
+      <c r="N149" s="3"/>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="5">
         <v>147</v>
       </c>
@@ -7074,15 +7252,16 @@
         <v>844</v>
       </c>
       <c r="F150" s="5"/>
-      <c r="G150" s="8"/>
+      <c r="G150" s="30"/>
       <c r="H150" s="8"/>
       <c r="I150" s="8"/>
       <c r="J150" s="8"/>
-      <c r="K150" s="6"/>
+      <c r="K150" s="8"/>
       <c r="L150" s="6"/>
-      <c r="M150" s="5"/>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M150" s="6"/>
+      <c r="N150" s="5"/>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>148</v>
       </c>
@@ -7099,15 +7278,16 @@
         <v>843</v>
       </c>
       <c r="F151" s="3"/>
-      <c r="G151" s="7"/>
+      <c r="G151" s="27"/>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
-      <c r="K151" s="4"/>
+      <c r="K151" s="7"/>
       <c r="L151" s="4"/>
-      <c r="M151" s="3"/>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M151" s="4"/>
+      <c r="N151" s="3"/>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>149</v>
       </c>
@@ -7124,15 +7304,16 @@
         <v>844</v>
       </c>
       <c r="F152" s="5"/>
-      <c r="G152" s="8"/>
+      <c r="G152" s="30"/>
       <c r="H152" s="8"/>
       <c r="I152" s="8"/>
       <c r="J152" s="8"/>
-      <c r="K152" s="6"/>
+      <c r="K152" s="8"/>
       <c r="L152" s="6"/>
-      <c r="M152" s="5"/>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M152" s="6"/>
+      <c r="N152" s="5"/>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>150</v>
       </c>
@@ -7149,15 +7330,16 @@
         <v>843</v>
       </c>
       <c r="F153" s="3"/>
-      <c r="G153" s="7"/>
+      <c r="G153" s="27"/>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
-      <c r="K153" s="4"/>
+      <c r="K153" s="7"/>
       <c r="L153" s="4"/>
-      <c r="M153" s="3"/>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M153" s="4"/>
+      <c r="N153" s="3"/>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>151</v>
       </c>
@@ -7174,15 +7356,16 @@
         <v>844</v>
       </c>
       <c r="F154" s="5"/>
-      <c r="G154" s="8"/>
+      <c r="G154" s="30"/>
       <c r="H154" s="8"/>
       <c r="I154" s="8"/>
       <c r="J154" s="8"/>
-      <c r="K154" s="6"/>
+      <c r="K154" s="8"/>
       <c r="L154" s="6"/>
-      <c r="M154" s="5"/>
-    </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M154" s="6"/>
+      <c r="N154" s="5"/>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>152</v>
       </c>
@@ -7199,15 +7382,16 @@
         <v>845</v>
       </c>
       <c r="F155" s="3"/>
-      <c r="G155" s="7"/>
+      <c r="G155" s="27"/>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
-      <c r="K155" s="4"/>
+      <c r="K155" s="7"/>
       <c r="L155" s="4"/>
-      <c r="M155" s="3"/>
-    </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M155" s="4"/>
+      <c r="N155" s="3"/>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>153</v>
       </c>
@@ -7224,15 +7408,16 @@
         <v>844</v>
       </c>
       <c r="F156" s="5"/>
-      <c r="G156" s="8"/>
+      <c r="G156" s="30"/>
       <c r="H156" s="8"/>
       <c r="I156" s="8"/>
       <c r="J156" s="8"/>
-      <c r="K156" s="6"/>
+      <c r="K156" s="8"/>
       <c r="L156" s="6"/>
-      <c r="M156" s="5"/>
-    </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M156" s="6"/>
+      <c r="N156" s="5"/>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>154</v>
       </c>
@@ -7249,15 +7434,16 @@
         <v>844</v>
       </c>
       <c r="F157" s="3"/>
-      <c r="G157" s="7"/>
+      <c r="G157" s="27"/>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
-      <c r="K157" s="4"/>
+      <c r="K157" s="7"/>
       <c r="L157" s="4"/>
-      <c r="M157" s="3"/>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M157" s="4"/>
+      <c r="N157" s="3"/>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" s="5">
         <v>155</v>
       </c>
@@ -7274,34 +7460,36 @@
         <v>844</v>
       </c>
       <c r="F158" s="5"/>
-      <c r="G158" s="8"/>
+      <c r="G158" s="30"/>
       <c r="H158" s="8"/>
       <c r="I158" s="8"/>
       <c r="J158" s="8"/>
-      <c r="K158" s="6"/>
+      <c r="K158" s="8"/>
       <c r="L158" s="6"/>
-      <c r="M158" s="5"/>
+      <c r="M158" s="6"/>
+      <c r="N158" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:M2" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:M158">
+  <autoFilter ref="A2:N2" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N158">
+    <sortCondition ref="I4:I158"/>
     <sortCondition ref="H4:H158"/>
-    <sortCondition ref="G4:G158"/>
     <sortCondition ref="A4:A158"/>
     <sortCondition ref="C4:C158"/>
     <sortCondition ref="B4:B158"/>
   </sortState>
-  <mergeCells count="10">
-    <mergeCell ref="M1:M2"/>
+  <mergeCells count="11">
+    <mergeCell ref="N1:N2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrega el módulo en el que me encuentra trabajando.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D867C0B9-F072-4C25-B325-92AC360A2991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E7C0AE-7301-426B-8B6C-FF031E06875E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4141" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4143" uniqueCount="852">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2697,6 +2697,12 @@
   </si>
   <si>
     <t>Fecha de inicio</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/05/2025: Se emepiza con el analsisi del módulo y su desarrollo </t>
   </si>
 </sst>
 </file>
@@ -2872,6 +2878,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2899,26 +2920,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3253,7 +3259,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,7 +3269,7 @@
     <col min="3" max="3" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="15" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
@@ -3274,51 +3280,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="24" t="s">
         <v>814</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="30" t="s">
         <v>840</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="30" t="s">
         <v>841</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="32" t="s">
         <v>849</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="26" t="s">
         <v>704</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="19" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="24" t="s">
         <v>716</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="28" t="s">
         <v>837</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="23" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="29"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="9" t="s">
         <v>705</v>
       </c>
@@ -3331,9 +3337,9 @@
       <c r="K2" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="18"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -3354,7 +3360,7 @@
       <c r="F3" s="17" t="s">
         <v>842</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="7" t="s">
         <v>711</v>
       </c>
@@ -3388,7 +3394,7 @@
         <v>843</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="30"/>
+      <c r="G4" s="19"/>
       <c r="H4" s="8" t="s">
         <v>711</v>
       </c>
@@ -3422,7 +3428,7 @@
         <v>843</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="27"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="7" t="s">
         <v>711</v>
       </c>
@@ -3456,7 +3462,7 @@
         <v>843</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="30"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="8" t="s">
         <v>711</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>843</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="27"/>
+      <c r="G7" s="18"/>
       <c r="H7" s="7" t="s">
         <v>711</v>
       </c>
@@ -3524,7 +3530,7 @@
         <v>844</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="30"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="8" t="s">
         <v>711</v>
       </c>
@@ -3558,7 +3564,7 @@
         <v>844</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="27"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="7" t="s">
         <v>711</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>844</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="30"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="8" t="s">
         <v>711</v>
       </c>
@@ -3626,7 +3632,7 @@
         <v>843</v>
       </c>
       <c r="F11" s="3"/>
-      <c r="G11" s="27"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -3652,7 +3658,7 @@
         <v>843</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="30"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -3678,14 +3684,20 @@
         <v>843</v>
       </c>
       <c r="F13" s="3"/>
-      <c r="G13" s="27"/>
+      <c r="G13" s="18">
+        <v>45783</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
-      <c r="L13" s="4"/>
+      <c r="L13" s="4" t="s">
+        <v>850</v>
+      </c>
       <c r="M13" s="4"/>
-      <c r="N13" s="3"/>
+      <c r="N13" s="3" t="s">
+        <v>851</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -3704,7 +3716,7 @@
         <v>843</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="30"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -3732,7 +3744,7 @@
         <v>844</v>
       </c>
       <c r="F15" s="3"/>
-      <c r="G15" s="27"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -3758,7 +3770,7 @@
         <v>844</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="30"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -3784,7 +3796,7 @@
         <v>844</v>
       </c>
       <c r="F17" s="3"/>
-      <c r="G17" s="27"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -3810,7 +3822,7 @@
         <v>844</v>
       </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="30"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -3836,7 +3848,7 @@
         <v>844</v>
       </c>
       <c r="F19" s="3"/>
-      <c r="G19" s="27"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -3862,7 +3874,7 @@
         <v>844</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" s="30"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -3888,7 +3900,7 @@
         <v>843</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="27"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -3914,7 +3926,7 @@
         <v>843</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="30"/>
+      <c r="G22" s="19"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -3940,7 +3952,7 @@
         <v>843</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="27"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -3966,7 +3978,7 @@
         <v>843</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="30"/>
+      <c r="G24" s="19"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -3992,7 +4004,7 @@
         <v>844</v>
       </c>
       <c r="F25" s="3"/>
-      <c r="G25" s="27">
+      <c r="G25" s="18">
         <v>45785</v>
       </c>
       <c r="H25" s="7"/>
@@ -4024,7 +4036,7 @@
         <v>845</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="30"/>
+      <c r="G26" s="19"/>
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -4050,7 +4062,7 @@
         <v>845</v>
       </c>
       <c r="F27" s="3"/>
-      <c r="G27" s="27"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
@@ -4076,7 +4088,7 @@
         <v>844</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="30"/>
+      <c r="G28" s="19"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -4102,7 +4114,7 @@
         <v>843</v>
       </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="27"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -4128,7 +4140,7 @@
         <v>843</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" s="30"/>
+      <c r="G30" s="19"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
@@ -4154,7 +4166,7 @@
         <v>845</v>
       </c>
       <c r="F31" s="3"/>
-      <c r="G31" s="27"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -4182,7 +4194,7 @@
         <v>845</v>
       </c>
       <c r="F32" s="5"/>
-      <c r="G32" s="30"/>
+      <c r="G32" s="19"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
@@ -4208,7 +4220,7 @@
         <v>844</v>
       </c>
       <c r="F33" s="3"/>
-      <c r="G33" s="27"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -4234,7 +4246,7 @@
         <v>845</v>
       </c>
       <c r="F34" s="5"/>
-      <c r="G34" s="30"/>
+      <c r="G34" s="19"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -4262,7 +4274,7 @@
         <v>843</v>
       </c>
       <c r="F35" s="14"/>
-      <c r="G35" s="31"/>
+      <c r="G35" s="20"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -4288,7 +4300,7 @@
         <v>843</v>
       </c>
       <c r="F36" s="11"/>
-      <c r="G36" s="32"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -4314,7 +4326,7 @@
         <v>843</v>
       </c>
       <c r="F37" s="3"/>
-      <c r="G37" s="27"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
@@ -4340,7 +4352,7 @@
         <v>843</v>
       </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="30"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -4366,7 +4378,7 @@
         <v>844</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" s="27"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
@@ -4392,7 +4404,7 @@
         <v>844</v>
       </c>
       <c r="F40" s="5"/>
-      <c r="G40" s="30"/>
+      <c r="G40" s="19"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
@@ -4418,7 +4430,7 @@
         <v>844</v>
       </c>
       <c r="F41" s="3"/>
-      <c r="G41" s="27"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
@@ -4444,7 +4456,7 @@
         <v>844</v>
       </c>
       <c r="F42" s="5"/>
-      <c r="G42" s="30"/>
+      <c r="G42" s="19"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -4470,7 +4482,7 @@
         <v>844</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="27"/>
+      <c r="G43" s="18"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
@@ -4496,7 +4508,7 @@
         <v>844</v>
       </c>
       <c r="F44" s="5"/>
-      <c r="G44" s="30"/>
+      <c r="G44" s="19"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -4522,7 +4534,7 @@
         <v>844</v>
       </c>
       <c r="F45" s="3"/>
-      <c r="G45" s="27"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
@@ -4548,7 +4560,7 @@
         <v>844</v>
       </c>
       <c r="F46" s="5"/>
-      <c r="G46" s="30"/>
+      <c r="G46" s="19"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
@@ -4574,7 +4586,7 @@
         <v>844</v>
       </c>
       <c r="F47" s="3"/>
-      <c r="G47" s="27"/>
+      <c r="G47" s="18"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
@@ -4600,7 +4612,7 @@
         <v>844</v>
       </c>
       <c r="F48" s="5"/>
-      <c r="G48" s="30"/>
+      <c r="G48" s="19"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
@@ -4626,7 +4638,7 @@
         <v>844</v>
       </c>
       <c r="F49" s="3"/>
-      <c r="G49" s="27"/>
+      <c r="G49" s="18"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
@@ -4652,7 +4664,7 @@
         <v>844</v>
       </c>
       <c r="F50" s="5"/>
-      <c r="G50" s="30"/>
+      <c r="G50" s="19"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
@@ -4678,7 +4690,7 @@
         <v>843</v>
       </c>
       <c r="F51" s="3"/>
-      <c r="G51" s="27"/>
+      <c r="G51" s="18"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
@@ -4704,7 +4716,7 @@
         <v>844</v>
       </c>
       <c r="F52" s="5"/>
-      <c r="G52" s="30"/>
+      <c r="G52" s="19"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
@@ -4730,7 +4742,7 @@
         <v>844</v>
       </c>
       <c r="F53" s="3"/>
-      <c r="G53" s="27"/>
+      <c r="G53" s="18"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
@@ -4756,7 +4768,7 @@
         <v>843</v>
       </c>
       <c r="F54" s="5"/>
-      <c r="G54" s="30"/>
+      <c r="G54" s="19"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
@@ -4782,7 +4794,7 @@
         <v>845</v>
       </c>
       <c r="F55" s="3"/>
-      <c r="G55" s="27"/>
+      <c r="G55" s="18"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
@@ -4808,7 +4820,7 @@
         <v>844</v>
       </c>
       <c r="F56" s="5"/>
-      <c r="G56" s="30"/>
+      <c r="G56" s="19"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
@@ -4834,7 +4846,7 @@
         <v>844</v>
       </c>
       <c r="F57" s="3"/>
-      <c r="G57" s="27"/>
+      <c r="G57" s="18"/>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
@@ -4860,7 +4872,7 @@
         <v>843</v>
       </c>
       <c r="F58" s="5"/>
-      <c r="G58" s="30"/>
+      <c r="G58" s="19"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
@@ -4886,7 +4898,7 @@
         <v>844</v>
       </c>
       <c r="F59" s="3"/>
-      <c r="G59" s="27"/>
+      <c r="G59" s="18"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
@@ -4912,7 +4924,7 @@
         <v>844</v>
       </c>
       <c r="F60" s="5"/>
-      <c r="G60" s="30"/>
+      <c r="G60" s="19"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
@@ -4938,7 +4950,7 @@
         <v>843</v>
       </c>
       <c r="F61" s="3"/>
-      <c r="G61" s="27"/>
+      <c r="G61" s="18"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -4964,7 +4976,7 @@
         <v>844</v>
       </c>
       <c r="F62" s="5"/>
-      <c r="G62" s="30"/>
+      <c r="G62" s="19"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -4990,7 +5002,7 @@
         <v>845</v>
       </c>
       <c r="F63" s="3"/>
-      <c r="G63" s="27"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -5016,7 +5028,7 @@
         <v>845</v>
       </c>
       <c r="F64" s="5"/>
-      <c r="G64" s="30"/>
+      <c r="G64" s="19"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
@@ -5042,7 +5054,7 @@
         <v>843</v>
       </c>
       <c r="F65" s="3"/>
-      <c r="G65" s="27"/>
+      <c r="G65" s="18"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
@@ -5068,7 +5080,7 @@
         <v>844</v>
       </c>
       <c r="F66" s="5"/>
-      <c r="G66" s="30"/>
+      <c r="G66" s="19"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
@@ -5094,7 +5106,7 @@
         <v>844</v>
       </c>
       <c r="F67" s="3"/>
-      <c r="G67" s="27"/>
+      <c r="G67" s="18"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -5120,7 +5132,7 @@
         <v>844</v>
       </c>
       <c r="F68" s="5"/>
-      <c r="G68" s="30"/>
+      <c r="G68" s="19"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
@@ -5146,7 +5158,7 @@
         <v>844</v>
       </c>
       <c r="F69" s="3"/>
-      <c r="G69" s="27"/>
+      <c r="G69" s="18"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
@@ -5172,7 +5184,7 @@
         <v>844</v>
       </c>
       <c r="F70" s="5"/>
-      <c r="G70" s="30"/>
+      <c r="G70" s="19"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8"/>
@@ -5198,7 +5210,7 @@
         <v>844</v>
       </c>
       <c r="F71" s="3"/>
-      <c r="G71" s="27"/>
+      <c r="G71" s="18"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
@@ -5224,7 +5236,7 @@
         <v>844</v>
       </c>
       <c r="F72" s="5"/>
-      <c r="G72" s="30"/>
+      <c r="G72" s="19"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
@@ -5250,7 +5262,7 @@
         <v>845</v>
       </c>
       <c r="F73" s="3"/>
-      <c r="G73" s="27"/>
+      <c r="G73" s="18"/>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
@@ -5276,7 +5288,7 @@
         <v>843</v>
       </c>
       <c r="F74" s="5"/>
-      <c r="G74" s="30"/>
+      <c r="G74" s="19"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
@@ -5302,7 +5314,7 @@
         <v>844</v>
       </c>
       <c r="F75" s="3"/>
-      <c r="G75" s="27"/>
+      <c r="G75" s="18"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
@@ -5328,7 +5340,7 @@
         <v>845</v>
       </c>
       <c r="F76" s="5"/>
-      <c r="G76" s="30"/>
+      <c r="G76" s="19"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
@@ -5354,7 +5366,7 @@
         <v>845</v>
       </c>
       <c r="F77" s="3"/>
-      <c r="G77" s="27"/>
+      <c r="G77" s="18"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
@@ -5380,7 +5392,7 @@
         <v>843</v>
       </c>
       <c r="F78" s="5"/>
-      <c r="G78" s="30"/>
+      <c r="G78" s="19"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
@@ -5406,7 +5418,7 @@
         <v>845</v>
       </c>
       <c r="F79" s="3"/>
-      <c r="G79" s="27"/>
+      <c r="G79" s="18"/>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
@@ -5432,7 +5444,7 @@
         <v>845</v>
       </c>
       <c r="F80" s="5"/>
-      <c r="G80" s="30"/>
+      <c r="G80" s="19"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
       <c r="J80" s="8"/>
@@ -5458,7 +5470,7 @@
         <v>844</v>
       </c>
       <c r="F81" s="3"/>
-      <c r="G81" s="27"/>
+      <c r="G81" s="18"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
@@ -5484,7 +5496,7 @@
         <v>844</v>
       </c>
       <c r="F82" s="5"/>
-      <c r="G82" s="30"/>
+      <c r="G82" s="19"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
@@ -5510,7 +5522,7 @@
         <v>843</v>
       </c>
       <c r="F83" s="3"/>
-      <c r="G83" s="27"/>
+      <c r="G83" s="18"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
@@ -5536,7 +5548,7 @@
         <v>844</v>
       </c>
       <c r="F84" s="5"/>
-      <c r="G84" s="30"/>
+      <c r="G84" s="19"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
@@ -5562,7 +5574,7 @@
         <v>843</v>
       </c>
       <c r="F85" s="3"/>
-      <c r="G85" s="27"/>
+      <c r="G85" s="18"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
@@ -5588,7 +5600,7 @@
         <v>843</v>
       </c>
       <c r="F86" s="5"/>
-      <c r="G86" s="30"/>
+      <c r="G86" s="19"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
@@ -5614,7 +5626,7 @@
         <v>843</v>
       </c>
       <c r="F87" s="3"/>
-      <c r="G87" s="27"/>
+      <c r="G87" s="18"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
@@ -5640,7 +5652,7 @@
         <v>844</v>
       </c>
       <c r="F88" s="5"/>
-      <c r="G88" s="30"/>
+      <c r="G88" s="19"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
@@ -5666,7 +5678,7 @@
         <v>844</v>
       </c>
       <c r="F89" s="3"/>
-      <c r="G89" s="27"/>
+      <c r="G89" s="18"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
@@ -5692,7 +5704,7 @@
         <v>845</v>
       </c>
       <c r="F90" s="5"/>
-      <c r="G90" s="30"/>
+      <c r="G90" s="19"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
@@ -5718,7 +5730,7 @@
         <v>844</v>
       </c>
       <c r="F91" s="3"/>
-      <c r="G91" s="27"/>
+      <c r="G91" s="18"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
@@ -5744,7 +5756,7 @@
         <v>844</v>
       </c>
       <c r="F92" s="5"/>
-      <c r="G92" s="30"/>
+      <c r="G92" s="19"/>
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
       <c r="J92" s="8"/>
@@ -5770,7 +5782,7 @@
         <v>844</v>
       </c>
       <c r="F93" s="3"/>
-      <c r="G93" s="27"/>
+      <c r="G93" s="18"/>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
@@ -5796,7 +5808,7 @@
         <v>845</v>
       </c>
       <c r="F94" s="5"/>
-      <c r="G94" s="30"/>
+      <c r="G94" s="19"/>
       <c r="H94" s="8"/>
       <c r="I94" s="8"/>
       <c r="J94" s="8"/>
@@ -5822,7 +5834,7 @@
         <v>844</v>
       </c>
       <c r="F95" s="3"/>
-      <c r="G95" s="27"/>
+      <c r="G95" s="18"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
@@ -5848,7 +5860,7 @@
         <v>844</v>
       </c>
       <c r="F96" s="5"/>
-      <c r="G96" s="30"/>
+      <c r="G96" s="19"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
       <c r="J96" s="8"/>
@@ -5874,7 +5886,7 @@
         <v>843</v>
       </c>
       <c r="F97" s="3"/>
-      <c r="G97" s="27"/>
+      <c r="G97" s="18"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
@@ -5900,7 +5912,7 @@
         <v>844</v>
       </c>
       <c r="F98" s="5"/>
-      <c r="G98" s="30"/>
+      <c r="G98" s="19"/>
       <c r="H98" s="8"/>
       <c r="I98" s="8"/>
       <c r="J98" s="8"/>
@@ -5926,7 +5938,7 @@
         <v>844</v>
       </c>
       <c r="F99" s="3"/>
-      <c r="G99" s="27"/>
+      <c r="G99" s="18"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
@@ -5952,7 +5964,7 @@
         <v>844</v>
       </c>
       <c r="F100" s="5"/>
-      <c r="G100" s="30"/>
+      <c r="G100" s="19"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8"/>
       <c r="J100" s="8"/>
@@ -5978,7 +5990,7 @@
         <v>843</v>
       </c>
       <c r="F101" s="3"/>
-      <c r="G101" s="27"/>
+      <c r="G101" s="18"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
@@ -6004,7 +6016,7 @@
         <v>843</v>
       </c>
       <c r="F102" s="5"/>
-      <c r="G102" s="30"/>
+      <c r="G102" s="19"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
       <c r="J102" s="8"/>
@@ -6030,7 +6042,7 @@
         <v>843</v>
       </c>
       <c r="F103" s="3"/>
-      <c r="G103" s="27"/>
+      <c r="G103" s="18"/>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
@@ -6056,7 +6068,7 @@
         <v>843</v>
       </c>
       <c r="F104" s="5"/>
-      <c r="G104" s="30"/>
+      <c r="G104" s="19"/>
       <c r="H104" s="8"/>
       <c r="I104" s="8"/>
       <c r="J104" s="8"/>
@@ -6082,7 +6094,7 @@
         <v>845</v>
       </c>
       <c r="F105" s="3"/>
-      <c r="G105" s="27"/>
+      <c r="G105" s="18"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
@@ -6108,7 +6120,7 @@
         <v>843</v>
       </c>
       <c r="F106" s="5"/>
-      <c r="G106" s="30"/>
+      <c r="G106" s="19"/>
       <c r="H106" s="8"/>
       <c r="I106" s="8"/>
       <c r="J106" s="8"/>
@@ -6134,7 +6146,7 @@
         <v>844</v>
       </c>
       <c r="F107" s="3"/>
-      <c r="G107" s="27"/>
+      <c r="G107" s="18"/>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
@@ -6160,7 +6172,7 @@
         <v>843</v>
       </c>
       <c r="F108" s="5"/>
-      <c r="G108" s="30"/>
+      <c r="G108" s="19"/>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
       <c r="J108" s="8"/>
@@ -6186,7 +6198,7 @@
         <v>844</v>
       </c>
       <c r="F109" s="3"/>
-      <c r="G109" s="27"/>
+      <c r="G109" s="18"/>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
@@ -6212,7 +6224,7 @@
         <v>844</v>
       </c>
       <c r="F110" s="5"/>
-      <c r="G110" s="30"/>
+      <c r="G110" s="19"/>
       <c r="H110" s="8"/>
       <c r="I110" s="8"/>
       <c r="J110" s="8"/>
@@ -6238,7 +6250,7 @@
         <v>844</v>
       </c>
       <c r="F111" s="3"/>
-      <c r="G111" s="27"/>
+      <c r="G111" s="18"/>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
@@ -6264,7 +6276,7 @@
         <v>844</v>
       </c>
       <c r="F112" s="5"/>
-      <c r="G112" s="30"/>
+      <c r="G112" s="19"/>
       <c r="H112" s="8"/>
       <c r="I112" s="8"/>
       <c r="J112" s="8"/>
@@ -6290,7 +6302,7 @@
         <v>844</v>
       </c>
       <c r="F113" s="3"/>
-      <c r="G113" s="27"/>
+      <c r="G113" s="18"/>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
@@ -6316,7 +6328,7 @@
         <v>844</v>
       </c>
       <c r="F114" s="5"/>
-      <c r="G114" s="30"/>
+      <c r="G114" s="19"/>
       <c r="H114" s="8"/>
       <c r="I114" s="8"/>
       <c r="J114" s="8"/>
@@ -6342,7 +6354,7 @@
         <v>844</v>
       </c>
       <c r="F115" s="3"/>
-      <c r="G115" s="27"/>
+      <c r="G115" s="18"/>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
@@ -6368,7 +6380,7 @@
         <v>844</v>
       </c>
       <c r="F116" s="5"/>
-      <c r="G116" s="30"/>
+      <c r="G116" s="19"/>
       <c r="H116" s="8"/>
       <c r="I116" s="8"/>
       <c r="J116" s="8"/>
@@ -6394,7 +6406,7 @@
         <v>844</v>
       </c>
       <c r="F117" s="3"/>
-      <c r="G117" s="27"/>
+      <c r="G117" s="18"/>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
@@ -6420,7 +6432,7 @@
         <v>844</v>
       </c>
       <c r="F118" s="5"/>
-      <c r="G118" s="30"/>
+      <c r="G118" s="19"/>
       <c r="H118" s="8"/>
       <c r="I118" s="8"/>
       <c r="J118" s="8"/>
@@ -6446,7 +6458,7 @@
         <v>844</v>
       </c>
       <c r="F119" s="3"/>
-      <c r="G119" s="27"/>
+      <c r="G119" s="18"/>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
@@ -6472,7 +6484,7 @@
         <v>844</v>
       </c>
       <c r="F120" s="5"/>
-      <c r="G120" s="30"/>
+      <c r="G120" s="19"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
@@ -6498,7 +6510,7 @@
         <v>844</v>
       </c>
       <c r="F121" s="3"/>
-      <c r="G121" s="27"/>
+      <c r="G121" s="18"/>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
@@ -6524,7 +6536,7 @@
         <v>844</v>
       </c>
       <c r="F122" s="5"/>
-      <c r="G122" s="30"/>
+      <c r="G122" s="19"/>
       <c r="H122" s="8"/>
       <c r="I122" s="8"/>
       <c r="J122" s="8"/>
@@ -6550,7 +6562,7 @@
         <v>844</v>
       </c>
       <c r="F123" s="3"/>
-      <c r="G123" s="27"/>
+      <c r="G123" s="18"/>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
@@ -6576,7 +6588,7 @@
         <v>844</v>
       </c>
       <c r="F124" s="5"/>
-      <c r="G124" s="30"/>
+      <c r="G124" s="19"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
@@ -6602,7 +6614,7 @@
         <v>844</v>
       </c>
       <c r="F125" s="3"/>
-      <c r="G125" s="27"/>
+      <c r="G125" s="18"/>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
@@ -6628,7 +6640,7 @@
         <v>844</v>
       </c>
       <c r="F126" s="5"/>
-      <c r="G126" s="30"/>
+      <c r="G126" s="19"/>
       <c r="H126" s="8"/>
       <c r="I126" s="8"/>
       <c r="J126" s="8"/>
@@ -6654,7 +6666,7 @@
         <v>844</v>
       </c>
       <c r="F127" s="3"/>
-      <c r="G127" s="27"/>
+      <c r="G127" s="18"/>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
@@ -6680,7 +6692,7 @@
         <v>844</v>
       </c>
       <c r="F128" s="5"/>
-      <c r="G128" s="30"/>
+      <c r="G128" s="19"/>
       <c r="H128" s="8"/>
       <c r="I128" s="8"/>
       <c r="J128" s="8"/>
@@ -6706,7 +6718,7 @@
         <v>844</v>
       </c>
       <c r="F129" s="3"/>
-      <c r="G129" s="27"/>
+      <c r="G129" s="18"/>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
@@ -6732,7 +6744,7 @@
         <v>843</v>
       </c>
       <c r="F130" s="5"/>
-      <c r="G130" s="30"/>
+      <c r="G130" s="19"/>
       <c r="H130" s="8"/>
       <c r="I130" s="8"/>
       <c r="J130" s="8"/>
@@ -6758,7 +6770,7 @@
         <v>844</v>
       </c>
       <c r="F131" s="3"/>
-      <c r="G131" s="27"/>
+      <c r="G131" s="18"/>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
@@ -6784,7 +6796,7 @@
         <v>844</v>
       </c>
       <c r="F132" s="5"/>
-      <c r="G132" s="30"/>
+      <c r="G132" s="19"/>
       <c r="H132" s="8"/>
       <c r="I132" s="8"/>
       <c r="J132" s="8"/>
@@ -6810,7 +6822,7 @@
         <v>844</v>
       </c>
       <c r="F133" s="3"/>
-      <c r="G133" s="27"/>
+      <c r="G133" s="18"/>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
@@ -6836,7 +6848,7 @@
         <v>843</v>
       </c>
       <c r="F134" s="5"/>
-      <c r="G134" s="30"/>
+      <c r="G134" s="19"/>
       <c r="H134" s="8"/>
       <c r="I134" s="8"/>
       <c r="J134" s="8"/>
@@ -6862,7 +6874,7 @@
         <v>843</v>
       </c>
       <c r="F135" s="3"/>
-      <c r="G135" s="27"/>
+      <c r="G135" s="18"/>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
@@ -6888,7 +6900,7 @@
         <v>844</v>
       </c>
       <c r="F136" s="5"/>
-      <c r="G136" s="30"/>
+      <c r="G136" s="19"/>
       <c r="H136" s="8"/>
       <c r="I136" s="8"/>
       <c r="J136" s="8"/>
@@ -6914,7 +6926,7 @@
         <v>844</v>
       </c>
       <c r="F137" s="3"/>
-      <c r="G137" s="27"/>
+      <c r="G137" s="18"/>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
@@ -6940,7 +6952,7 @@
         <v>844</v>
       </c>
       <c r="F138" s="5"/>
-      <c r="G138" s="30"/>
+      <c r="G138" s="19"/>
       <c r="H138" s="8"/>
       <c r="I138" s="8"/>
       <c r="J138" s="8"/>
@@ -6966,7 +6978,7 @@
         <v>845</v>
       </c>
       <c r="F139" s="3"/>
-      <c r="G139" s="27"/>
+      <c r="G139" s="18"/>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
@@ -6992,7 +7004,7 @@
         <v>844</v>
       </c>
       <c r="F140" s="5"/>
-      <c r="G140" s="30"/>
+      <c r="G140" s="19"/>
       <c r="H140" s="8"/>
       <c r="I140" s="8"/>
       <c r="J140" s="8"/>
@@ -7018,7 +7030,7 @@
         <v>844</v>
       </c>
       <c r="F141" s="3"/>
-      <c r="G141" s="27"/>
+      <c r="G141" s="18"/>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
@@ -7044,7 +7056,7 @@
         <v>844</v>
       </c>
       <c r="F142" s="5"/>
-      <c r="G142" s="30"/>
+      <c r="G142" s="19"/>
       <c r="H142" s="8"/>
       <c r="I142" s="8"/>
       <c r="J142" s="8"/>
@@ -7070,7 +7082,7 @@
         <v>844</v>
       </c>
       <c r="F143" s="3"/>
-      <c r="G143" s="27"/>
+      <c r="G143" s="18"/>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
@@ -7096,7 +7108,7 @@
         <v>845</v>
       </c>
       <c r="F144" s="5"/>
-      <c r="G144" s="30"/>
+      <c r="G144" s="19"/>
       <c r="H144" s="8"/>
       <c r="I144" s="8"/>
       <c r="J144" s="8"/>
@@ -7122,7 +7134,7 @@
         <v>844</v>
       </c>
       <c r="F145" s="3"/>
-      <c r="G145" s="27"/>
+      <c r="G145" s="18"/>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
@@ -7148,7 +7160,7 @@
         <v>844</v>
       </c>
       <c r="F146" s="5"/>
-      <c r="G146" s="30"/>
+      <c r="G146" s="19"/>
       <c r="H146" s="8"/>
       <c r="I146" s="8"/>
       <c r="J146" s="8"/>
@@ -7174,7 +7186,7 @@
         <v>844</v>
       </c>
       <c r="F147" s="3"/>
-      <c r="G147" s="27"/>
+      <c r="G147" s="18"/>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
@@ -7200,7 +7212,7 @@
         <v>843</v>
       </c>
       <c r="F148" s="5"/>
-      <c r="G148" s="30"/>
+      <c r="G148" s="19"/>
       <c r="H148" s="8"/>
       <c r="I148" s="8"/>
       <c r="J148" s="8"/>
@@ -7226,7 +7238,7 @@
         <v>844</v>
       </c>
       <c r="F149" s="3"/>
-      <c r="G149" s="27"/>
+      <c r="G149" s="18"/>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
@@ -7252,7 +7264,7 @@
         <v>844</v>
       </c>
       <c r="F150" s="5"/>
-      <c r="G150" s="30"/>
+      <c r="G150" s="19"/>
       <c r="H150" s="8"/>
       <c r="I150" s="8"/>
       <c r="J150" s="8"/>
@@ -7278,7 +7290,7 @@
         <v>843</v>
       </c>
       <c r="F151" s="3"/>
-      <c r="G151" s="27"/>
+      <c r="G151" s="18"/>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
@@ -7304,7 +7316,7 @@
         <v>844</v>
       </c>
       <c r="F152" s="5"/>
-      <c r="G152" s="30"/>
+      <c r="G152" s="19"/>
       <c r="H152" s="8"/>
       <c r="I152" s="8"/>
       <c r="J152" s="8"/>
@@ -7330,7 +7342,7 @@
         <v>843</v>
       </c>
       <c r="F153" s="3"/>
-      <c r="G153" s="27"/>
+      <c r="G153" s="18"/>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
@@ -7356,7 +7368,7 @@
         <v>844</v>
       </c>
       <c r="F154" s="5"/>
-      <c r="G154" s="30"/>
+      <c r="G154" s="19"/>
       <c r="H154" s="8"/>
       <c r="I154" s="8"/>
       <c r="J154" s="8"/>
@@ -7382,7 +7394,7 @@
         <v>845</v>
       </c>
       <c r="F155" s="3"/>
-      <c r="G155" s="27"/>
+      <c r="G155" s="18"/>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
@@ -7408,7 +7420,7 @@
         <v>844</v>
       </c>
       <c r="F156" s="5"/>
-      <c r="G156" s="30"/>
+      <c r="G156" s="19"/>
       <c r="H156" s="8"/>
       <c r="I156" s="8"/>
       <c r="J156" s="8"/>
@@ -7434,7 +7446,7 @@
         <v>844</v>
       </c>
       <c r="F157" s="3"/>
-      <c r="G157" s="27"/>
+      <c r="G157" s="18"/>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
@@ -7460,7 +7472,7 @@
         <v>844</v>
       </c>
       <c r="F158" s="5"/>
-      <c r="G158" s="30"/>
+      <c r="G158" s="19"/>
       <c r="H158" s="8"/>
       <c r="I158" s="8"/>
       <c r="J158" s="8"/>
@@ -7526,42 +7538,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="30" t="s">
         <v>710</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -7589,7 +7601,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="22"/>
+      <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">

</xml_diff>

<commit_message>
Se agrega ID_Cron de prueba en el archivo de plan de trabajo para el proceso de Facturas Pendienetes en Cedis Ori
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD2C934-8996-4333-B7C5-648D2A72EF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF77B0E-187C-425C-AC41-2984C388EC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2702,7 +2702,7 @@
     <t>Ricardo</t>
   </si>
   <si>
-    <t xml:space="preserve">08/05/2025: Se emepiza con el analsisi del módulo y su desarrollo </t>
+    <t xml:space="preserve">08/05/2025: Se emepiza con el analsisi del módulo y su desarrollo  </t>
   </si>
 </sst>
 </file>
@@ -3259,7 +3259,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
actualizacion de fechas de ricardo, compo observaciones
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\net1\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF77B0E-187C-425C-AC41-2984C388EC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A512CD1-7300-439A-AD77-12EE24E63C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -2702,7 +2702,7 @@
     <t>Ricardo</t>
   </si>
   <si>
-    <t xml:space="preserve">08/05/2025: Se emepiza con el analsisi del módulo y su desarrollo  </t>
+    <t xml:space="preserve">08/05/2025: Se empieza con el analsis del módulo y su desarrollo  </t>
   </si>
 </sst>
 </file>
@@ -3259,7 +3259,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualizo Plan de Trabajo con el avance del Reporte de Convertidores sin Expedición.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\net1\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A512CD1-7300-439A-AD77-12EE24E63C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F37D550-0349-4F60-A711-DC38D371B14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4143" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="852">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2693,9 +2693,6 @@
     <t>Enrique</t>
   </si>
   <si>
-    <t>08/05/2025: Se inicia desarrollo del módulo.</t>
-  </si>
-  <si>
     <t>Fecha de inicio</t>
   </si>
   <si>
@@ -2703,6 +2700,10 @@
   </si>
   <si>
     <t xml:space="preserve">08/05/2025: Se empieza con el analsis del módulo y su desarrollo  </t>
+  </si>
+  <si>
+    <t>08/05/2025: Se inicia desarrollo del módulo.
+09/05/2025: Se termina el desarrollo en ambiente local.</t>
   </si>
 </sst>
 </file>
@@ -3257,9 +3258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3299,7 +3300,7 @@
         <v>841</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="H1" s="26" t="s">
         <v>704</v>
@@ -3692,13 +3693,13 @@
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="4" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="M13" s="4">
         <v>1689811</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -3989,7 +3990,7 @@
       <c r="M24" s="6"/>
       <c r="N24" s="5"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -4009,16 +4010,20 @@
       <c r="G25" s="18">
         <v>45785</v>
       </c>
-      <c r="H25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>711</v>
+      </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
       <c r="L25" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="M25" s="4"/>
+      <c r="M25" s="4">
+        <v>7947853</v>
+      </c>
       <c r="N25" s="3" t="s">
-        <v>848</v>
+        <v>851</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se actualiza listado de procesos a desarrollar.
Se inhabilitaron dos reportes automáticos a solicitud de Dirección General.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F37D550-0349-4F60-A711-DC38D371B14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5908DA-CC26-4B00-B8E3-EA32FE7374BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$N$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$2:$O$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$2:$O$599</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4149" uniqueCount="854">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2704,13 +2704,19 @@
   <si>
     <t>08/05/2025: Se inicia desarrollo del módulo.
 09/05/2025: Se termina el desarrollo en ambiente local.</t>
+  </si>
+  <si>
+    <t>12/05/2025: D.G. solicita inactivar la instancia automática de éste reporte, ya que no se utiliza.</t>
+  </si>
+  <si>
+    <t>15/05/2025: Se desactivó la emisión automática de este reporte a solicitud de D.G.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2728,6 +2734,25 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2826,7 +2851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2893,6 +2918,30 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3259,8 +3308,8 @@
   <dimension ref="A1:N158"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <pane ySplit="2" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3281,51 +3330,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="32" t="s">
         <v>814</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="38" t="s">
         <v>840</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="38" t="s">
         <v>841</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="40" t="s">
         <v>848</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="34" t="s">
         <v>704</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="24" t="s">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="32" t="s">
         <v>716</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="36" t="s">
         <v>837</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="31" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="33"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="41"/>
       <c r="H2" s="9" t="s">
         <v>705</v>
       </c>
@@ -3338,9 +3387,9 @@
       <c r="K2" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="23"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="31"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -4074,7 +4123,9 @@
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="4"/>
+      <c r="L27" s="4" t="s">
+        <v>847</v>
+      </c>
       <c r="M27" s="4"/>
       <c r="N27" s="3"/>
     </row>
@@ -6556,17 +6607,17 @@
       <c r="A123" s="3">
         <v>120</v>
       </c>
-      <c r="B123" s="3">
+      <c r="B123" s="23">
         <v>213</v>
       </c>
-      <c r="C123" s="3" t="s">
+      <c r="C123" s="23" t="s">
         <v>428</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="23" t="s">
         <v>429</v>
       </c>
-      <c r="E123" s="3" t="s">
-        <v>844</v>
+      <c r="E123" s="23" t="s">
+        <v>845</v>
       </c>
       <c r="F123" s="3"/>
       <c r="G123" s="18"/>
@@ -6576,7 +6627,9 @@
       <c r="K123" s="7"/>
       <c r="L123" s="4"/>
       <c r="M123" s="4"/>
-      <c r="N123" s="3"/>
+      <c r="N123" s="3" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
@@ -7280,31 +7333,33 @@
       <c r="M150" s="6"/>
       <c r="N150" s="5"/>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A151" s="3">
+    <row r="151" spans="1:14" ht="24" x14ac:dyDescent="0.25">
+      <c r="A151" s="26">
         <v>148</v>
       </c>
-      <c r="B151" s="3">
+      <c r="B151" s="26">
         <v>110</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="C151" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="D151" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="E151" s="3" t="s">
-        <v>843</v>
-      </c>
-      <c r="F151" s="3"/>
-      <c r="G151" s="18"/>
-      <c r="H151" s="7"/>
-      <c r="I151" s="7"/>
-      <c r="J151" s="7"/>
-      <c r="K151" s="7"/>
-      <c r="L151" s="4"/>
-      <c r="M151" s="4"/>
-      <c r="N151" s="3"/>
+      <c r="E151" s="26" t="s">
+        <v>844</v>
+      </c>
+      <c r="F151" s="26"/>
+      <c r="G151" s="27"/>
+      <c r="H151" s="28"/>
+      <c r="I151" s="28"/>
+      <c r="J151" s="28"/>
+      <c r="K151" s="28"/>
+      <c r="L151" s="29"/>
+      <c r="M151" s="29"/>
+      <c r="N151" s="23" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
@@ -7545,42 +7600,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>710</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35" t="s">
         <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -7608,7 +7663,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="27"/>
+      <c r="O2" s="35"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -11407,35 +11462,39 @@
       <c r="O122" s="6"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A123" s="3">
+      <c r="A123" s="23">
         <v>121</v>
       </c>
-      <c r="B123" s="3">
+      <c r="B123" s="23">
         <v>110</v>
       </c>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3" t="s">
+      <c r="C123" s="23">
+        <v>63380</v>
+      </c>
+      <c r="D123" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="E123" s="3" t="s">
+      <c r="E123" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="F123" s="7" t="s">
-        <v>711</v>
-      </c>
-      <c r="G123" s="7" t="s">
-        <v>711</v>
-      </c>
-      <c r="H123" s="7" t="s">
-        <v>711</v>
-      </c>
-      <c r="I123" s="7"/>
-      <c r="J123" s="7"/>
-      <c r="K123" s="7"/>
-      <c r="L123" s="7"/>
-      <c r="M123" s="7"/>
-      <c r="N123" s="7"/>
-      <c r="O123" s="4"/>
+      <c r="F123" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="G123" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="H123" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="I123" s="24"/>
+      <c r="J123" s="24"/>
+      <c r="K123" s="24"/>
+      <c r="L123" s="24"/>
+      <c r="M123" s="24"/>
+      <c r="N123" s="24"/>
+      <c r="O123" s="25" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
@@ -11466,7 +11525,9 @@
       <c r="L124" s="8"/>
       <c r="M124" s="8"/>
       <c r="N124" s="8"/>
-      <c r="O124" s="6"/>
+      <c r="O124" s="6" t="s">
+        <v>844</v>
+      </c>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
@@ -27370,7 +27431,7 @@
       <c r="O599" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:O599" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Se actualiza el plan de trabajo, se empieza a trabajar con un nuevo proceso.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F37D550-0349-4F60-A711-DC38D371B14C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2270FCAC-C7F5-46B0-9ACC-018303CF5F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4147" uniqueCount="853">
   <si>
     <t>ID_REP</t>
   </si>
@@ -2704,6 +2704,9 @@
   <si>
     <t>08/05/2025: Se inicia desarrollo del módulo.
 09/05/2025: Se termina el desarrollo en ambiente local.</t>
+  </si>
+  <si>
+    <t>08/05/2025: Se empieza con el analisis y se empezaron a sacar las cossultas</t>
   </si>
 </sst>
 </file>
@@ -3258,9 +3261,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
+      <selection pane="bottomLeft" activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,14 +4046,22 @@
         <v>845</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="8"/>
+      <c r="G26" s="19">
+        <v>45796</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>711</v>
+      </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="6"/>
+      <c r="L26" s="6" t="s">
+        <v>849</v>
+      </c>
       <c r="M26" s="6"/>
-      <c r="N26" s="5"/>
+      <c r="N26" s="5" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="3">

</xml_diff>

<commit_message>
Se actualiza plan de trabajo, se emepieza a trabajar en un nuevo proceso.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2270FCAC-C7F5-46B0-9ACC-018303CF5F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4553C4E8-EECA-4904-ADE2-31FFDE5947FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2699,14 +2699,14 @@
     <t>Ricardo</t>
   </si>
   <si>
-    <t xml:space="preserve">08/05/2025: Se empieza con el analsis del módulo y su desarrollo  </t>
-  </si>
-  <si>
     <t>08/05/2025: Se inicia desarrollo del módulo.
 09/05/2025: Se termina el desarrollo en ambiente local.</t>
   </si>
   <si>
-    <t>08/05/2025: Se empieza con el analisis y se empezaron a sacar las cossultas</t>
+    <t xml:space="preserve">08/05/2025: Se empieza con el analsis del módulo y su desarrollo </t>
+  </si>
+  <si>
+    <t>08/05/2025: Se empieza con el analisis y se empezaron a sacar las consultas</t>
   </si>
 </sst>
 </file>
@@ -3702,7 +3702,7 @@
         <v>1689811</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4026,7 +4026,7 @@
         <v>7947853</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se agrega el proceso de Facturas Pendientes en Cedis Ori
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EDDCB2-D77C-4E77-A216-F08FDCEF5678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ABD3B8-4C27-460E-ADDD-91AD58811B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2703,10 +2703,11 @@
 09/05/2025: Se termina el desarrollo en ambiente local.</t>
   </si>
   <si>
-    <t xml:space="preserve">08/05/2025: Se empieza con el analsis del módulo y su desarrollo </t>
-  </si>
-  <si>
     <t>08/05/2025: Se empieza con el analisis y se empezaron a sacar las consultas</t>
+  </si>
+  <si>
+    <t>08/05/2025: Se empieza con el analsis del módulo y su desarrollo 
+20/05/2025: Se sube al repositorio</t>
   </si>
 </sst>
 </file>
@@ -3263,7 +3264,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N24" sqref="N24"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,7 +3672,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -3702,7 +3703,7 @@
         <v>1689811</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -4060,7 +4061,7 @@
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="5" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se actualiza el plan de trabajo, se agrega hoja de reportes no frecuentes.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E1E7D6-5A6A-4B69-AFF0-562CD67ED532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8C18F-6B51-4E25-88F6-1B2BBB44DB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
     <sheet name="Detalle" sheetId="1" r:id="rId2"/>
     <sheet name="Activos" sheetId="6" r:id="rId3"/>
     <sheet name="Detalle_Activos" sheetId="7" r:id="rId4"/>
+    <sheet name="Reportes No Frecuentes" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$N$158</definedName>
@@ -150,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6009" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6018" uniqueCount="978">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3064,13 +3065,29 @@
 09/05/2025: Se termina el desarrollo en ambiente local.</t>
   </si>
   <si>
-    <t>08/05/2025: Se empieza con el analisis y se empezaron a sacar las consultas</t>
-  </si>
-  <si>
     <t>15/05/2025 8:55 - Se inactiva a solicitud de D.G.</t>
   </si>
   <si>
     <t>12/05/2025 8:46 - Este reporte se ejecutaba tanto Bajo Demanda como de Forma Automática, sin embargo DG solicitó inactivar el proceso Automático.</t>
+  </si>
+  <si>
+    <t>ID REP</t>
+  </si>
+  <si>
+    <t>ID_CRON UTILZADO EN EL MOMENTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/05/2025: Se empieza con el analisis y se empezaron a sacar las consultas
+</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>29/05/2025: Se inicia con el analisis del módulo para poder migrarlo</t>
   </si>
 </sst>
 </file>
@@ -3328,6 +3345,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3355,6 +3388,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3364,28 +3403,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3717,9 +3734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A2"/>
+      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3729,7 +3746,7 @@
     <col min="3" max="3" width="56.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="15" style="42" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" style="1" bestFit="1" customWidth="1"/>
@@ -3740,51 +3757,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="37" t="s">
         <v>505</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="39" t="s">
         <v>964</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="33" t="s">
         <v>369</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="25" t="s">
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="31" t="s">
         <v>381</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="35" t="s">
         <v>502</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="30" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="37"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="40"/>
       <c r="H2" s="9" t="s">
         <v>370</v>
       </c>
@@ -3797,9 +3814,9 @@
       <c r="K2" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="24"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -3820,7 +3837,7 @@
       <c r="F3" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="G3" s="38"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="7" t="s">
         <v>376</v>
       </c>
@@ -3857,7 +3874,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B4,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G4" s="39"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="8" t="s">
         <v>376</v>
       </c>
@@ -3894,7 +3911,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B5,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G5" s="38"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="7" t="s">
         <v>376</v>
       </c>
@@ -3931,7 +3948,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B6,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G6" s="39"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="8" t="s">
         <v>376</v>
       </c>
@@ -3968,7 +3985,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B7,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="7" t="s">
         <v>376</v>
       </c>
@@ -4005,7 +4022,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B8,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G8" s="39"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="8" t="s">
         <v>376</v>
       </c>
@@ -4042,7 +4059,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B9,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G9" s="38"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="7" t="s">
         <v>376</v>
       </c>
@@ -4079,7 +4096,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B10,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G10" s="39"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="8" t="s">
         <v>376</v>
       </c>
@@ -4116,7 +4133,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B11,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G11" s="38"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -4145,7 +4162,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B12,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>19</v>
       </c>
-      <c r="G12" s="39"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -4174,7 +4191,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B13,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="24">
         <v>45783</v>
       </c>
       <c r="H13" s="7"/>
@@ -4211,7 +4228,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B14,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>66</v>
       </c>
-      <c r="G14" s="39"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -4242,7 +4259,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B15,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G15" s="38"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -4271,7 +4288,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B16,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G16" s="39"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -4300,7 +4317,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B17,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G17" s="38"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -4329,7 +4346,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B18,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G18" s="39"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
@@ -4358,7 +4375,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B19,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="38"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -4387,7 +4404,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B20,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G20" s="39"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -4416,7 +4433,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B21,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G21" s="38"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -4445,7 +4462,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B22,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G22" s="39"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -4474,7 +4491,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B23,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G23" s="38"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -4503,7 +4520,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B24,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G24" s="39"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
@@ -4532,7 +4549,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B25,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="24">
         <v>45785</v>
       </c>
       <c r="H25" s="7" t="s">
@@ -4551,7 +4568,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>23</v>
       </c>
@@ -4571,7 +4588,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B26,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="25">
         <v>45796</v>
       </c>
       <c r="H26" s="8" t="s">
@@ -4585,7 +4602,7 @@
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="5" t="s">
-        <v>970</v>
+        <v>975</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -4608,7 +4625,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B27,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>16</v>
       </c>
-      <c r="G27" s="38"/>
+      <c r="G27" s="24"/>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
@@ -4637,7 +4654,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B28,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G28" s="39"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -4666,7 +4683,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B29,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G29" s="38"/>
+      <c r="G29" s="24"/>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -4695,7 +4712,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B30,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G30" s="39"/>
+      <c r="G30" s="25"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
@@ -4724,7 +4741,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B31,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G31" s="38"/>
+      <c r="G31" s="24"/>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -4755,14 +4772,24 @@
         <f>_xlfn.IFNA(VLOOKUP(B32,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>5</v>
       </c>
-      <c r="G32" s="39"/>
-      <c r="H32" s="8"/>
+      <c r="G32" s="25">
+        <v>45806</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>976</v>
+      </c>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="5"/>
+      <c r="L32" s="6" t="s">
+        <v>965</v>
+      </c>
+      <c r="M32" s="5">
+        <v>129887</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>977</v>
+      </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -4784,7 +4811,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B33,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G33" s="38"/>
+      <c r="G33" s="24"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -4813,7 +4840,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B34,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G34" s="39"/>
+      <c r="G34" s="25"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -4844,7 +4871,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B35,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G35" s="40"/>
+      <c r="G35" s="26"/>
       <c r="H35" s="15"/>
       <c r="I35" s="15"/>
       <c r="J35" s="15"/>
@@ -4873,7 +4900,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B36,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G36" s="41"/>
+      <c r="G36" s="27"/>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
@@ -4902,7 +4929,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B37,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>4</v>
       </c>
-      <c r="G37" s="38"/>
+      <c r="G37" s="24"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
@@ -4931,7 +4958,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B38,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G38" s="39"/>
+      <c r="G38" s="25"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -4960,7 +4987,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B39,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G39" s="38"/>
+      <c r="G39" s="24"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
@@ -4989,7 +5016,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B40,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G40" s="39"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
@@ -5018,7 +5045,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B41,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G41" s="38"/>
+      <c r="G41" s="24"/>
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
@@ -5047,7 +5074,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B42,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G42" s="39"/>
+      <c r="G42" s="25"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -5076,7 +5103,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B43,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G43" s="38"/>
+      <c r="G43" s="24"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
@@ -5105,7 +5132,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B44,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G44" s="39"/>
+      <c r="G44" s="25"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -5134,7 +5161,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B45,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G45" s="38"/>
+      <c r="G45" s="24"/>
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
@@ -5163,7 +5190,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B46,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G46" s="39"/>
+      <c r="G46" s="25"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
@@ -5192,7 +5219,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B47,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G47" s="38"/>
+      <c r="G47" s="24"/>
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
@@ -5221,7 +5248,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B48,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G48" s="39"/>
+      <c r="G48" s="25"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
@@ -5250,7 +5277,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B49,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G49" s="38"/>
+      <c r="G49" s="24"/>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
@@ -5279,7 +5306,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B50,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G50" s="39"/>
+      <c r="G50" s="25"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
       <c r="J50" s="8"/>
@@ -5308,7 +5335,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B51,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G51" s="38"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
@@ -5337,7 +5364,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B52,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G52" s="39"/>
+      <c r="G52" s="25"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
@@ -5366,7 +5393,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B53,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G53" s="38"/>
+      <c r="G53" s="24"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
@@ -5395,7 +5422,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B54,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G54" s="39"/>
+      <c r="G54" s="25"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
@@ -5424,7 +5451,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B55,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G55" s="38"/>
+      <c r="G55" s="24"/>
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
@@ -5453,7 +5480,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B56,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G56" s="39"/>
+      <c r="G56" s="25"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
       <c r="J56" s="8"/>
@@ -5482,7 +5509,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B57,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G57" s="38"/>
+      <c r="G57" s="24"/>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
@@ -5511,7 +5538,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B58,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G58" s="39"/>
+      <c r="G58" s="25"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
       <c r="J58" s="8"/>
@@ -5540,7 +5567,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B59,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G59" s="38"/>
+      <c r="G59" s="24"/>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
@@ -5569,7 +5596,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B60,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G60" s="39"/>
+      <c r="G60" s="25"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
       <c r="J60" s="8"/>
@@ -5598,7 +5625,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B61,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G61" s="38"/>
+      <c r="G61" s="24"/>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
@@ -5627,7 +5654,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B62,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G62" s="39"/>
+      <c r="G62" s="25"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
@@ -5656,7 +5683,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B63,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G63" s="38"/>
+      <c r="G63" s="24"/>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -5685,7 +5712,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B64,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>151</v>
       </c>
-      <c r="G64" s="39"/>
+      <c r="G64" s="25"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
@@ -5714,7 +5741,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B65,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>164</v>
       </c>
-      <c r="G65" s="38"/>
+      <c r="G65" s="24"/>
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
@@ -5743,7 +5770,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B66,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G66" s="39"/>
+      <c r="G66" s="25"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
       <c r="J66" s="8"/>
@@ -5772,7 +5799,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B67,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G67" s="38"/>
+      <c r="G67" s="24"/>
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
@@ -5801,7 +5828,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B68,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G68" s="39"/>
+      <c r="G68" s="25"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
       <c r="J68" s="8"/>
@@ -5830,7 +5857,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B69,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G69" s="38"/>
+      <c r="G69" s="24"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
@@ -5859,7 +5886,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B70,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G70" s="39"/>
+      <c r="G70" s="25"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
       <c r="J70" s="8"/>
@@ -5888,7 +5915,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B71,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G71" s="38"/>
+      <c r="G71" s="24"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
@@ -5917,7 +5944,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B72,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G72" s="39"/>
+      <c r="G72" s="25"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
       <c r="J72" s="8"/>
@@ -5946,7 +5973,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B73,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>2</v>
       </c>
-      <c r="G73" s="38"/>
+      <c r="G73" s="24"/>
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
@@ -5975,7 +6002,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B74,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G74" s="39"/>
+      <c r="G74" s="25"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
       <c r="J74" s="8"/>
@@ -6004,7 +6031,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B75,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G75" s="38"/>
+      <c r="G75" s="24"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
@@ -6033,7 +6060,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B76,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G76" s="39"/>
+      <c r="G76" s="25"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
@@ -6062,7 +6089,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B77,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G77" s="38"/>
+      <c r="G77" s="24"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
@@ -6091,7 +6118,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B78,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G78" s="39"/>
+      <c r="G78" s="25"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
       <c r="J78" s="8"/>
@@ -6120,7 +6147,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B79,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G79" s="38"/>
+      <c r="G79" s="24"/>
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
@@ -6149,7 +6176,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B80,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G80" s="39"/>
+      <c r="G80" s="25"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
       <c r="J80" s="8"/>
@@ -6178,7 +6205,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B81,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G81" s="38"/>
+      <c r="G81" s="24"/>
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
@@ -6207,7 +6234,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B82,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G82" s="39"/>
+      <c r="G82" s="25"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
@@ -6236,7 +6263,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B83,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G83" s="38"/>
+      <c r="G83" s="24"/>
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
@@ -6265,7 +6292,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B84,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G84" s="39"/>
+      <c r="G84" s="25"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
@@ -6294,7 +6321,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B85,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G85" s="38"/>
+      <c r="G85" s="24"/>
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
@@ -6323,7 +6350,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B86,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G86" s="39"/>
+      <c r="G86" s="25"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
@@ -6352,7 +6379,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B87,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G87" s="38"/>
+      <c r="G87" s="24"/>
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
@@ -6381,7 +6408,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B88,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G88" s="39"/>
+      <c r="G88" s="25"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
@@ -6410,7 +6437,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B89,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G89" s="38"/>
+      <c r="G89" s="24"/>
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
@@ -6439,7 +6466,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B90,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G90" s="39"/>
+      <c r="G90" s="25"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
@@ -6468,7 +6495,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B91,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G91" s="38"/>
+      <c r="G91" s="24"/>
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
@@ -6497,7 +6524,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B92,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G92" s="39"/>
+      <c r="G92" s="25"/>
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
       <c r="J92" s="8"/>
@@ -6526,7 +6553,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B93,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G93" s="38"/>
+      <c r="G93" s="24"/>
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
@@ -6555,7 +6582,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B94,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>5</v>
       </c>
-      <c r="G94" s="39"/>
+      <c r="G94" s="25"/>
       <c r="H94" s="8"/>
       <c r="I94" s="8"/>
       <c r="J94" s="8"/>
@@ -6584,7 +6611,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B95,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G95" s="38"/>
+      <c r="G95" s="24"/>
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
@@ -6613,7 +6640,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B96,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G96" s="39"/>
+      <c r="G96" s="25"/>
       <c r="H96" s="8"/>
       <c r="I96" s="8"/>
       <c r="J96" s="8"/>
@@ -6642,7 +6669,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B97,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G97" s="38"/>
+      <c r="G97" s="24"/>
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
@@ -6671,7 +6698,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B98,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G98" s="39"/>
+      <c r="G98" s="25"/>
       <c r="H98" s="8"/>
       <c r="I98" s="8"/>
       <c r="J98" s="8"/>
@@ -6700,7 +6727,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B99,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G99" s="38"/>
+      <c r="G99" s="24"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
@@ -6729,7 +6756,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B100,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G100" s="39"/>
+      <c r="G100" s="25"/>
       <c r="H100" s="8"/>
       <c r="I100" s="8"/>
       <c r="J100" s="8"/>
@@ -6758,7 +6785,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B101,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G101" s="38"/>
+      <c r="G101" s="24"/>
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
@@ -6787,7 +6814,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B102,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G102" s="39"/>
+      <c r="G102" s="25"/>
       <c r="H102" s="8"/>
       <c r="I102" s="8"/>
       <c r="J102" s="8"/>
@@ -6816,7 +6843,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B103,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G103" s="38"/>
+      <c r="G103" s="24"/>
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
@@ -6845,7 +6872,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B104,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G104" s="39"/>
+      <c r="G104" s="25"/>
       <c r="H104" s="8"/>
       <c r="I104" s="8"/>
       <c r="J104" s="8"/>
@@ -6874,7 +6901,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B105,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G105" s="38"/>
+      <c r="G105" s="24"/>
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
@@ -6903,7 +6930,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B106,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G106" s="39"/>
+      <c r="G106" s="25"/>
       <c r="H106" s="8"/>
       <c r="I106" s="8"/>
       <c r="J106" s="8"/>
@@ -6932,7 +6959,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B107,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G107" s="38"/>
+      <c r="G107" s="24"/>
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
@@ -6961,7 +6988,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B108,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G108" s="39"/>
+      <c r="G108" s="25"/>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
       <c r="J108" s="8"/>
@@ -6990,7 +7017,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B109,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G109" s="38"/>
+      <c r="G109" s="24"/>
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
@@ -7019,7 +7046,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B110,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G110" s="39"/>
+      <c r="G110" s="25"/>
       <c r="H110" s="8"/>
       <c r="I110" s="8"/>
       <c r="J110" s="8"/>
@@ -7048,7 +7075,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B111,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G111" s="38"/>
+      <c r="G111" s="24"/>
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
@@ -7077,7 +7104,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B112,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G112" s="39"/>
+      <c r="G112" s="25"/>
       <c r="H112" s="8"/>
       <c r="I112" s="8"/>
       <c r="J112" s="8"/>
@@ -7106,7 +7133,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B113,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G113" s="38"/>
+      <c r="G113" s="24"/>
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
@@ -7135,7 +7162,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B114,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G114" s="39"/>
+      <c r="G114" s="25"/>
       <c r="H114" s="8"/>
       <c r="I114" s="8"/>
       <c r="J114" s="8"/>
@@ -7164,7 +7191,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B115,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G115" s="38"/>
+      <c r="G115" s="24"/>
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
@@ -7193,7 +7220,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B116,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G116" s="39"/>
+      <c r="G116" s="25"/>
       <c r="H116" s="8"/>
       <c r="I116" s="8"/>
       <c r="J116" s="8"/>
@@ -7222,7 +7249,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B117,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G117" s="38"/>
+      <c r="G117" s="24"/>
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
@@ -7251,7 +7278,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B118,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G118" s="39"/>
+      <c r="G118" s="25"/>
       <c r="H118" s="8"/>
       <c r="I118" s="8"/>
       <c r="J118" s="8"/>
@@ -7280,7 +7307,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B119,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G119" s="38"/>
+      <c r="G119" s="24"/>
       <c r="H119" s="7"/>
       <c r="I119" s="7"/>
       <c r="J119" s="7"/>
@@ -7309,7 +7336,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B120,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G120" s="39"/>
+      <c r="G120" s="25"/>
       <c r="H120" s="8"/>
       <c r="I120" s="8"/>
       <c r="J120" s="8"/>
@@ -7338,7 +7365,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B121,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G121" s="38"/>
+      <c r="G121" s="24"/>
       <c r="H121" s="7"/>
       <c r="I121" s="7"/>
       <c r="J121" s="7"/>
@@ -7367,7 +7394,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B122,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G122" s="39"/>
+      <c r="G122" s="25"/>
       <c r="H122" s="8"/>
       <c r="I122" s="8"/>
       <c r="J122" s="8"/>
@@ -7396,7 +7423,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B123,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>2</v>
       </c>
-      <c r="G123" s="38"/>
+      <c r="G123" s="24"/>
       <c r="H123" s="7"/>
       <c r="I123" s="7"/>
       <c r="J123" s="7"/>
@@ -7404,7 +7431,7 @@
       <c r="L123" s="4"/>
       <c r="M123" s="4"/>
       <c r="N123" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.25">
@@ -7427,7 +7454,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B124,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G124" s="39"/>
+      <c r="G124" s="25"/>
       <c r="H124" s="8"/>
       <c r="I124" s="8"/>
       <c r="J124" s="8"/>
@@ -7456,7 +7483,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B125,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G125" s="38"/>
+      <c r="G125" s="24"/>
       <c r="H125" s="7"/>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
@@ -7485,7 +7512,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B126,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G126" s="39"/>
+      <c r="G126" s="25"/>
       <c r="H126" s="8"/>
       <c r="I126" s="8"/>
       <c r="J126" s="8"/>
@@ -7514,7 +7541,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B127,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G127" s="38"/>
+      <c r="G127" s="24"/>
       <c r="H127" s="7"/>
       <c r="I127" s="7"/>
       <c r="J127" s="7"/>
@@ -7543,7 +7570,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B128,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G128" s="39"/>
+      <c r="G128" s="25"/>
       <c r="H128" s="8"/>
       <c r="I128" s="8"/>
       <c r="J128" s="8"/>
@@ -7572,7 +7599,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B129,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G129" s="38"/>
+      <c r="G129" s="24"/>
       <c r="H129" s="7"/>
       <c r="I129" s="7"/>
       <c r="J129" s="7"/>
@@ -7601,7 +7628,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B130,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G130" s="39"/>
+      <c r="G130" s="25"/>
       <c r="H130" s="8"/>
       <c r="I130" s="8"/>
       <c r="J130" s="8"/>
@@ -7630,7 +7657,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B131,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G131" s="38"/>
+      <c r="G131" s="24"/>
       <c r="H131" s="7"/>
       <c r="I131" s="7"/>
       <c r="J131" s="7"/>
@@ -7659,7 +7686,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B132,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G132" s="39"/>
+      <c r="G132" s="25"/>
       <c r="H132" s="8"/>
       <c r="I132" s="8"/>
       <c r="J132" s="8"/>
@@ -7688,7 +7715,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B133,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G133" s="38"/>
+      <c r="G133" s="24"/>
       <c r="H133" s="7"/>
       <c r="I133" s="7"/>
       <c r="J133" s="7"/>
@@ -7717,7 +7744,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B134,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>2</v>
       </c>
-      <c r="G134" s="39"/>
+      <c r="G134" s="25"/>
       <c r="H134" s="8"/>
       <c r="I134" s="8"/>
       <c r="J134" s="8"/>
@@ -7746,7 +7773,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B135,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>4</v>
       </c>
-      <c r="G135" s="38"/>
+      <c r="G135" s="24"/>
       <c r="H135" s="7"/>
       <c r="I135" s="7"/>
       <c r="J135" s="7"/>
@@ -7775,7 +7802,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B136,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G136" s="39"/>
+      <c r="G136" s="25"/>
       <c r="H136" s="8"/>
       <c r="I136" s="8"/>
       <c r="J136" s="8"/>
@@ -7804,7 +7831,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B137,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G137" s="38"/>
+      <c r="G137" s="24"/>
       <c r="H137" s="7"/>
       <c r="I137" s="7"/>
       <c r="J137" s="7"/>
@@ -7833,7 +7860,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B138,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G138" s="39"/>
+      <c r="G138" s="25"/>
       <c r="H138" s="8"/>
       <c r="I138" s="8"/>
       <c r="J138" s="8"/>
@@ -7862,7 +7889,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B139,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G139" s="38"/>
+      <c r="G139" s="24"/>
       <c r="H139" s="7"/>
       <c r="I139" s="7"/>
       <c r="J139" s="7"/>
@@ -7891,7 +7918,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B140,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G140" s="39"/>
+      <c r="G140" s="25"/>
       <c r="H140" s="8"/>
       <c r="I140" s="8"/>
       <c r="J140" s="8"/>
@@ -7920,7 +7947,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B141,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G141" s="38"/>
+      <c r="G141" s="24"/>
       <c r="H141" s="7"/>
       <c r="I141" s="7"/>
       <c r="J141" s="7"/>
@@ -7949,7 +7976,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B142,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G142" s="39"/>
+      <c r="G142" s="25"/>
       <c r="H142" s="8"/>
       <c r="I142" s="8"/>
       <c r="J142" s="8"/>
@@ -7978,7 +8005,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B143,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G143" s="38"/>
+      <c r="G143" s="24"/>
       <c r="H143" s="7"/>
       <c r="I143" s="7"/>
       <c r="J143" s="7"/>
@@ -8007,7 +8034,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B144,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>4</v>
       </c>
-      <c r="G144" s="39"/>
+      <c r="G144" s="25"/>
       <c r="H144" s="8"/>
       <c r="I144" s="8"/>
       <c r="J144" s="8"/>
@@ -8036,7 +8063,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B145,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G145" s="38"/>
+      <c r="G145" s="24"/>
       <c r="H145" s="7"/>
       <c r="I145" s="7"/>
       <c r="J145" s="7"/>
@@ -8065,7 +8092,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B146,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G146" s="39"/>
+      <c r="G146" s="25"/>
       <c r="H146" s="8"/>
       <c r="I146" s="8"/>
       <c r="J146" s="8"/>
@@ -8094,7 +8121,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B147,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G147" s="38"/>
+      <c r="G147" s="24"/>
       <c r="H147" s="7"/>
       <c r="I147" s="7"/>
       <c r="J147" s="7"/>
@@ -8123,7 +8150,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B148,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G148" s="39"/>
+      <c r="G148" s="25"/>
       <c r="H148" s="8"/>
       <c r="I148" s="8"/>
       <c r="J148" s="8"/>
@@ -8152,7 +8179,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B149,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G149" s="38"/>
+      <c r="G149" s="24"/>
       <c r="H149" s="7"/>
       <c r="I149" s="7"/>
       <c r="J149" s="7"/>
@@ -8181,7 +8208,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B150,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G150" s="39"/>
+      <c r="G150" s="25"/>
       <c r="H150" s="8"/>
       <c r="I150" s="8"/>
       <c r="J150" s="8"/>
@@ -8210,7 +8237,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B151,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G151" s="38"/>
+      <c r="G151" s="24"/>
       <c r="H151" s="7"/>
       <c r="I151" s="7"/>
       <c r="J151" s="7"/>
@@ -8218,7 +8245,7 @@
       <c r="L151" s="4"/>
       <c r="M151" s="4"/>
       <c r="N151" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
@@ -8241,7 +8268,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B152,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G152" s="39"/>
+      <c r="G152" s="25"/>
       <c r="H152" s="8"/>
       <c r="I152" s="8"/>
       <c r="J152" s="8"/>
@@ -8270,7 +8297,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B153,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G153" s="38"/>
+      <c r="G153" s="24"/>
       <c r="H153" s="7"/>
       <c r="I153" s="7"/>
       <c r="J153" s="7"/>
@@ -8299,7 +8326,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B154,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G154" s="39"/>
+      <c r="G154" s="25"/>
       <c r="H154" s="8"/>
       <c r="I154" s="8"/>
       <c r="J154" s="8"/>
@@ -8328,7 +8355,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B155,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G155" s="38"/>
+      <c r="G155" s="24"/>
       <c r="H155" s="7"/>
       <c r="I155" s="7"/>
       <c r="J155" s="7"/>
@@ -8357,7 +8384,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B156,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
-      <c r="G156" s="39"/>
+      <c r="G156" s="25"/>
       <c r="H156" s="8"/>
       <c r="I156" s="8"/>
       <c r="J156" s="8"/>
@@ -8386,7 +8413,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B157,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G157" s="38"/>
+      <c r="G157" s="24"/>
       <c r="H157" s="7"/>
       <c r="I157" s="7"/>
       <c r="J157" s="7"/>
@@ -8415,7 +8442,7 @@
         <f>_xlfn.IFNA(VLOOKUP(B158,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G158" s="39"/>
+      <c r="G158" s="25"/>
       <c r="H158" s="8"/>
       <c r="I158" s="8"/>
       <c r="J158" s="8"/>
@@ -8481,42 +8508,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="31" t="s">
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="37" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -8544,7 +8571,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="32"/>
+      <c r="O2" s="38"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -29948,16 +29975,16 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="43">
+      <c r="A72" s="29">
         <v>213</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="B72" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="C72" s="43" t="s">
+      <c r="C72" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="D72" s="43">
+      <c r="D72" s="29">
         <v>2</v>
       </c>
     </row>
@@ -30587,7 +30614,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529EAA4D-3610-4D91-B7A8-8EE8CE665350}">
   <dimension ref="A1:D547"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -34364,30 +34393,30 @@
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A270" s="43">
+      <c r="A270" s="29">
         <v>213</v>
       </c>
-      <c r="B270" s="43" t="s">
+      <c r="B270" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="C270" s="43" t="s">
+      <c r="C270" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="D270" s="43" t="s">
+      <c r="D270" s="29" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A271" s="43">
+      <c r="A271" s="29">
         <v>213</v>
       </c>
-      <c r="B271" s="43" t="s">
+      <c r="B271" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="C271" s="43" t="s">
+      <c r="C271" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="D271" s="43" t="s">
+      <c r="D271" s="29" t="s">
         <v>722</v>
       </c>
     </row>
@@ -38253,6 +38282,54 @@
       </c>
       <c r="D547" t="s">
         <v>961</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27D949D-A68D-494C-A22F-69E09E6E483C}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>974</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>972</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>973</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2">
+        <v>90</v>
+      </c>
+      <c r="C2">
+        <v>8814011</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se ajusto la funcion Tcampo_reg, se agrego validaciones el retorno de valores, se aplica cambios en plan de trabajo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE8C18F-6B51-4E25-88F6-1B2BBB44DB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BB2B1C-CD7F-4F2F-959A-EC53B7A99A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6018" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6019" uniqueCount="978">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3734,9 +3734,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N33" sqref="N33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4741,15 +4741,21 @@
         <f>_xlfn.IFNA(VLOOKUP(B31,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G31" s="24"/>
-      <c r="H31" s="7"/>
+      <c r="G31" s="24">
+        <v>45797</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>376</v>
+      </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="M31" s="4"/>
+      <c r="M31" s="4">
+        <v>7760421</v>
+      </c>
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -10714,7 +10720,7 @@
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>68</v>
       </c>
@@ -25806,7 +25812,7 @@
       <c r="N521" s="7"/>
       <c r="O521" s="7"/>
     </row>
-    <row r="522" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A522" s="8">
         <v>520</v>
       </c>
@@ -26644,7 +26650,7 @@
       <c r="N547" s="8"/>
       <c r="O547" s="8"/>
     </row>
-    <row r="548" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A548" s="7">
         <v>546</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion de plan de trabajo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITEXTENSIONS\Spooler_newww\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BB2B1C-CD7F-4F2F-959A-EC53B7A99A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C124F6C6-0F06-4D02-B255-1A0FE7A3C6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6019" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6023" uniqueCount="980">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3088,6 +3088,13 @@
   </si>
   <si>
     <t>29/05/2025: Se inicia con el analisis del módulo para poder migrarlo</t>
+  </si>
+  <si>
+    <t>12/05/2025: Se inicia desarrollo del módulo.
+29/05/2025: Se termina el desarrollo en ambiente local.</t>
+  </si>
+  <si>
+    <t>02/06/2025: Se inicia desarrollo del módulo.</t>
   </si>
 </sst>
 </file>
@@ -3734,9 +3741,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:N158"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4208,7 +4215,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -4228,16 +4235,24 @@
         <f>_xlfn.IFNA(VLOOKUP(B14,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>66</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="25">
+        <v>45789</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>376</v>
+      </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="6" t="s">
         <v>967</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="5"/>
+      <c r="M14" s="6">
+        <v>8389847</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>978</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -4625,14 +4640,20 @@
         <f>_xlfn.IFNA(VLOOKUP(B27,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>16</v>
       </c>
-      <c r="G27" s="24"/>
+      <c r="G27" s="24">
+        <v>45810</v>
+      </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
-      <c r="L27" s="4"/>
+      <c r="L27" s="4" t="s">
+        <v>967</v>
+      </c>
       <c r="M27" s="4"/>
-      <c r="N27" s="3"/>
+      <c r="N27" s="3" t="s">
+        <v>979</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -10720,7 +10741,7 @@
       <c r="N69" s="7"/>
       <c r="O69" s="7"/>
     </row>
-    <row r="70" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>68</v>
       </c>
@@ -25812,7 +25833,7 @@
       <c r="N521" s="7"/>
       <c r="O521" s="7"/>
     </row>
-    <row r="522" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A522" s="8">
         <v>520</v>
       </c>
@@ -26650,7 +26671,7 @@
       <c r="N547" s="8"/>
       <c r="O547" s="8"/>
     </row>
-    <row r="548" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A548" s="7">
         <v>546</v>
       </c>

</xml_diff>

<commit_message>
Se agrega un reporte Bajo Demanda que no se había identificado antes.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITEXTENSIONS\Spooler_newww\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C124F6C6-0F06-4D02-B255-1A0FE7A3C6F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AC87D0-A0F5-4F41-8619-B2EC53BAD709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6023" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6028" uniqueCount="984">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3095,6 +3095,18 @@
   </si>
   <si>
     <t>02/06/2025: Se inicia desarrollo del módulo.</t>
+  </si>
+  <si>
+    <t>Supplier Invoice</t>
+  </si>
+  <si>
+    <t>supp_inv</t>
+  </si>
+  <si>
+    <t>30/05/2025 13:14 - Se detectó su ejecución en el módulo de prioridades; como correo de notificación se tiene a 'carlosrao@logis.com.mx'.</t>
+  </si>
+  <si>
+    <t>Desconocido</t>
   </si>
 </sst>
 </file>
@@ -3176,7 +3188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -3277,11 +3289,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thick">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3409,6 +3436,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3739,11 +3796,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
-  <dimension ref="A1:N158"/>
+  <dimension ref="A1:N159"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="2" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8449,34 +8506,64 @@
       <c r="M157" s="4"/>
       <c r="N157" s="3"/>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A158" s="5">
+    <row r="158" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="44">
         <v>155</v>
       </c>
-      <c r="B158" s="5">
+      <c r="B158" s="44">
         <v>304</v>
       </c>
-      <c r="C158" s="5" t="s">
+      <c r="C158" s="44" t="s">
         <v>340</v>
       </c>
-      <c r="D158" s="5" t="s">
+      <c r="D158" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="E158" s="5" t="s">
+      <c r="E158" s="44" t="s">
         <v>509</v>
       </c>
-      <c r="F158" s="19">
+      <c r="F158" s="45">
         <f>_xlfn.IFNA(VLOOKUP(B158,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G158" s="25"/>
-      <c r="H158" s="8"/>
-      <c r="I158" s="8"/>
-      <c r="J158" s="8"/>
-      <c r="K158" s="8"/>
-      <c r="L158" s="6"/>
-      <c r="M158" s="6"/>
-      <c r="N158" s="5"/>
+      <c r="G158" s="46"/>
+      <c r="H158" s="47"/>
+      <c r="I158" s="47"/>
+      <c r="J158" s="47"/>
+      <c r="K158" s="47"/>
+      <c r="L158" s="48"/>
+      <c r="M158" s="48"/>
+      <c r="N158" s="44"/>
+    </row>
+    <row r="159" spans="1:14" ht="24.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="49">
+        <v>156</v>
+      </c>
+      <c r="B159" s="49">
+        <v>25</v>
+      </c>
+      <c r="C159" s="49" t="s">
+        <v>980</v>
+      </c>
+      <c r="D159" s="49" t="s">
+        <v>981</v>
+      </c>
+      <c r="E159" s="49" t="s">
+        <v>509</v>
+      </c>
+      <c r="F159" s="50" t="s">
+        <v>983</v>
+      </c>
+      <c r="G159" s="51"/>
+      <c r="H159" s="52"/>
+      <c r="I159" s="52"/>
+      <c r="J159" s="52"/>
+      <c r="K159" s="52"/>
+      <c r="L159" s="53"/>
+      <c r="M159" s="53"/>
+      <c r="N159" s="49" t="s">
+        <v>982</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:N158" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>

</xml_diff>

<commit_message>
se actualiza archivo de seguimiento
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AC87D0-A0F5-4F41-8619-B2EC53BAD709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AABD90-BFA9-4E3D-A42E-6829EA8C6722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6028" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6023" uniqueCount="980">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3095,18 +3095,6 @@
   </si>
   <si>
     <t>02/06/2025: Se inicia desarrollo del módulo.</t>
-  </si>
-  <si>
-    <t>Supplier Invoice</t>
-  </si>
-  <si>
-    <t>supp_inv</t>
-  </si>
-  <si>
-    <t>30/05/2025 13:14 - Se detectó su ejecución en el módulo de prioridades; como correo de notificación se tiene a 'carlosrao@logis.com.mx'.</t>
-  </si>
-  <si>
-    <t>Desconocido</t>
   </si>
 </sst>
 </file>
@@ -3395,6 +3383,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3436,36 +3454,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3799,8 +3787,8 @@
   <dimension ref="A1:N159"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3821,51 +3809,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="41" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="47" t="s">
         <v>505</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="47" t="s">
         <v>506</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="49" t="s">
         <v>964</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="43" t="s">
         <v>369</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="31" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="41" t="s">
         <v>381</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="45" t="s">
         <v>502</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="40" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="40"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="9" t="s">
         <v>370</v>
       </c>
@@ -3878,9 +3866,9 @@
       <c r="K2" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="30"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -8507,63 +8495,51 @@
       <c r="N157" s="3"/>
     </row>
     <row r="158" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="44">
+      <c r="A158" s="30">
         <v>155</v>
       </c>
-      <c r="B158" s="44">
+      <c r="B158" s="30">
         <v>304</v>
       </c>
-      <c r="C158" s="44" t="s">
+      <c r="C158" s="30" t="s">
         <v>340</v>
       </c>
-      <c r="D158" s="44" t="s">
+      <c r="D158" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="E158" s="44" t="s">
+      <c r="E158" s="30" t="s">
         <v>509</v>
       </c>
-      <c r="F158" s="45">
+      <c r="F158" s="31">
         <f>_xlfn.IFNA(VLOOKUP(B158,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G158" s="46"/>
-      <c r="H158" s="47"/>
-      <c r="I158" s="47"/>
-      <c r="J158" s="47"/>
-      <c r="K158" s="47"/>
-      <c r="L158" s="48"/>
-      <c r="M158" s="48"/>
-      <c r="N158" s="44"/>
-    </row>
-    <row r="159" spans="1:14" ht="24.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="49">
+      <c r="G158" s="32"/>
+      <c r="H158" s="33"/>
+      <c r="I158" s="33"/>
+      <c r="J158" s="33"/>
+      <c r="K158" s="33"/>
+      <c r="L158" s="34"/>
+      <c r="M158" s="34"/>
+      <c r="N158" s="30"/>
+    </row>
+    <row r="159" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="35">
         <v>156</v>
       </c>
-      <c r="B159" s="49">
-        <v>25</v>
-      </c>
-      <c r="C159" s="49" t="s">
-        <v>980</v>
-      </c>
-      <c r="D159" s="49" t="s">
-        <v>981</v>
-      </c>
-      <c r="E159" s="49" t="s">
-        <v>509</v>
-      </c>
-      <c r="F159" s="50" t="s">
-        <v>983</v>
-      </c>
-      <c r="G159" s="51"/>
-      <c r="H159" s="52"/>
-      <c r="I159" s="52"/>
-      <c r="J159" s="52"/>
-      <c r="K159" s="52"/>
-      <c r="L159" s="53"/>
-      <c r="M159" s="53"/>
-      <c r="N159" s="49" t="s">
-        <v>982</v>
-      </c>
+      <c r="B159" s="35"/>
+      <c r="C159" s="35"/>
+      <c r="D159" s="35"/>
+      <c r="E159" s="35"/>
+      <c r="F159" s="36"/>
+      <c r="G159" s="37"/>
+      <c r="H159" s="38"/>
+      <c r="I159" s="38"/>
+      <c r="J159" s="38"/>
+      <c r="K159" s="38"/>
+      <c r="L159" s="39"/>
+      <c r="M159" s="39"/>
+      <c r="N159" s="35"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:N158" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
@@ -8622,42 +8598,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="47" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="37" t="s">
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="47" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -8685,7 +8661,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="38"/>
+      <c r="O2" s="48"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7">

</xml_diff>

<commit_message>
se actualizo las funciones CrearExcel_filen de la clase de Excel y abc_cel de la clase Utilerias, se comentaron los mensajes y se actualizo el plan de trabajo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AABD90-BFA9-4E3D-A42E-6829EA8C6722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6701AD-C7A9-4EF4-896E-E84CADD1837F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6023" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6025" uniqueCount="981">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3095,6 +3095,9 @@
   </si>
   <si>
     <t>02/06/2025: Se inicia desarrollo del módulo.</t>
+  </si>
+  <si>
+    <t>31/05/2025: Se inicia desarrollo del módulo., se realiza pruebas en servidor de desarrollo</t>
   </si>
 </sst>
 </file>
@@ -3787,8 +3790,8 @@
   <dimension ref="A1:N159"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4783,11 +4786,13 @@
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="6"/>
+      <c r="L30" s="6" t="s">
+        <v>498</v>
+      </c>
       <c r="M30" s="6"/>
       <c r="N30" s="5"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="24" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -4822,7 +4827,9 @@
       <c r="M31" s="4">
         <v>7760421</v>
       </c>
-      <c r="N31" s="3"/>
+      <c r="N31" s="3" t="s">
+        <v>980</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -4912,7 +4919,9 @@
         <f>_xlfn.IFNA(VLOOKUP(B34,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G34" s="25"/>
+      <c r="G34" s="25">
+        <v>45811</v>
+      </c>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>

</xml_diff>

<commit_message>
Se actualiza Plan de Trabajo, se inicia con el módulo Talones con Seguro y se agregan SP´s utilizados en los procesos que he realizado.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITEXTENSIONS\Spooler_newww\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\Migracion Spooler\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC751F9-4FBC-4C24-B150-93D47901E81F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED45B243-9B49-4D34-99FA-CD992DE8EA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6036" uniqueCount="987">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6041" uniqueCount="991">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3087,10 +3087,6 @@
   </si>
   <si>
     <t xml:space="preserve">NOMBRE </t>
-  </si>
-  <si>
-    <t xml:space="preserve">08/05/2025: Se empieza con el analisis y se empezaron a sacar las consultas
-</t>
   </si>
   <si>
     <t>29/05/2025: Se inicia con el analisis del módulo para poder migrarlo</t>
@@ -3127,13 +3123,42 @@
     <t>P_DAT_SFTP_ACCESOS_CLI
 P_DAT_EVIDENCIAS_CLIENTE
 P_INS_STATUS_EVIDENCIA_BITA</t>
+  </si>
+  <si>
+    <t>08/05/2025: Se empieza con el analisis y se empezaron a sacar las consultas
+02/06/2025: Se sube a repositorio y se hace una prueba desde el servidor</t>
+  </si>
+  <si>
+    <t>SC_RS.SPG_RS_DIST_FACTURAS_PEND_ORI.P_DAT_EVIDENCIAS_TOTAL
+SC_RS.SPG_RS_DIST_FACTURAS_PEND_ORI.P_DAT_HASTA_ENTRE_TOTAL</t>
+  </si>
+  <si>
+    <t>SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_SCAN_ENTRA_CLI_A
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_SCAN_ENTRA_CLI_B
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_SIN_DAT_LOGISTICO
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_SIN_CONVERTIDOR
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_TRANSF_DOC_A_CTRL_DOC
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_CONV_NO_VALIDADO
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_ARMADO_DOC_MANIF_CONV
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_CONV_SIN_EXP
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_ENSOBRENTADO_DOC_EXP
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_TRA_DOC_CONV_CRTL_DOC
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_TRAS_POR_RECIBIR
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_CONV_POR_CERRAR
+SC_RS_DIST.SPG_RS_DIST_DOC_LTL_PEND_SCAN.P_DAT_MERC_CONV_POR_IMPRIM</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>04/06/2025: Se inicia con el analisis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3174,12 +3199,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3451,6 +3470,12 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3465,12 +3490,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3827,9 +3846,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:O161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3847,20 +3866,20 @@
     <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" customWidth="1"/>
     <col min="14" max="14" width="80.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="80.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="46" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="47" t="s">
@@ -3872,30 +3891,30 @@
       <c r="G1" s="49" t="s">
         <v>964</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="45" t="s">
         <v>369</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="41" t="s">
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="43" t="s">
         <v>381</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="40" t="s">
         <v>502</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="N1" s="42" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="45" t="s">
-        <v>985</v>
+      <c r="O1" s="40" t="s">
+        <v>984</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="48"/>
       <c r="F2" s="48"/>
       <c r="G2" s="50"/>
@@ -3911,10 +3930,10 @@
       <c r="K2" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="46"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -4279,7 +4298,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="36" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -4315,7 +4334,9 @@
       <c r="N13" s="3" t="s">
         <v>966</v>
       </c>
-      <c r="O13" s="4"/>
+      <c r="O13" s="3" t="s">
+        <v>987</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="36" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -4353,10 +4374,10 @@
         <v>8389847</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -4699,7 +4720,7 @@
       </c>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" ht="24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="156" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -4733,9 +4754,11 @@
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="5" t="s">
-        <v>975</v>
-      </c>
-      <c r="O26" s="6"/>
+        <v>986</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>988</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -4745,10 +4768,10 @@
         <v>352</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>981</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>982</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>509</v>
@@ -4776,10 +4799,10 @@
         <v>353</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>509</v>
@@ -4799,7 +4822,7 @@
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="5" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="O28" s="6"/>
     </row>
@@ -4833,7 +4856,7 @@
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="O29" s="4"/>
     </row>
@@ -4965,7 +4988,7 @@
         <v>7760421</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="O33" s="4"/>
     </row>
@@ -5005,7 +5028,7 @@
         <v>129887</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="O34" s="5"/>
     </row>
@@ -5029,14 +5052,22 @@
         <f>_xlfn.IFNA(VLOOKUP(B35,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G35" s="24"/>
-      <c r="H35" s="7"/>
+      <c r="G35" s="24">
+        <v>45812</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>989</v>
+      </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="4"/>
+      <c r="L35" s="4" t="s">
+        <v>965</v>
+      </c>
       <c r="M35" s="4"/>
-      <c r="N35" s="3"/>
+      <c r="N35" s="3" t="s">
+        <v>990</v>
+      </c>
       <c r="O35" s="4"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Plan de trabajo, se agregaron en la columna de SP de los modulos terminado, los sp que utilizan
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\Migracion Spooler\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED45B243-9B49-4D34-99FA-CD992DE8EA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDD3795-61B4-4A4B-B138-43F61989CED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Reportes No Frecuentes" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$N$160</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$N$161</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$2:$O$630</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Detalle_Activos!$A$1:$D$651</definedName>
   </definedNames>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6041" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6049" uniqueCount="998">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3094,9 +3094,6 @@
   <si>
     <t>12/05/2025: Se inicia desarrollo del módulo.
 29/05/2025: Se termina el desarrollo en ambiente local.</t>
-  </si>
-  <si>
-    <t>31/05/2025: Se inicia desarrollo del módulo., se realiza pruebas en servidor de desarrollo</t>
   </si>
   <si>
     <t>02/06/2025: Se inicia desarrollo del módulo. (el proceso se dividirá en dos partes: cargos y envíos).</t>
@@ -3152,6 +3149,37 @@
   </si>
   <si>
     <t>04/06/2025: Se inicia con el analisis</t>
+  </si>
+  <si>
+    <t>SC_RS.SPG_RS_DIST.P_RS_GSK_PEDIMENTOS</t>
+  </si>
+  <si>
+    <t>SC_RS.SPG_RS_DIST.P_RS_PORTEOS_TLN</t>
+  </si>
+  <si>
+    <t>SC_RS.SPG_RS_DIST_DAF_REPORTES.P_DAT_RESUMEN_CLIENTES_BIM,
+SC_RS.SPG_RS_DIST_DAF_REPORTES.P_DAT_RESUMEN_CLIENTES_MES,
+SC_RS.SPG_RS_DIST_DAF_REPORTES.P_DAT_RESUMEN_CLIENTES_MAS_FIN,
+SC_RS.SPG_RS_DIST_DAF_REPORTES.P_DAT_RESUMEN_CLIENTES,
+SC_RS.SPG_RS_DIST_DAF_REPORTES.P_DAT_RESUMEN_FOLIOS,
+SC_RS.SPG_RS_DIST_DAF_REPORTES.P_DAT_FOLIOS</t>
+  </si>
+  <si>
+    <t>SC_RS.SPG_RS_DIST_DAF_REPORTES.P_DAT_FONDO_FIJO,
+SC_DIST.SPG_RS_COEX.P_OBTEN_INGR_EGRE_PEN_FACT</t>
+  </si>
+  <si>
+    <t>SC_DIST.SPG_DIST_DOC_NUI_RESERVA.P_DAT_RESERVACION_LTL</t>
+  </si>
+  <si>
+    <t>SC_DIST.SPG_DIST_DOC_NUI_RESERVA.P_DAT_RESERVACION_CD</t>
+  </si>
+  <si>
+    <t>SC_RS.SPG_RS_DIST_TRAD_LISTA_CITAS.P_DAT_TRADING_CITAS_RESUMEN,
+SC_RS.SPG_RS_DIST_TRAD_LISTA_CITAS.P_DAT_TRADING_CITAS</t>
+  </si>
+  <si>
+    <t>20/05/2025: Se inicia desarrollo del módulo.,31/05/2025:  se realiza pruebas en servidor de desarrollo, se finaliza</t>
   </si>
 </sst>
 </file>
@@ -3846,9 +3874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:O161"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3907,7 +3935,7 @@
         <v>374</v>
       </c>
       <c r="O1" s="40" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -4008,7 +4036,9 @@
         <v>3723307</v>
       </c>
       <c r="N4" s="5"/>
-      <c r="O4" s="6"/>
+      <c r="O4" s="5" t="s">
+        <v>990</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -4046,9 +4076,11 @@
         <v>6651805</v>
       </c>
       <c r="N5" s="3"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O5" s="3" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="72" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -4084,9 +4116,11 @@
         <v>4220496</v>
       </c>
       <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O6" s="5" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -4122,7 +4156,9 @@
         <v>5566768</v>
       </c>
       <c r="N7" s="3"/>
-      <c r="O7" s="4"/>
+      <c r="O7" s="3" t="s">
+        <v>993</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -4160,7 +4196,9 @@
         <v>5545714</v>
       </c>
       <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="5" t="s">
+        <v>994</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -4198,7 +4236,9 @@
         <v>7774047</v>
       </c>
       <c r="N9" s="3"/>
-      <c r="O9" s="4"/>
+      <c r="O9" s="3" t="s">
+        <v>995</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -4236,7 +4276,9 @@
         <v>7864811</v>
       </c>
       <c r="N10" s="5"/>
-      <c r="O10" s="6"/>
+      <c r="O10" s="5" t="s">
+        <v>994</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -4298,7 +4340,7 @@
       <c r="N12" s="5"/>
       <c r="O12" s="6"/>
     </row>
-    <row r="13" spans="1:15" ht="36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -4335,7 +4377,7 @@
         <v>966</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="36" x14ac:dyDescent="0.25">
@@ -4377,7 +4419,7 @@
         <v>976</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -4754,10 +4796,10 @@
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="5" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -4768,10 +4810,10 @@
         <v>352</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>979</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>980</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>981</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>509</v>
@@ -4799,10 +4841,10 @@
         <v>353</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>509</v>
@@ -4822,7 +4864,7 @@
       </c>
       <c r="M28" s="6"/>
       <c r="N28" s="5" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="O28" s="6"/>
     </row>
@@ -4856,7 +4898,7 @@
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="O29" s="4"/>
     </row>
@@ -4952,7 +4994,7 @@
       <c r="N32" s="5"/>
       <c r="O32" s="6"/>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -4988,9 +5030,11 @@
         <v>7760421</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>977</v>
-      </c>
-      <c r="O33" s="4"/>
+        <v>997</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>996</v>
+      </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
@@ -5056,7 +5100,7 @@
         <v>45812</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -5066,7 +5110,7 @@
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="O35" s="4"/>
     </row>
@@ -8848,7 +8892,7 @@
       <c r="O161" s="39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N160" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
+  <autoFilter ref="A2:N161" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N160">
     <sortCondition ref="I4:I160"/>
     <sortCondition ref="H4:H160"/>

</xml_diff>

<commit_message>
Se actualiza el Plan de trabajo integrando observaciones y seguimiento de procesos que no se deben considerar en ésta Migración.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDD3795-61B4-4A4B-B138-43F61989CED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4454EE7-FE51-4F33-85DD-3CB818C1E333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Reportes No Frecuentes" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$N$161</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Concentrado!$A$2:$N$160</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$2:$O$630</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Detalle_Activos!$A$1:$D$651</definedName>
   </definedNames>
@@ -104,7 +104,7 @@
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
-    Nombre de la persona que migró el módulo.</t>
+    ID_CRON con el que se puede probar el proceso una vez que se terminó de Migrar.</t>
       </text>
     </comment>
     <comment ref="N1" authorId="6" shapeId="0" xr:uid="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6049" uniqueCount="998">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6103" uniqueCount="999">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3109,9 +3109,6 @@
   </si>
   <si>
     <t>talones_envio</t>
-  </si>
-  <si>
-    <t>Pendiente de confirmacion por el usuario …</t>
   </si>
   <si>
     <t>SP´s</t>
@@ -3180,6 +3177,13 @@
   </si>
   <si>
     <t>20/05/2025: Se inicia desarrollo del módulo.,31/05/2025:  se realiza pruebas en servidor de desarrollo, se finaliza</t>
+  </si>
+  <si>
+    <t>ÉSTE PROCESO SE MIGRÓ AL NUEVO PORTAL WEB</t>
+  </si>
+  <si>
+    <t>Pendiente de confirmacion por el usuario …
+06/06/2025: Como se comentó, se van a migrar los tres procesos que están incluidos en éste, toda vez que el área de negocio no ha confirmado cuál de ellos utiliza y cuál de ellos ya no les es funcional.</t>
   </si>
 </sst>
 </file>
@@ -3261,7 +3265,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -3362,26 +3366,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="9"/>
-      </left>
-      <right style="thin">
-        <color theme="9"/>
-      </right>
-      <top style="thick">
-        <color theme="9"/>
-      </top>
-      <bottom style="thin">
-        <color theme="9"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3483,21 +3472,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3539,6 +3513,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3847,7 +3845,7 @@
     <text>Nombre de la persona que migró el módulo.</text>
   </threadedComment>
   <threadedComment ref="M1" dT="2025-04-23T23:38:33.71" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{38372124-5616-401A-B40A-476DE7B44D8B}">
-    <text>Nombre de la persona que migró el módulo.</text>
+    <text>ID_CRON con el que se puede probar el proceso una vez que se terminó de Migrar.</text>
   </threadedComment>
   <threadedComment ref="N1" dT="2025-04-23T23:38:58.34" personId="{17A92D77-750E-4356-B72E-04E536E71984}" id="{11C6CB88-DB2E-466E-B609-ED6D3F57F8FC}">
     <text>Observaciones o comentarios que se consideren importantes al migrar un módulo.</text>
@@ -3872,11 +3870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
-  <dimension ref="A1:O161"/>
+  <dimension ref="A1:O160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N38" sqref="N38"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3898,54 +3896,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="42" t="s">
         <v>505</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="42" t="s">
         <v>506</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="44" t="s">
         <v>964</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="40" t="s">
         <v>369</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="43" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="38" t="s">
         <v>381</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="35" t="s">
         <v>502</v>
       </c>
-      <c r="N1" s="42" t="s">
+      <c r="N1" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="40" t="s">
-        <v>983</v>
+      <c r="O1" s="35" t="s">
+        <v>982</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="50"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="45"/>
       <c r="H2" s="9" t="s">
         <v>370</v>
       </c>
@@ -3958,16 +3956,16 @@
       <c r="K2" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="41"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="36"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="17">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="17">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -4001,10 +3999,10 @@
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="19">
         <v>1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="19">
         <v>336</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -4037,14 +4035,14 @@
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="17">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="17">
         <v>337</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4056,7 +4054,7 @@
       <c r="E5" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B5,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4077,14 +4075,14 @@
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="72" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="19">
         <v>3</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="19">
         <v>329</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -4117,14 +4115,14 @@
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="17">
         <v>4</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="17">
         <v>330</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -4136,7 +4134,7 @@
       <c r="E7" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B7,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4157,14 +4155,14 @@
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="19">
         <v>5</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="19">
         <v>196</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -4197,14 +4195,14 @@
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="17">
         <v>6</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="17">
         <v>334</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -4216,7 +4214,7 @@
       <c r="E9" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F9" s="19">
+      <c r="F9" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B9,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4237,14 +4235,14 @@
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="19">
         <v>7</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="19">
         <v>335</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -4277,14 +4275,14 @@
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="17">
         <v>8</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="17">
         <v>183</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -4296,7 +4294,7 @@
       <c r="E11" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B11,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4311,10 +4309,10 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="19">
         <v>9</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="19">
         <v>108</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -4341,10 +4339,10 @@
       <c r="O12" s="6"/>
     </row>
     <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="17">
         <v>10</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="17">
         <v>106</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -4356,7 +4354,7 @@
       <c r="E13" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B13,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4377,14 +4375,14 @@
         <v>966</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="36" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="19">
         <v>11</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="19">
         <v>351</v>
       </c>
       <c r="C14" s="5" t="s">
@@ -4419,14 +4417,14 @@
         <v>976</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="17">
         <v>12</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="17">
         <v>102</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -4438,175 +4436,283 @@
       <c r="E15" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B15,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="4"/>
+      <c r="G15" s="51" t="s">
+        <v>507</v>
+      </c>
+      <c r="H15" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="J15" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="K15" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="L15" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="M15" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="N15" s="20" t="s">
+        <v>997</v>
+      </c>
+      <c r="O15" s="52" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="49">
         <v>13</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="49">
         <v>102</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="23" t="s">
         <v>482</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="23" t="s">
         <v>483</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="23" t="s">
         <v>509</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="49">
         <f>_xlfn.IFNA(VLOOKUP(B16,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G16" s="25"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
+      <c r="G16" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="I16" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="J16" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="K16" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="L16" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="M16" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>997</v>
+      </c>
+      <c r="O16" s="50" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="54">
         <v>14</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="54">
         <v>102</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="F17" s="19">
+      <c r="F17" s="54">
         <f>_xlfn.IFNA(VLOOKUP(B17,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G17" s="24"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="4"/>
+      <c r="G17" s="51" t="s">
+        <v>507</v>
+      </c>
+      <c r="H17" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="I17" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="J17" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="K17" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="L17" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="M17" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="N17" s="20" t="s">
+        <v>997</v>
+      </c>
+      <c r="O17" s="52" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="49">
         <v>15</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="49">
         <v>102</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="23" t="s">
         <v>486</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="23" t="s">
         <v>509</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="49">
         <f>_xlfn.IFNA(VLOOKUP(B18,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
+      <c r="G18" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="H18" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="I18" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="J18" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="K18" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="L18" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="M18" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="N18" s="23" t="s">
+        <v>997</v>
+      </c>
+      <c r="O18" s="50" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="54">
         <v>16</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="54">
         <v>102</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="20" t="s">
         <v>488</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="20" t="s">
         <v>489</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="F19" s="19">
+      <c r="F19" s="54">
         <f>_xlfn.IFNA(VLOOKUP(B19,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="4"/>
+      <c r="G19" s="51" t="s">
+        <v>507</v>
+      </c>
+      <c r="H19" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="I19" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="J19" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="K19" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="L19" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="M19" s="52" t="s">
+        <v>507</v>
+      </c>
+      <c r="N19" s="20" t="s">
+        <v>997</v>
+      </c>
+      <c r="O19" s="52" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="49">
         <v>17</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="49">
         <v>341</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="23" t="s">
         <v>476</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="23" t="s">
         <v>509</v>
       </c>
-      <c r="F20" s="19">
+      <c r="F20" s="49">
         <f>_xlfn.IFNA(VLOOKUP(B20,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
+      <c r="G20" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="H20" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="I20" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="J20" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="K20" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="L20" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="M20" s="50" t="s">
+        <v>507</v>
+      </c>
+      <c r="N20" s="23" t="s">
+        <v>997</v>
+      </c>
+      <c r="O20" s="50" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="17">
         <v>18</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="17">
         <v>282</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -4618,7 +4724,7 @@
       <c r="E21" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B21,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4633,10 +4739,10 @@
       <c r="O21" s="4"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="19">
         <v>19</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="19">
         <v>348</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -4663,10 +4769,10 @@
       <c r="O22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="17">
         <v>20</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="17">
         <v>186</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -4678,7 +4784,7 @@
       <c r="E23" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B23,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4693,10 +4799,10 @@
       <c r="O23" s="4"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="19">
         <v>21</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="19">
         <v>347</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -4723,10 +4829,10 @@
       <c r="O24" s="6"/>
     </row>
     <row r="25" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="17">
         <v>22</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="17">
         <v>235</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -4738,7 +4844,7 @@
       <c r="E25" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B25,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4763,10 +4869,10 @@
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="1:15" ht="156" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="19">
         <v>23</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="19">
         <v>234</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -4796,17 +4902,17 @@
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="5" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="17">
         <v>24</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="17">
         <v>352</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -4818,7 +4924,7 @@
       <c r="E27" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="17">
         <v>1</v>
       </c>
       <c r="G27" s="3"/>
@@ -4834,10 +4940,10 @@
       <c r="O27" s="3"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="A28" s="19">
         <v>25</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="19">
         <v>353</v>
       </c>
       <c r="C28" s="5" t="s">
@@ -4868,11 +4974,11 @@
       </c>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+    <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
         <v>26</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="17">
         <v>80</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -4884,7 +4990,7 @@
       <c r="E29" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B29,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>16</v>
       </c>
@@ -4898,15 +5004,15 @@
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="3" t="s">
-        <v>982</v>
+        <v>998</v>
       </c>
       <c r="O29" s="4"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="A30" s="19">
         <v>27</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="19">
         <v>226</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -4933,10 +5039,10 @@
       <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="A31" s="17">
         <v>28</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="17">
         <v>89</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -4948,7 +5054,7 @@
       <c r="E31" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B31,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -4963,10 +5069,10 @@
       <c r="O31" s="4"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="A32" s="19">
         <v>29</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="19">
         <v>153</v>
       </c>
       <c r="C32" s="5" t="s">
@@ -4995,10 +5101,10 @@
       <c r="O32" s="6"/>
     </row>
     <row r="33" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="A33" s="17">
         <v>30</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="17">
         <v>159</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -5010,14 +5116,14 @@
       <c r="E33" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B33,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
       <c r="G33" s="24">
         <v>45797</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="H33" s="7" t="s">
         <v>376</v>
       </c>
       <c r="I33" s="7"/>
@@ -5030,17 +5136,17 @@
         <v>7760421</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="A34" s="19">
         <v>31</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="19">
         <v>149</v>
       </c>
       <c r="C34" s="5" t="s">
@@ -5077,10 +5183,10 @@
       <c r="O34" s="5"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+      <c r="A35" s="17">
         <v>32</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="17">
         <v>199</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -5092,7 +5198,7 @@
       <c r="E35" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F35" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B35,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5100,7 +5206,7 @@
         <v>45812</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -5110,15 +5216,15 @@
       </c>
       <c r="M35" s="4"/>
       <c r="N35" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="O35" s="4"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="A36" s="19">
         <v>33</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="19">
         <v>175</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -5149,10 +5255,10 @@
       <c r="O36" s="6"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3">
+      <c r="A37" s="55">
         <v>34</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="55">
         <v>36</v>
       </c>
       <c r="C37" s="21" t="s">
@@ -5164,7 +5270,7 @@
       <c r="E37" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="F37" s="19" t="str">
+      <c r="F37" s="55" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B37,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -5179,10 +5285,10 @@
       <c r="O37" s="16"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="A38" s="56">
         <v>35</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="56">
         <v>37</v>
       </c>
       <c r="C38" s="22" t="s">
@@ -5194,7 +5300,7 @@
       <c r="E38" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="F38" s="19" t="str">
+      <c r="F38" s="56" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B38,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -5209,10 +5315,10 @@
       <c r="O38" s="13"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+      <c r="A39" s="17">
         <v>36</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="17">
         <v>39</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -5224,7 +5330,7 @@
       <c r="E39" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B39,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>4</v>
       </c>
@@ -5239,10 +5345,10 @@
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+      <c r="A40" s="19">
         <v>37</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="19">
         <v>91</v>
       </c>
       <c r="C40" s="23" t="s">
@@ -5269,10 +5375,10 @@
       <c r="O40" s="6"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
+      <c r="A41" s="17">
         <v>38</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="17">
         <v>44</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -5284,7 +5390,7 @@
       <c r="E41" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F41" s="19">
+      <c r="F41" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B41,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5299,10 +5405,10 @@
       <c r="O41" s="4"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="A42" s="19">
         <v>39</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="19">
         <v>117</v>
       </c>
       <c r="C42" s="5" t="s">
@@ -5329,10 +5435,10 @@
       <c r="O42" s="6"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+      <c r="A43" s="17">
         <v>40</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="17">
         <v>58</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -5344,7 +5450,7 @@
       <c r="E43" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F43" s="19">
+      <c r="F43" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B43,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5359,10 +5465,10 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+      <c r="A44" s="19">
         <v>41</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="19">
         <v>62</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -5389,10 +5495,10 @@
       <c r="O44" s="6"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="A45" s="17">
         <v>42</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="17">
         <v>63</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -5404,7 +5510,7 @@
       <c r="E45" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F45" s="19">
+      <c r="F45" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B45,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5419,10 +5525,10 @@
       <c r="O45" s="4"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+      <c r="A46" s="19">
         <v>43</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="19">
         <v>60</v>
       </c>
       <c r="C46" s="5" t="s">
@@ -5449,10 +5555,10 @@
       <c r="O46" s="6"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+      <c r="A47" s="17">
         <v>44</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="17">
         <v>59</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -5464,7 +5570,7 @@
       <c r="E47" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F47" s="19">
+      <c r="F47" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B47,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5479,10 +5585,10 @@
       <c r="O47" s="4"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
+      <c r="A48" s="19">
         <v>45</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="19">
         <v>55</v>
       </c>
       <c r="C48" s="5" t="s">
@@ -5509,10 +5615,10 @@
       <c r="O48" s="6"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+      <c r="A49" s="17">
         <v>46</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="17">
         <v>61</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -5524,7 +5630,7 @@
       <c r="E49" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F49" s="19">
+      <c r="F49" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B49,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5539,10 +5645,10 @@
       <c r="O49" s="4"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
+      <c r="A50" s="19">
         <v>47</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="19">
         <v>56</v>
       </c>
       <c r="C50" s="5" t="s">
@@ -5569,10 +5675,10 @@
       <c r="O50" s="6"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
+      <c r="A51" s="17">
         <v>48</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="17">
         <v>73</v>
       </c>
       <c r="C51" s="20" t="s">
@@ -5584,7 +5690,7 @@
       <c r="E51" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F51" s="19" t="str">
+      <c r="F51" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B51,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -5599,10 +5705,10 @@
       <c r="O51" s="4"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
+      <c r="A52" s="19">
         <v>49</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="19">
         <v>57</v>
       </c>
       <c r="C52" s="5" t="s">
@@ -5629,10 +5735,10 @@
       <c r="O52" s="6"/>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
+      <c r="A53" s="17">
         <v>50</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="17">
         <v>165</v>
       </c>
       <c r="C53" s="20" t="s">
@@ -5644,7 +5750,7 @@
       <c r="E53" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F53" s="19" t="str">
+      <c r="F53" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B53,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -5659,10 +5765,10 @@
       <c r="O53" s="4"/>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
+      <c r="A54" s="19">
         <v>51</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="19">
         <v>250</v>
       </c>
       <c r="C54" s="5" t="s">
@@ -5689,10 +5795,10 @@
       <c r="O54" s="6"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
+      <c r="A55" s="17">
         <v>52</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="17">
         <v>251</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -5704,7 +5810,7 @@
       <c r="E55" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F55" s="19">
+      <c r="F55" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B55,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5719,10 +5825,10 @@
       <c r="O55" s="4"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
+      <c r="A56" s="19">
         <v>53</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="19">
         <v>107</v>
       </c>
       <c r="C56" s="5" t="s">
@@ -5749,10 +5855,10 @@
       <c r="O56" s="6"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
+      <c r="A57" s="17">
         <v>54</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="17">
         <v>288</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -5764,7 +5870,7 @@
       <c r="E57" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F57" s="19">
+      <c r="F57" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B57,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5779,10 +5885,10 @@
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
+      <c r="A58" s="19">
         <v>55</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="19">
         <v>320</v>
       </c>
       <c r="C58" s="5" t="s">
@@ -5809,10 +5915,10 @@
       <c r="O58" s="6"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
+      <c r="A59" s="17">
         <v>56</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="17">
         <v>77</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -5824,7 +5930,7 @@
       <c r="E59" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F59" s="19">
+      <c r="F59" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B59,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5839,10 +5945,10 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
+      <c r="A60" s="19">
         <v>57</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B60" s="19">
         <v>268</v>
       </c>
       <c r="C60" s="23" t="s">
@@ -5869,10 +5975,10 @@
       <c r="O60" s="6"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
+      <c r="A61" s="17">
         <v>58</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="17">
         <v>132</v>
       </c>
       <c r="C61" s="3" t="s">
@@ -5884,7 +5990,7 @@
       <c r="E61" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F61" s="19">
+      <c r="F61" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B61,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -5899,10 +6005,10 @@
       <c r="O61" s="4"/>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
+      <c r="A62" s="19">
         <v>59</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="19">
         <v>135</v>
       </c>
       <c r="C62" s="5" t="s">
@@ -5929,10 +6035,10 @@
       <c r="O62" s="6"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" s="3">
+      <c r="A63" s="17">
         <v>60</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="17">
         <v>141</v>
       </c>
       <c r="C63" s="20" t="s">
@@ -5944,7 +6050,7 @@
       <c r="E63" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F63" s="19" t="str">
+      <c r="F63" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B63,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -5959,10 +6065,10 @@
       <c r="O63" s="4"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="3">
+      <c r="A64" s="19">
         <v>61</v>
       </c>
-      <c r="B64" s="5">
+      <c r="B64" s="19">
         <v>139</v>
       </c>
       <c r="C64" s="5" t="s">
@@ -5989,10 +6095,10 @@
       <c r="O64" s="6"/>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+      <c r="A65" s="17">
         <v>62</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="17">
         <v>160</v>
       </c>
       <c r="C65" s="20" t="s">
@@ -6004,7 +6110,7 @@
       <c r="E65" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F65" s="19" t="str">
+      <c r="F65" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B65,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -6019,10 +6125,10 @@
       <c r="O65" s="4"/>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+      <c r="A66" s="19">
         <v>63</v>
       </c>
-      <c r="B66" s="5">
+      <c r="B66" s="19">
         <v>174</v>
       </c>
       <c r="C66" s="5" t="s">
@@ -6049,10 +6155,10 @@
       <c r="O66" s="6"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
+      <c r="A67" s="17">
         <v>64</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="17">
         <v>244</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -6064,7 +6170,7 @@
       <c r="E67" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F67" s="19">
+      <c r="F67" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B67,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>164</v>
       </c>
@@ -6079,10 +6185,10 @@
       <c r="O67" s="4"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="3">
+      <c r="A68" s="19">
         <v>65</v>
       </c>
-      <c r="B68" s="5">
+      <c r="B68" s="19">
         <v>318</v>
       </c>
       <c r="C68" s="5" t="s">
@@ -6109,10 +6215,10 @@
       <c r="O68" s="6"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+      <c r="A69" s="17">
         <v>66</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="17">
         <v>263</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -6124,7 +6230,7 @@
       <c r="E69" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F69" s="19">
+      <c r="F69" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B69,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6139,10 +6245,10 @@
       <c r="O69" s="4"/>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+      <c r="A70" s="19">
         <v>67</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="19">
         <v>54</v>
       </c>
       <c r="C70" s="5" t="s">
@@ -6169,10 +6275,10 @@
       <c r="O70" s="6"/>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
+      <c r="A71" s="17">
         <v>68</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="17">
         <v>53</v>
       </c>
       <c r="C71" s="20" t="s">
@@ -6184,7 +6290,7 @@
       <c r="E71" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F71" s="19" t="str">
+      <c r="F71" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B71,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -6199,10 +6305,10 @@
       <c r="O71" s="4"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A72" s="3">
+      <c r="A72" s="19">
         <v>69</v>
       </c>
-      <c r="B72" s="5">
+      <c r="B72" s="19">
         <v>49</v>
       </c>
       <c r="C72" s="5" t="s">
@@ -6229,10 +6335,10 @@
       <c r="O72" s="6"/>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="3">
+      <c r="A73" s="17">
         <v>70</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="17">
         <v>51</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -6244,7 +6350,7 @@
       <c r="E73" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F73" s="19">
+      <c r="F73" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B73,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6259,10 +6365,10 @@
       <c r="O73" s="4"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A74" s="3">
+      <c r="A74" s="19">
         <v>71</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="19">
         <v>52</v>
       </c>
       <c r="C74" s="5" t="s">
@@ -6289,10 +6395,10 @@
       <c r="O74" s="6"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="3">
+      <c r="A75" s="17">
         <v>72</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="17">
         <v>176</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -6304,7 +6410,7 @@
       <c r="E75" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F75" s="19">
+      <c r="F75" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B75,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>2</v>
       </c>
@@ -6319,10 +6425,10 @@
       <c r="O75" s="4"/>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A76" s="3">
+      <c r="A76" s="19">
         <v>73</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="19">
         <v>161</v>
       </c>
       <c r="C76" s="23" t="s">
@@ -6349,10 +6455,10 @@
       <c r="O76" s="6"/>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" s="3">
+      <c r="A77" s="17">
         <v>74</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="17">
         <v>82</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -6364,7 +6470,7 @@
       <c r="E77" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F77" s="19">
+      <c r="F77" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B77,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6379,10 +6485,10 @@
       <c r="O77" s="4"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A78" s="3">
+      <c r="A78" s="19">
         <v>75</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="19">
         <v>262</v>
       </c>
       <c r="C78" s="5" t="s">
@@ -6409,10 +6515,10 @@
       <c r="O78" s="6"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A79" s="3">
+      <c r="A79" s="17">
         <v>76</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="17">
         <v>261</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -6424,7 +6530,7 @@
       <c r="E79" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F79" s="19">
+      <c r="F79" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B79,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6439,10 +6545,10 @@
       <c r="O79" s="4"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A80" s="3">
+      <c r="A80" s="19">
         <v>77</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="19">
         <v>236</v>
       </c>
       <c r="C80" s="5" t="s">
@@ -6469,10 +6575,10 @@
       <c r="O80" s="6"/>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A81" s="3">
+      <c r="A81" s="17">
         <v>78</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="17">
         <v>256</v>
       </c>
       <c r="C81" s="20" t="s">
@@ -6484,7 +6590,7 @@
       <c r="E81" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F81" s="19" t="str">
+      <c r="F81" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B81,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -6499,10 +6605,10 @@
       <c r="O81" s="4"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="3">
+      <c r="A82" s="19">
         <v>79</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="19">
         <v>249</v>
       </c>
       <c r="C82" s="5" t="s">
@@ -6529,10 +6635,10 @@
       <c r="O82" s="6"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" s="3">
+      <c r="A83" s="17">
         <v>80</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="17">
         <v>100</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -6544,7 +6650,7 @@
       <c r="E83" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F83" s="19">
+      <c r="F83" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B83,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6559,10 +6665,10 @@
       <c r="O83" s="4"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A84" s="3">
+      <c r="A84" s="19">
         <v>81</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="19">
         <v>124</v>
       </c>
       <c r="C84" s="23" t="s">
@@ -6589,10 +6695,10 @@
       <c r="O84" s="6"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A85" s="3">
+      <c r="A85" s="17">
         <v>82</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="17">
         <v>94</v>
       </c>
       <c r="C85" s="20" t="s">
@@ -6604,7 +6710,7 @@
       <c r="E85" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F85" s="19" t="str">
+      <c r="F85" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B85,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -6619,10 +6725,10 @@
       <c r="O85" s="4"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
+      <c r="A86" s="19">
         <v>83</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="19">
         <v>315</v>
       </c>
       <c r="C86" s="5" t="s">
@@ -6649,10 +6755,10 @@
       <c r="O86" s="6"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A87" s="3">
+      <c r="A87" s="17">
         <v>84</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="17">
         <v>197</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -6664,7 +6770,7 @@
       <c r="E87" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F87" s="19">
+      <c r="F87" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B87,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6679,10 +6785,10 @@
       <c r="O87" s="4"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A88" s="3">
+      <c r="A88" s="19">
         <v>85</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B88" s="19">
         <v>109</v>
       </c>
       <c r="C88" s="23" t="s">
@@ -6709,10 +6815,10 @@
       <c r="O88" s="6"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A89" s="3">
+      <c r="A89" s="17">
         <v>86</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="17">
         <v>87</v>
       </c>
       <c r="C89" s="20" t="s">
@@ -6724,7 +6830,7 @@
       <c r="E89" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F89" s="19" t="str">
+      <c r="F89" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B89,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -6739,10 +6845,10 @@
       <c r="O89" s="4"/>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
+      <c r="A90" s="19">
         <v>87</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B90" s="19">
         <v>48</v>
       </c>
       <c r="C90" s="5" t="s">
@@ -6769,10 +6875,10 @@
       <c r="O90" s="6"/>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A91" s="3">
+      <c r="A91" s="17">
         <v>88</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="17">
         <v>78</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -6784,7 +6890,7 @@
       <c r="E91" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F91" s="19">
+      <c r="F91" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B91,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6799,10 +6905,10 @@
       <c r="O91" s="4"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A92" s="3">
+      <c r="A92" s="19">
         <v>89</v>
       </c>
-      <c r="B92" s="5">
+      <c r="B92" s="19">
         <v>221</v>
       </c>
       <c r="C92" s="5" t="s">
@@ -6829,10 +6935,10 @@
       <c r="O92" s="6"/>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A93" s="3">
+      <c r="A93" s="17">
         <v>90</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="17">
         <v>333</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -6844,7 +6950,7 @@
       <c r="E93" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F93" s="19">
+      <c r="F93" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B93,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6859,10 +6965,10 @@
       <c r="O93" s="4"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A94" s="3">
+      <c r="A94" s="19">
         <v>91</v>
       </c>
-      <c r="B94" s="5">
+      <c r="B94" s="19">
         <v>79</v>
       </c>
       <c r="C94" s="5" t="s">
@@ -6889,10 +6995,10 @@
       <c r="O94" s="6"/>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A95" s="3">
+      <c r="A95" s="17">
         <v>92</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="17">
         <v>96</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -6904,7 +7010,7 @@
       <c r="E95" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F95" s="19">
+      <c r="F95" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B95,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6919,10 +7025,10 @@
       <c r="O95" s="4"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A96" s="3">
+      <c r="A96" s="19">
         <v>93</v>
       </c>
-      <c r="B96" s="5">
+      <c r="B96" s="19">
         <v>98</v>
       </c>
       <c r="C96" s="5" t="s">
@@ -6949,10 +7055,10 @@
       <c r="O96" s="6"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A97" s="3">
+      <c r="A97" s="17">
         <v>94</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="17">
         <v>88</v>
       </c>
       <c r="C97" s="3" t="s">
@@ -6964,7 +7070,7 @@
       <c r="E97" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F97" s="19">
+      <c r="F97" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B97,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -6979,10 +7085,10 @@
       <c r="O97" s="4"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A98" s="3">
+      <c r="A98" s="19">
         <v>95</v>
       </c>
-      <c r="B98" s="5">
+      <c r="B98" s="19">
         <v>237</v>
       </c>
       <c r="C98" s="5" t="s">
@@ -7009,10 +7115,10 @@
       <c r="O98" s="6"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A99" s="3">
+      <c r="A99" s="17">
         <v>96</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="17">
         <v>203</v>
       </c>
       <c r="C99" s="20" t="s">
@@ -7024,7 +7130,7 @@
       <c r="E99" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F99" s="19" t="str">
+      <c r="F99" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B99,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7039,10 +7145,10 @@
       <c r="O99" s="4"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A100" s="3">
+      <c r="A100" s="19">
         <v>97</v>
       </c>
-      <c r="B100" s="5">
+      <c r="B100" s="19">
         <v>105</v>
       </c>
       <c r="C100" s="5" t="s">
@@ -7069,10 +7175,10 @@
       <c r="O100" s="6"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A101" s="3">
+      <c r="A101" s="17">
         <v>98</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="17">
         <v>206</v>
       </c>
       <c r="C101" s="3" t="s">
@@ -7084,7 +7190,7 @@
       <c r="E101" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F101" s="19">
+      <c r="F101" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B101,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -7099,10 +7205,10 @@
       <c r="O101" s="4"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A102" s="3">
+      <c r="A102" s="19">
         <v>99</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B102" s="19">
         <v>167</v>
       </c>
       <c r="C102" s="5" t="s">
@@ -7129,10 +7235,10 @@
       <c r="O102" s="6"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A103" s="3">
+      <c r="A103" s="17">
         <v>100</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="17">
         <v>290</v>
       </c>
       <c r="C103" s="3" t="s">
@@ -7144,7 +7250,7 @@
       <c r="E103" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F103" s="19">
+      <c r="F103" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B103,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -7159,10 +7265,10 @@
       <c r="O103" s="4"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A104" s="3">
+      <c r="A104" s="19">
         <v>101</v>
       </c>
-      <c r="B104" s="5">
+      <c r="B104" s="19">
         <v>228</v>
       </c>
       <c r="C104" s="5" t="s">
@@ -7189,10 +7295,10 @@
       <c r="O104" s="6"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A105" s="3">
+      <c r="A105" s="17">
         <v>102</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105" s="17">
         <v>248</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -7204,7 +7310,7 @@
       <c r="E105" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F105" s="19">
+      <c r="F105" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B105,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -7219,10 +7325,10 @@
       <c r="O105" s="4"/>
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A106" s="3">
+      <c r="A106" s="19">
         <v>103</v>
       </c>
-      <c r="B106" s="5">
+      <c r="B106" s="19">
         <v>142</v>
       </c>
       <c r="C106" s="5" t="s">
@@ -7249,10 +7355,10 @@
       <c r="O106" s="6"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A107" s="3">
+      <c r="A107" s="17">
         <v>104</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107" s="17">
         <v>95</v>
       </c>
       <c r="C107" s="20" t="s">
@@ -7264,7 +7370,7 @@
       <c r="E107" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F107" s="19" t="str">
+      <c r="F107" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B107,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7279,10 +7385,10 @@
       <c r="O107" s="4"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="3">
+      <c r="A108" s="19">
         <v>105</v>
       </c>
-      <c r="B108" s="5">
+      <c r="B108" s="19">
         <v>126</v>
       </c>
       <c r="C108" s="5" t="s">
@@ -7309,10 +7415,10 @@
       <c r="O108" s="6"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="3">
+      <c r="A109" s="17">
         <v>106</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="17">
         <v>309</v>
       </c>
       <c r="C109" s="20" t="s">
@@ -7324,7 +7430,7 @@
       <c r="E109" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F109" s="19" t="str">
+      <c r="F109" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B109,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7339,10 +7445,10 @@
       <c r="O109" s="4"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A110" s="3">
+      <c r="A110" s="19">
         <v>107</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B110" s="19">
         <v>179</v>
       </c>
       <c r="C110" s="5" t="s">
@@ -7369,10 +7475,10 @@
       <c r="O110" s="6"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A111" s="3">
+      <c r="A111" s="17">
         <v>108</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="17">
         <v>66</v>
       </c>
       <c r="C111" s="20" t="s">
@@ -7384,7 +7490,7 @@
       <c r="E111" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F111" s="19" t="str">
+      <c r="F111" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B111,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7399,10 +7505,10 @@
       <c r="O111" s="4"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A112" s="3">
+      <c r="A112" s="19">
         <v>109</v>
       </c>
-      <c r="B112" s="5">
+      <c r="B112" s="19">
         <v>50</v>
       </c>
       <c r="C112" s="5" t="s">
@@ -7429,10 +7535,10 @@
       <c r="O112" s="6"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A113" s="3">
+      <c r="A113" s="17">
         <v>110</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B113" s="17">
         <v>169</v>
       </c>
       <c r="C113" s="3" t="s">
@@ -7444,7 +7550,7 @@
       <c r="E113" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F113" s="19">
+      <c r="F113" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B113,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -7459,10 +7565,10 @@
       <c r="O113" s="4"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A114" s="3">
+      <c r="A114" s="19">
         <v>111</v>
       </c>
-      <c r="B114" s="5">
+      <c r="B114" s="19">
         <v>65</v>
       </c>
       <c r="C114" s="23" t="s">
@@ -7489,10 +7595,10 @@
       <c r="O114" s="6"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A115" s="3">
+      <c r="A115" s="17">
         <v>112</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B115" s="17">
         <v>133</v>
       </c>
       <c r="C115" s="20" t="s">
@@ -7504,7 +7610,7 @@
       <c r="E115" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F115" s="19" t="str">
+      <c r="F115" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B115,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7519,10 +7625,10 @@
       <c r="O115" s="4"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A116" s="3">
+      <c r="A116" s="19">
         <v>113</v>
       </c>
-      <c r="B116" s="5">
+      <c r="B116" s="19">
         <v>171</v>
       </c>
       <c r="C116" s="5" t="s">
@@ -7549,10 +7655,10 @@
       <c r="O116" s="6"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A117" s="3">
+      <c r="A117" s="17">
         <v>114</v>
       </c>
-      <c r="B117" s="3">
+      <c r="B117" s="17">
         <v>90</v>
       </c>
       <c r="C117" s="20" t="s">
@@ -7564,7 +7670,7 @@
       <c r="E117" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F117" s="19" t="str">
+      <c r="F117" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B117,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7579,10 +7685,10 @@
       <c r="O117" s="4"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A118" s="3">
+      <c r="A118" s="19">
         <v>115</v>
       </c>
-      <c r="B118" s="5">
+      <c r="B118" s="19">
         <v>147</v>
       </c>
       <c r="C118" s="23" t="s">
@@ -7609,10 +7715,10 @@
       <c r="O118" s="6"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A119" s="3">
+      <c r="A119" s="17">
         <v>116</v>
       </c>
-      <c r="B119" s="3">
+      <c r="B119" s="17">
         <v>103</v>
       </c>
       <c r="C119" s="20" t="s">
@@ -7624,7 +7730,7 @@
       <c r="E119" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F119" s="19" t="str">
+      <c r="F119" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B119,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7639,10 +7745,10 @@
       <c r="O119" s="4"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A120" s="3">
+      <c r="A120" s="19">
         <v>117</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B120" s="19">
         <v>172</v>
       </c>
       <c r="C120" s="23" t="s">
@@ -7669,10 +7775,10 @@
       <c r="O120" s="6"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A121" s="3">
+      <c r="A121" s="17">
         <v>118</v>
       </c>
-      <c r="B121" s="3">
+      <c r="B121" s="17">
         <v>121</v>
       </c>
       <c r="C121" s="20" t="s">
@@ -7684,7 +7790,7 @@
       <c r="E121" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F121" s="19" t="str">
+      <c r="F121" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B121,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -7699,10 +7805,10 @@
       <c r="O121" s="4"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A122" s="3">
+      <c r="A122" s="19">
         <v>119</v>
       </c>
-      <c r="B122" s="5">
+      <c r="B122" s="19">
         <v>97</v>
       </c>
       <c r="C122" s="23" t="s">
@@ -7729,10 +7835,10 @@
       <c r="O122" s="6"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A123" s="3">
+      <c r="A123" s="17">
         <v>120</v>
       </c>
-      <c r="B123" s="3">
+      <c r="B123" s="17">
         <v>47</v>
       </c>
       <c r="C123" s="3" t="s">
@@ -7744,7 +7850,7 @@
       <c r="E123" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F123" s="19">
+      <c r="F123" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B123,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -7759,10 +7865,10 @@
       <c r="O123" s="4"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A124" s="3">
+      <c r="A124" s="19">
         <v>121</v>
       </c>
-      <c r="B124" s="5">
+      <c r="B124" s="19">
         <v>72</v>
       </c>
       <c r="C124" s="5" t="s">
@@ -7789,42 +7895,42 @@
       <c r="O124" s="6"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A125" s="3">
+      <c r="A125" s="54">
         <v>122</v>
       </c>
-      <c r="B125" s="3">
+      <c r="B125" s="54">
         <v>213</v>
       </c>
       <c r="C125" s="20" t="s">
         <v>266</v>
       </c>
-      <c r="D125" s="3" t="s">
+      <c r="D125" s="20" t="s">
         <v>267</v>
       </c>
-      <c r="E125" s="3" t="s">
+      <c r="E125" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="F125" s="19">
+      <c r="F125" s="54">
         <f>_xlfn.IFNA(VLOOKUP(B125,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>2</v>
       </c>
-      <c r="G125" s="24"/>
-      <c r="H125" s="7"/>
-      <c r="I125" s="7"/>
-      <c r="J125" s="7"/>
-      <c r="K125" s="7"/>
-      <c r="L125" s="4"/>
-      <c r="M125" s="4"/>
-      <c r="N125" s="3" t="s">
+      <c r="G125" s="51"/>
+      <c r="H125" s="52"/>
+      <c r="I125" s="52"/>
+      <c r="J125" s="52"/>
+      <c r="K125" s="52"/>
+      <c r="L125" s="53"/>
+      <c r="M125" s="53"/>
+      <c r="N125" s="20" t="s">
         <v>970</v>
       </c>
-      <c r="O125" s="4"/>
+      <c r="O125" s="53"/>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A126" s="3">
+      <c r="A126" s="19">
         <v>123</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B126" s="19">
         <v>157</v>
       </c>
       <c r="C126" s="5" t="s">
@@ -7851,10 +7957,10 @@
       <c r="O126" s="6"/>
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A127" s="3">
+      <c r="A127" s="17">
         <v>124</v>
       </c>
-      <c r="B127" s="3">
+      <c r="B127" s="17">
         <v>222</v>
       </c>
       <c r="C127" s="3" t="s">
@@ -7866,7 +7972,7 @@
       <c r="E127" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F127" s="19">
+      <c r="F127" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B127,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -7881,10 +7987,10 @@
       <c r="O127" s="4"/>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A128" s="3">
+      <c r="A128" s="19">
         <v>125</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B128" s="19">
         <v>158</v>
       </c>
       <c r="C128" s="5" t="s">
@@ -7911,10 +8017,10 @@
       <c r="O128" s="6"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A129" s="3">
+      <c r="A129" s="17">
         <v>126</v>
       </c>
-      <c r="B129" s="3">
+      <c r="B129" s="17">
         <v>170</v>
       </c>
       <c r="C129" s="3" t="s">
@@ -7926,7 +8032,7 @@
       <c r="E129" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F129" s="19">
+      <c r="F129" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B129,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -7941,10 +8047,10 @@
       <c r="O129" s="4"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A130" s="3">
+      <c r="A130" s="19">
         <v>127</v>
       </c>
-      <c r="B130" s="5">
+      <c r="B130" s="19">
         <v>266</v>
       </c>
       <c r="C130" s="5" t="s">
@@ -7971,10 +8077,10 @@
       <c r="O130" s="6"/>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A131" s="3">
+      <c r="A131" s="17">
         <v>128</v>
       </c>
-      <c r="B131" s="3">
+      <c r="B131" s="17">
         <v>76</v>
       </c>
       <c r="C131" s="3" t="s">
@@ -7986,7 +8092,7 @@
       <c r="E131" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F131" s="19">
+      <c r="F131" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B131,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8001,10 +8107,10 @@
       <c r="O131" s="4"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A132" s="3">
+      <c r="A132" s="19">
         <v>129</v>
       </c>
-      <c r="B132" s="5">
+      <c r="B132" s="19">
         <v>114</v>
       </c>
       <c r="C132" s="23" t="s">
@@ -8031,10 +8137,10 @@
       <c r="O132" s="6"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A133" s="3">
+      <c r="A133" s="17">
         <v>130</v>
       </c>
-      <c r="B133" s="3">
+      <c r="B133" s="17">
         <v>295</v>
       </c>
       <c r="C133" s="20" t="s">
@@ -8046,7 +8152,7 @@
       <c r="E133" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F133" s="19" t="str">
+      <c r="F133" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B133,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -8061,10 +8167,10 @@
       <c r="O133" s="4"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A134" s="3">
+      <c r="A134" s="19">
         <v>131</v>
       </c>
-      <c r="B134" s="5">
+      <c r="B134" s="19">
         <v>218</v>
       </c>
       <c r="C134" s="5" t="s">
@@ -8091,10 +8197,10 @@
       <c r="O134" s="6"/>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A135" s="3">
+      <c r="A135" s="17">
         <v>132</v>
       </c>
-      <c r="B135" s="3">
+      <c r="B135" s="17">
         <v>195</v>
       </c>
       <c r="C135" s="3" t="s">
@@ -8106,7 +8212,7 @@
       <c r="E135" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F135" s="19">
+      <c r="F135" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B135,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8121,10 +8227,10 @@
       <c r="O135" s="4"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A136" s="3">
+      <c r="A136" s="19">
         <v>133</v>
       </c>
-      <c r="B136" s="5">
+      <c r="B136" s="19">
         <v>287</v>
       </c>
       <c r="C136" s="5" t="s">
@@ -8151,10 +8257,10 @@
       <c r="O136" s="6"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A137" s="3">
+      <c r="A137" s="17">
         <v>134</v>
       </c>
-      <c r="B137" s="3">
+      <c r="B137" s="17">
         <v>242</v>
       </c>
       <c r="C137" s="3" t="s">
@@ -8166,7 +8272,7 @@
       <c r="E137" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F137" s="19">
+      <c r="F137" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B137,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>4</v>
       </c>
@@ -8181,10 +8287,10 @@
       <c r="O137" s="4"/>
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A138" s="3">
+      <c r="A138" s="19">
         <v>135</v>
       </c>
-      <c r="B138" s="5">
+      <c r="B138" s="19">
         <v>99</v>
       </c>
       <c r="C138" s="5" t="s">
@@ -8211,10 +8317,10 @@
       <c r="O138" s="6"/>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A139" s="3">
+      <c r="A139" s="17">
         <v>136</v>
       </c>
-      <c r="B139" s="3">
+      <c r="B139" s="17">
         <v>137</v>
       </c>
       <c r="C139" s="3" t="s">
@@ -8226,7 +8332,7 @@
       <c r="E139" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F139" s="19">
+      <c r="F139" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B139,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8241,10 +8347,10 @@
       <c r="O139" s="4"/>
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A140" s="3">
+      <c r="A140" s="19">
         <v>137</v>
       </c>
-      <c r="B140" s="5">
+      <c r="B140" s="19">
         <v>191</v>
       </c>
       <c r="C140" s="23" t="s">
@@ -8271,10 +8377,10 @@
       <c r="O140" s="6"/>
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A141" s="3">
+      <c r="A141" s="17">
         <v>138</v>
       </c>
-      <c r="B141" s="3">
+      <c r="B141" s="17">
         <v>201</v>
       </c>
       <c r="C141" s="3" t="s">
@@ -8286,7 +8392,7 @@
       <c r="E141" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F141" s="19">
+      <c r="F141" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B141,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8301,10 +8407,10 @@
       <c r="O141" s="4"/>
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A142" s="3">
+      <c r="A142" s="19">
         <v>139</v>
       </c>
-      <c r="B142" s="5">
+      <c r="B142" s="19">
         <v>260</v>
       </c>
       <c r="C142" s="5" t="s">
@@ -8331,10 +8437,10 @@
       <c r="O142" s="6"/>
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A143" s="3">
+      <c r="A143" s="17">
         <v>140</v>
       </c>
-      <c r="B143" s="3">
+      <c r="B143" s="17">
         <v>71</v>
       </c>
       <c r="C143" s="3" t="s">
@@ -8346,7 +8452,7 @@
       <c r="E143" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F143" s="19">
+      <c r="F143" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B143,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8361,10 +8467,10 @@
       <c r="O143" s="4"/>
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A144" s="3">
+      <c r="A144" s="19">
         <v>141</v>
       </c>
-      <c r="B144" s="5">
+      <c r="B144" s="19">
         <v>68</v>
       </c>
       <c r="C144" s="23" t="s">
@@ -8391,10 +8497,10 @@
       <c r="O144" s="6"/>
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A145" s="3">
+      <c r="A145" s="17">
         <v>142</v>
       </c>
-      <c r="B145" s="3">
+      <c r="B145" s="17">
         <v>259</v>
       </c>
       <c r="C145" s="3" t="s">
@@ -8406,7 +8512,7 @@
       <c r="E145" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F145" s="19">
+      <c r="F145" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B145,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8421,10 +8527,10 @@
       <c r="O145" s="4"/>
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A146" s="3">
+      <c r="A146" s="19">
         <v>143</v>
       </c>
-      <c r="B146" s="5">
+      <c r="B146" s="19">
         <v>130</v>
       </c>
       <c r="C146" s="5" t="s">
@@ -8451,10 +8557,10 @@
       <c r="O146" s="6"/>
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A147" s="3">
+      <c r="A147" s="17">
         <v>144</v>
       </c>
-      <c r="B147" s="3">
+      <c r="B147" s="17">
         <v>46</v>
       </c>
       <c r="C147" s="3" t="s">
@@ -8466,7 +8572,7 @@
       <c r="E147" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F147" s="19">
+      <c r="F147" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B147,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8481,10 +8587,10 @@
       <c r="O147" s="4"/>
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A148" s="3">
+      <c r="A148" s="19">
         <v>145</v>
       </c>
-      <c r="B148" s="5">
+      <c r="B148" s="19">
         <v>312</v>
       </c>
       <c r="C148" s="5" t="s">
@@ -8511,10 +8617,10 @@
       <c r="O148" s="6"/>
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A149" s="3">
+      <c r="A149" s="17">
         <v>146</v>
       </c>
-      <c r="B149" s="3">
+      <c r="B149" s="17">
         <v>70</v>
       </c>
       <c r="C149" s="20" t="s">
@@ -8526,7 +8632,7 @@
       <c r="E149" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F149" s="19" t="str">
+      <c r="F149" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B149,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -8541,10 +8647,10 @@
       <c r="O149" s="4"/>
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A150" s="3">
+      <c r="A150" s="19">
         <v>147</v>
       </c>
-      <c r="B150" s="5">
+      <c r="B150" s="19">
         <v>129</v>
       </c>
       <c r="C150" s="23" t="s">
@@ -8571,10 +8677,10 @@
       <c r="O150" s="6"/>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A151" s="3">
+      <c r="A151" s="17">
         <v>148</v>
       </c>
-      <c r="B151" s="3">
+      <c r="B151" s="17">
         <v>67</v>
       </c>
       <c r="C151" s="20" t="s">
@@ -8586,7 +8692,7 @@
       <c r="E151" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F151" s="19" t="str">
+      <c r="F151" s="17" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B151,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -8601,10 +8707,10 @@
       <c r="O151" s="4"/>
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A152" s="3">
+      <c r="A152" s="19">
         <v>149</v>
       </c>
-      <c r="B152" s="5">
+      <c r="B152" s="19">
         <v>155</v>
       </c>
       <c r="C152" s="5" t="s">
@@ -8631,10 +8737,10 @@
       <c r="O152" s="6"/>
     </row>
     <row r="153" spans="1:15" ht="24" x14ac:dyDescent="0.25">
-      <c r="A153" s="3">
+      <c r="A153" s="17">
         <v>150</v>
       </c>
-      <c r="B153" s="3">
+      <c r="B153" s="17">
         <v>110</v>
       </c>
       <c r="C153" s="3" t="s">
@@ -8646,7 +8752,7 @@
       <c r="E153" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F153" s="19">
+      <c r="F153" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B153,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8663,10 +8769,10 @@
       <c r="O153" s="4"/>
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A154" s="3">
+      <c r="A154" s="19">
         <v>151</v>
       </c>
-      <c r="B154" s="5">
+      <c r="B154" s="19">
         <v>338</v>
       </c>
       <c r="C154" s="5" t="s">
@@ -8693,10 +8799,10 @@
       <c r="O154" s="6"/>
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A155" s="3">
+      <c r="A155" s="17">
         <v>152</v>
       </c>
-      <c r="B155" s="3">
+      <c r="B155" s="17">
         <v>118</v>
       </c>
       <c r="C155" s="3" t="s">
@@ -8708,7 +8814,7 @@
       <c r="E155" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F155" s="19">
+      <c r="F155" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B155,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8723,10 +8829,10 @@
       <c r="O155" s="4"/>
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A156" s="3">
+      <c r="A156" s="19">
         <v>153</v>
       </c>
-      <c r="B156" s="5">
+      <c r="B156" s="19">
         <v>294</v>
       </c>
       <c r="C156" s="23" t="s">
@@ -8753,10 +8859,10 @@
       <c r="O156" s="6"/>
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A157" s="3">
+      <c r="A157" s="17">
         <v>154</v>
       </c>
-      <c r="B157" s="3">
+      <c r="B157" s="17">
         <v>240</v>
       </c>
       <c r="C157" s="3" t="s">
@@ -8768,7 +8874,7 @@
       <c r="E157" s="3" t="s">
         <v>510</v>
       </c>
-      <c r="F157" s="19">
+      <c r="F157" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B157,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8783,10 +8889,10 @@
       <c r="O157" s="4"/>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A158" s="3">
+      <c r="A158" s="19">
         <v>155</v>
       </c>
-      <c r="B158" s="5">
+      <c r="B158" s="19">
         <v>84</v>
       </c>
       <c r="C158" s="23" t="s">
@@ -8813,10 +8919,10 @@
       <c r="O158" s="6"/>
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A159" s="3">
+      <c r="A159" s="17">
         <v>156</v>
       </c>
-      <c r="B159" s="3">
+      <c r="B159" s="17">
         <v>303</v>
       </c>
       <c r="C159" s="3" t="s">
@@ -8828,7 +8934,7 @@
       <c r="E159" s="3" t="s">
         <v>509</v>
       </c>
-      <c r="F159" s="19">
+      <c r="F159" s="17">
         <f>_xlfn.IFNA(VLOOKUP(B159,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
@@ -8842,11 +8948,11 @@
       <c r="N159" s="3"/>
       <c r="O159" s="4"/>
     </row>
-    <row r="160" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="3">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A160" s="31">
         <v>157</v>
       </c>
-      <c r="B160" s="30">
+      <c r="B160" s="31">
         <v>304</v>
       </c>
       <c r="C160" s="30" t="s">
@@ -8872,27 +8978,8 @@
       <c r="N160" s="30"/>
       <c r="O160" s="34"/>
     </row>
-    <row r="161" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="3">
-        <v>158</v>
-      </c>
-      <c r="B161" s="35"/>
-      <c r="C161" s="35"/>
-      <c r="D161" s="35"/>
-      <c r="E161" s="35"/>
-      <c r="F161" s="36"/>
-      <c r="G161" s="37"/>
-      <c r="H161" s="38"/>
-      <c r="I161" s="38"/>
-      <c r="J161" s="38"/>
-      <c r="K161" s="38"/>
-      <c r="L161" s="39"/>
-      <c r="M161" s="39"/>
-      <c r="N161" s="35"/>
-      <c r="O161" s="39"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:N161" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
+  <autoFilter ref="A2:N160" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:N160">
     <sortCondition ref="I4:I160"/>
     <sortCondition ref="H4:H160"/>
@@ -8949,42 +9036,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="42" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="47" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="42" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -9012,7 +9099,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="48"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7">

</xml_diff>

<commit_message>
Se empieza a trabajar en el módulo: Estadisticas Entregas CEDIS Resumen
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\Migracion Spooler\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4454EE7-FE51-4F33-85DD-3CB818C1E333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E924D-9C86-4B7B-BD2A-CD6EAEBF5068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6103" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6113" uniqueCount="1001">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3184,6 +3184,12 @@
   <si>
     <t>Pendiente de confirmacion por el usuario …
 06/06/2025: Como se comentó, se van a migrar los tres procesos que están incluidos en éste, toda vez que el área de negocio no ha confirmado cuál de ellos utiliza y cuál de ellos ya no les es funcional.</t>
+  </si>
+  <si>
+    <t>Este proceso ya no se hace desde el Spooler, según los comentarios que estan en el main, se comento la logica ya que el proceso se paso aun JOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/06/2025: Se empieza analizando el módulo </t>
   </si>
 </sst>
 </file>
@@ -3370,7 +3376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3472,6 +3478,30 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3514,29 +3544,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3872,9 +3881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:O160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,54 +3905,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="46" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="50" t="s">
         <v>505</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="G1" s="52" t="s">
         <v>964</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="48" t="s">
         <v>369</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="38" t="s">
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="43" t="s">
         <v>502</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="45" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="43" t="s">
         <v>982</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="45"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="9" t="s">
         <v>370</v>
       </c>
@@ -3956,10 +3965,10 @@
       <c r="K2" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="39"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="36"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
@@ -4440,39 +4449,39 @@
         <f>_xlfn.IFNA(VLOOKUP(B15,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="H15" s="52" t="s">
+      <c r="H15" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="I15" s="52" t="s">
+      <c r="I15" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="J15" s="52" t="s">
+      <c r="J15" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="K15" s="52" t="s">
+      <c r="K15" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="L15" s="52" t="s">
+      <c r="L15" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="M15" s="52" t="s">
+      <c r="M15" s="38" t="s">
         <v>507</v>
       </c>
       <c r="N15" s="20" t="s">
         <v>997</v>
       </c>
-      <c r="O15" s="52" t="s">
+      <c r="O15" s="38" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="49">
+      <c r="A16" s="35">
         <v>13</v>
       </c>
-      <c r="B16" s="49">
+      <c r="B16" s="35">
         <v>102</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -4484,43 +4493,43 @@
       <c r="E16" s="23" t="s">
         <v>509</v>
       </c>
-      <c r="F16" s="49">
+      <c r="F16" s="35">
         <f>_xlfn.IFNA(VLOOKUP(B16,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G16" s="50" t="s">
+      <c r="G16" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="J16" s="50" t="s">
+      <c r="J16" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="K16" s="50" t="s">
+      <c r="K16" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="L16" s="50" t="s">
+      <c r="L16" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="M16" s="50" t="s">
+      <c r="M16" s="36" t="s">
         <v>507</v>
       </c>
       <c r="N16" s="23" t="s">
         <v>997</v>
       </c>
-      <c r="O16" s="50" t="s">
+      <c r="O16" s="36" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="54">
+      <c r="A17" s="40">
         <v>14</v>
       </c>
-      <c r="B17" s="54">
+      <c r="B17" s="40">
         <v>102</v>
       </c>
       <c r="C17" s="20" t="s">
@@ -4532,43 +4541,43 @@
       <c r="E17" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="40">
         <f>_xlfn.IFNA(VLOOKUP(B17,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G17" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="H17" s="52" t="s">
+      <c r="H17" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="I17" s="52" t="s">
+      <c r="I17" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="J17" s="52" t="s">
+      <c r="J17" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="K17" s="52" t="s">
+      <c r="K17" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="L17" s="52" t="s">
+      <c r="L17" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="M17" s="52" t="s">
+      <c r="M17" s="38" t="s">
         <v>507</v>
       </c>
       <c r="N17" s="20" t="s">
         <v>997</v>
       </c>
-      <c r="O17" s="52" t="s">
+      <c r="O17" s="38" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="49">
+      <c r="A18" s="35">
         <v>15</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="35">
         <v>102</v>
       </c>
       <c r="C18" s="23" t="s">
@@ -4580,43 +4589,43 @@
       <c r="E18" s="23" t="s">
         <v>509</v>
       </c>
-      <c r="F18" s="49">
+      <c r="F18" s="35">
         <f>_xlfn.IFNA(VLOOKUP(B18,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G18" s="50" t="s">
+      <c r="G18" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="H18" s="50" t="s">
+      <c r="H18" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="I18" s="50" t="s">
+      <c r="I18" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="K18" s="50" t="s">
+      <c r="K18" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="L18" s="50" t="s">
+      <c r="L18" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="M18" s="50" t="s">
+      <c r="M18" s="36" t="s">
         <v>507</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>997</v>
       </c>
-      <c r="O18" s="50" t="s">
+      <c r="O18" s="36" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="54">
+      <c r="A19" s="40">
         <v>16</v>
       </c>
-      <c r="B19" s="54">
+      <c r="B19" s="40">
         <v>102</v>
       </c>
       <c r="C19" s="20" t="s">
@@ -4628,43 +4637,43 @@
       <c r="E19" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="40">
         <f>_xlfn.IFNA(VLOOKUP(B19,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G19" s="51" t="s">
+      <c r="G19" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="H19" s="52" t="s">
+      <c r="H19" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="I19" s="52" t="s">
+      <c r="I19" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="J19" s="52" t="s">
+      <c r="J19" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="K19" s="52" t="s">
+      <c r="K19" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="L19" s="52" t="s">
+      <c r="L19" s="38" t="s">
         <v>507</v>
       </c>
-      <c r="M19" s="52" t="s">
+      <c r="M19" s="38" t="s">
         <v>507</v>
       </c>
       <c r="N19" s="20" t="s">
         <v>997</v>
       </c>
-      <c r="O19" s="52" t="s">
+      <c r="O19" s="38" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="49">
+      <c r="A20" s="35">
         <v>17</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="35">
         <v>341</v>
       </c>
       <c r="C20" s="23" t="s">
@@ -4676,35 +4685,35 @@
       <c r="E20" s="23" t="s">
         <v>509</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="35">
         <f>_xlfn.IFNA(VLOOKUP(B20,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G20" s="50" t="s">
+      <c r="G20" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="H20" s="50" t="s">
+      <c r="H20" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="I20" s="50" t="s">
+      <c r="I20" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="J20" s="50" t="s">
+      <c r="J20" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="K20" s="50" t="s">
+      <c r="K20" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="L20" s="50" t="s">
+      <c r="L20" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="M20" s="50" t="s">
+      <c r="M20" s="36" t="s">
         <v>507</v>
       </c>
       <c r="N20" s="23" t="s">
         <v>997</v>
       </c>
-      <c r="O20" s="50" t="s">
+      <c r="O20" s="36" t="s">
         <v>507</v>
       </c>
     </row>
@@ -5028,14 +5037,20 @@
         <f>_xlfn.IFNA(VLOOKUP(B30,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>1</v>
       </c>
-      <c r="G30" s="25"/>
+      <c r="G30" s="25">
+        <v>45818</v>
+      </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
-      <c r="L30" s="6"/>
+      <c r="L30" s="6" t="s">
+        <v>965</v>
+      </c>
       <c r="M30" s="6"/>
-      <c r="N30" s="5"/>
+      <c r="N30" s="57" t="s">
+        <v>1000</v>
+      </c>
       <c r="O30" s="6"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -5255,10 +5270,10 @@
       <c r="O36" s="6"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="55">
+      <c r="A37" s="41">
         <v>34</v>
       </c>
-      <c r="B37" s="55">
+      <c r="B37" s="41">
         <v>36</v>
       </c>
       <c r="C37" s="21" t="s">
@@ -5270,7 +5285,7 @@
       <c r="E37" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="F37" s="55" t="str">
+      <c r="F37" s="41" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B37,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -5285,10 +5300,10 @@
       <c r="O37" s="16"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="56">
+      <c r="A38" s="42">
         <v>35</v>
       </c>
-      <c r="B38" s="56">
+      <c r="B38" s="42">
         <v>37</v>
       </c>
       <c r="C38" s="22" t="s">
@@ -5300,7 +5315,7 @@
       <c r="E38" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="F38" s="56" t="str">
+      <c r="F38" s="42" t="str">
         <f>_xlfn.IFNA(VLOOKUP(B38,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>No Activo</v>
       </c>
@@ -5314,34 +5329,50 @@
       <c r="N38" s="11"/>
       <c r="O38" s="13"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>36</v>
       </c>
       <c r="B39" s="17">
         <v>39</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="20" t="s">
         <v>508</v>
       </c>
-      <c r="F39" s="17">
+      <c r="F39" s="40">
         <f>_xlfn.IFNA(VLOOKUP(B39,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>4</v>
       </c>
-      <c r="G39" s="24"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="3"/>
+      <c r="G39" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="H39" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="I39" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="J39" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="K39" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="L39" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="M39" s="36" t="s">
+        <v>507</v>
+      </c>
+      <c r="N39" s="20" t="s">
+        <v>999</v>
+      </c>
       <c r="O39" s="4"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
@@ -7895,10 +7926,10 @@
       <c r="O124" s="6"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A125" s="54">
+      <c r="A125" s="40">
         <v>122</v>
       </c>
-      <c r="B125" s="54">
+      <c r="B125" s="40">
         <v>213</v>
       </c>
       <c r="C125" s="20" t="s">
@@ -7910,21 +7941,21 @@
       <c r="E125" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="F125" s="54">
+      <c r="F125" s="40">
         <f>_xlfn.IFNA(VLOOKUP(B125,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>2</v>
       </c>
-      <c r="G125" s="51"/>
-      <c r="H125" s="52"/>
-      <c r="I125" s="52"/>
-      <c r="J125" s="52"/>
-      <c r="K125" s="52"/>
-      <c r="L125" s="53"/>
-      <c r="M125" s="53"/>
+      <c r="G125" s="37"/>
+      <c r="H125" s="38"/>
+      <c r="I125" s="38"/>
+      <c r="J125" s="38"/>
+      <c r="K125" s="38"/>
+      <c r="L125" s="39"/>
+      <c r="M125" s="39"/>
       <c r="N125" s="20" t="s">
         <v>970</v>
       </c>
-      <c r="O125" s="53"/>
+      <c r="O125" s="39"/>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" s="19">
@@ -9036,42 +9067,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="50" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="42" t="s">
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="50" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -9099,7 +9130,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="43"/>
+      <c r="O2" s="51"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7">

</xml_diff>

<commit_message>
Se agrega nuevo módulo, para el reporte de "Talones con Seguro", adicional se actualiza plan de trabajo.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\Migracion Spooler\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E924D-9C86-4B7B-BD2A-CD6EAEBF5068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E1CD1E-6A01-4B2F-AD64-8F11F57C38AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6113" uniqueCount="1001">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6114" uniqueCount="1002">
   <si>
     <t>ID_REP</t>
   </si>
@@ -3145,9 +3145,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>04/06/2025: Se inicia con el analisis</t>
-  </si>
-  <si>
     <t>SC_RS.SPG_RS_DIST.P_RS_GSK_PEDIMENTOS</t>
   </si>
   <si>
@@ -3190,6 +3187,14 @@
   </si>
   <si>
     <t xml:space="preserve">10/06/2025: Se empieza analizando el módulo </t>
+  </si>
+  <si>
+    <t>04/06/2025: Se inicia con el analisis
+10/06/2025: Se termina desarrollo y se sube al repositorio</t>
+  </si>
+  <si>
+    <t>SC_RS_DIST.SPG_RS_DIST_TALONES_CON_SEGURO.P_DAT_FTL_CON_IMPORTE
+SC_RS_DIST.SPG_RS_DIST_TALONES_CON_SEGURO.P_DAT_TALON_CON_SEGURO</t>
   </si>
 </sst>
 </file>
@@ -3502,6 +3507,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3543,9 +3551,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3881,9 +3886,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:O160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3905,54 +3910,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>479</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="51" t="s">
         <v>505</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="51" t="s">
         <v>506</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="53" t="s">
         <v>964</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="49" t="s">
         <v>369</v>
       </c>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="46" t="s">
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="47" t="s">
         <v>381</v>
       </c>
-      <c r="M1" s="43" t="s">
+      <c r="M1" s="44" t="s">
         <v>502</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="N1" s="46" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="43" t="s">
+      <c r="O1" s="44" t="s">
         <v>982</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="53"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="9" t="s">
         <v>370</v>
       </c>
@@ -3965,10 +3970,10 @@
       <c r="K2" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="L2" s="47"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="44"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="45"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
@@ -4044,7 +4049,7 @@
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -4084,7 +4089,7 @@
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="72" x14ac:dyDescent="0.25">
@@ -4124,7 +4129,7 @@
       </c>
       <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.25">
@@ -4164,7 +4169,7 @@
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -4204,7 +4209,7 @@
       </c>
       <c r="N8" s="5"/>
       <c r="O8" s="5" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -4244,7 +4249,7 @@
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4284,7 +4289,7 @@
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="5" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -4471,7 +4476,7 @@
         <v>507</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O15" s="38" t="s">
         <v>507</v>
@@ -4519,7 +4524,7 @@
         <v>507</v>
       </c>
       <c r="N16" s="23" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O16" s="36" t="s">
         <v>507</v>
@@ -4567,7 +4572,7 @@
         <v>507</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O17" s="38" t="s">
         <v>507</v>
@@ -4615,7 +4620,7 @@
         <v>507</v>
       </c>
       <c r="N18" s="23" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O18" s="36" t="s">
         <v>507</v>
@@ -4663,7 +4668,7 @@
         <v>507</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O19" s="38" t="s">
         <v>507</v>
@@ -4711,7 +4716,7 @@
         <v>507</v>
       </c>
       <c r="N20" s="23" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="O20" s="36" t="s">
         <v>507</v>
@@ -5013,7 +5018,7 @@
       </c>
       <c r="M29" s="4"/>
       <c r="N29" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="O29" s="4"/>
     </row>
@@ -5048,8 +5053,8 @@
         <v>965</v>
       </c>
       <c r="M30" s="6"/>
-      <c r="N30" s="57" t="s">
-        <v>1000</v>
+      <c r="N30" s="43" t="s">
+        <v>999</v>
       </c>
       <c r="O30" s="6"/>
     </row>
@@ -5151,10 +5156,10 @@
         <v>7760421</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="O33" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -5197,7 +5202,7 @@
       </c>
       <c r="O34" s="5"/>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="24" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>32</v>
       </c>
@@ -5229,11 +5234,15 @@
       <c r="L35" s="4" t="s">
         <v>965</v>
       </c>
-      <c r="M35" s="4"/>
+      <c r="M35" s="4">
+        <v>7951071</v>
+      </c>
       <c r="N35" s="3" t="s">
-        <v>988</v>
-      </c>
-      <c r="O35" s="4"/>
+        <v>1000</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>1001</v>
+      </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="19">
@@ -5371,7 +5380,7 @@
         <v>507</v>
       </c>
       <c r="N39" s="20" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="O39" s="4"/>
     </row>
@@ -9067,42 +9076,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="F1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="56"/>
-      <c r="O1" s="50" t="s">
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="51" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
@@ -9130,7 +9139,7 @@
       <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="51"/>
+      <c r="O2" s="52"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="7">

</xml_diff>

<commit_message>
Se actualiza el plan de trabajo descativando el reporte de Talones(texto-excel).
</commit_message>
<xml_diff>
--- a/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
+++ b/00-Documentacion/Spooler-Distribucion-Plan_Trabajo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ricardo Lozada - Proyectos\Migración\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E1CD1E-6A01-4B2F-AD64-8F11F57C38AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CAE4B3-3979-46AB-82B4-B8FB7B703330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado" sheetId="5" r:id="rId1"/>
@@ -3179,10 +3179,6 @@
     <t>ÉSTE PROCESO SE MIGRÓ AL NUEVO PORTAL WEB</t>
   </si>
   <si>
-    <t>Pendiente de confirmacion por el usuario …
-06/06/2025: Como se comentó, se van a migrar los tres procesos que están incluidos en éste, toda vez que el área de negocio no ha confirmado cuál de ellos utiliza y cuál de ellos ya no les es funcional.</t>
-  </si>
-  <si>
     <t>Este proceso ya no se hace desde el Spooler, según los comentarios que estan en el main, se comento la logica ya que el proceso se paso aun JOB</t>
   </si>
   <si>
@@ -3195,6 +3191,11 @@
   <si>
     <t>SC_RS_DIST.SPG_RS_DIST_TALONES_CON_SEGURO.P_DAT_FTL_CON_IMPORTE
 SC_RS_DIST.SPG_RS_DIST_TALONES_CON_SEGURO.P_DAT_TALON_CON_SEGURO</t>
+  </si>
+  <si>
+    <t>Pendiente de confirmacion por el usuario …
+06/06/2025: Como se comentó, se van a migrar los tres procesos que están incluidos en éste, toda vez que el área de negocio no ha confirmado cuál de ellos utiliza y cuál de ellos ya no les es funcional.
+11/06/2025: Se desactivan los procesos automáticos ya que confirmó Sandy que éste reporte ya no se utiliza, por lo tanto tampoco se considerará para la migración.</t>
   </si>
 </sst>
 </file>
@@ -3886,9 +3887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318CFF63-88F3-4F4A-90F9-197F614EDEF7}">
   <dimension ref="A1:O160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
+      <selection pane="bottomLeft" activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4988,39 +4989,39 @@
       </c>
       <c r="O28" s="6"/>
     </row>
-    <row r="29" spans="1:15" ht="48" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
+    <row r="29" spans="1:15" ht="84" x14ac:dyDescent="0.25">
+      <c r="A29" s="40">
         <v>26</v>
       </c>
-      <c r="B29" s="17">
+      <c r="B29" s="40">
         <v>80</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="F29" s="17">
+      <c r="F29" s="40">
         <f>_xlfn.IFNA(VLOOKUP(B29,Activos!A$2:D$116,4,FALSE),"No Activo")</f>
         <v>16</v>
       </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="4" t="s">
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="39" t="s">
         <v>967</v>
       </c>
-      <c r="M29" s="4"/>
-      <c r="N29" s="3" t="s">
-        <v>997</v>
-      </c>
-      <c r="O29" s="4"/>
+      <c r="M29" s="39"/>
+      <c r="N29" s="20" t="s">
+        <v>1001</v>
+      </c>
+      <c r="O29" s="39"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="19">
@@ -5054,7 +5055,7 @@
       </c>
       <c r="M30" s="6"/>
       <c r="N30" s="43" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="O30" s="6"/>
     </row>
@@ -5238,10 +5239,10 @@
         <v>7951071</v>
       </c>
       <c r="N35" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="O35" s="3" t="s">
         <v>1000</v>
-      </c>
-      <c r="O35" s="3" t="s">
-        <v>1001</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -5380,7 +5381,7 @@
         <v>507</v>
       </c>
       <c r="N39" s="20" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="O39" s="4"/>
     </row>

</xml_diff>